<commit_message>
Updates in the World model, inclusion of synthetic fuels and hydrogen and calibration of the model following the NZE scenario goals of the IEA.
</commit_message>
<xml_diff>
--- a/models/14sectors_cat/energy.xlsx
+++ b/models/14sectors_cat/energy.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="13005" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="9750" windowHeight="3885" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Global" sheetId="1" r:id="rId1"/>
@@ -133,6 +133,9 @@
     <definedName name="end_hist_data" localSheetId="1">World!$C$107</definedName>
     <definedName name="eroi_initial_res_elec_dispatch" localSheetId="0">Global!$B$4:$B$11</definedName>
     <definedName name="esoi_phs_depleted_potential" localSheetId="0">Global!$G$30</definedName>
+    <definedName name="ETG" localSheetId="1">World!$B$235:$B$236</definedName>
+    <definedName name="ETL" localSheetId="1">World!$B$233:$B$234</definedName>
+    <definedName name="ETS">World!$B$233:$B$236</definedName>
     <definedName name="gas_historic_imports" localSheetId="3">Catalonia!$B$240:$Z$240</definedName>
     <definedName name="gas_historic_imports" localSheetId="2">Europe!$B$263:$Z$263</definedName>
     <definedName name="geot_PE_potential_heat" localSheetId="3">Catalonia!$C$232</definedName>
@@ -3911,6 +3914,31 @@
         </r>
       </text>
     </comment>
+    <comment ref="A232" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Enric:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+source: https://ens.dk/en/our-services/technology-catalogues/technology-data-renewable-fuels
+</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -9025,7 +9053,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2097" uniqueCount="404">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2102" uniqueCount="409">
   <si>
     <t>Type</t>
   </si>
@@ -10276,6 +10304,21 @@
   <si>
     <t xml:space="preserve">share FEH coal over FED solids </t>
   </si>
+  <si>
+    <t>Hydrogen and synthetic fuels efficency</t>
+  </si>
+  <si>
+    <t>Electricity to Amonia</t>
+  </si>
+  <si>
+    <t>Electricity to liquids synthetic fuels</t>
+  </si>
+  <si>
+    <t>Electricity to hydrogen</t>
+  </si>
+  <si>
+    <t>Electricity to synthetic methane</t>
+  </si>
 </sst>
 </file>
 
@@ -10295,7 +10338,7 @@
     <numFmt numFmtId="174" formatCode="_-* #,##0.0\ _€_-;\-* #,##0.0\ _€_-;_-* \-??\ _€_-;_-@_-"/>
     <numFmt numFmtId="175" formatCode="#,##0.00000000"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -10439,8 +10482,21 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="31">
+  <fills count="32">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -10619,6 +10675,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
         <bgColor rgb="FFF8F200"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor rgb="FF0072C6"/>
       </patternFill>
     </fill>
   </fills>
@@ -11379,7 +11441,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="320">
+  <cellXfs count="321">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -11985,35 +12047,17 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -12024,22 +12068,40 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="15" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -12051,25 +12113,25 @@
     <xf numFmtId="0" fontId="1" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -12078,10 +12140,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -13755,10 +13820,10 @@
   <sheetPr>
     <tabColor rgb="FF595959"/>
   </sheetPr>
-  <dimension ref="A2:AH229"/>
+  <dimension ref="A2:AH236"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B184" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="R200" sqref="R200:S212"/>
+    <sheetView tabSelected="1" topLeftCell="A178" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C193" sqref="C193"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15"/>
@@ -13809,7 +13874,7 @@
         <v>0.15</v>
       </c>
       <c r="C4" s="23">
-        <v>0.42302360615086498</v>
+        <v>0.36295699589181385</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -13820,7 +13885,7 @@
         <v>0.15</v>
       </c>
       <c r="C5" s="24">
-        <v>0.76230337422602645</v>
+        <v>0.76018222499999999</v>
       </c>
     </row>
     <row r="6" spans="1:16">
@@ -13832,7 +13897,7 @@
         <v>0.15</v>
       </c>
       <c r="C6" s="24">
-        <v>0.5</v>
+        <v>0.505761507</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -13844,7 +13909,7 @@
         <v>0.15</v>
       </c>
       <c r="C7" s="24">
-        <v>0.28227823191392448</v>
+        <v>0.28374165800000001</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -13853,10 +13918,10 @@
       </c>
       <c r="B8" s="4">
         <f>C8/4</f>
-        <v>8.4191698658939954E-2</v>
+        <v>8.2829583750000005E-2</v>
       </c>
       <c r="C8" s="24">
-        <v>0.33676679463575981</v>
+        <v>0.33131833500000002</v>
       </c>
     </row>
     <row r="9" spans="1:16">
@@ -13865,10 +13930,10 @@
       </c>
       <c r="B9" s="4">
         <f>C9/4</f>
-        <v>8.4191698658939954E-2</v>
+        <v>8.2829583750000005E-2</v>
       </c>
       <c r="C9" s="24">
-        <v>0.33676679463575981</v>
+        <v>0.33131833500000002</v>
       </c>
     </row>
     <row r="10" spans="1:16">
@@ -13877,10 +13942,10 @@
       </c>
       <c r="B10" s="4">
         <f>C10/4</f>
-        <v>4.7536595777077958E-2</v>
+        <v>4.4377618000000001E-2</v>
       </c>
       <c r="C10" s="24">
-        <v>0.19014638310831183</v>
+        <v>0.177510472</v>
       </c>
     </row>
     <row r="11" spans="1:16">
@@ -13889,10 +13954,10 @@
       </c>
       <c r="B11" s="25">
         <f>C11/4</f>
-        <v>9.9306596909994049E-2</v>
+        <v>9.4636784500000001E-2</v>
       </c>
       <c r="C11" s="26">
-        <v>0.3972263876399762</v>
+        <v>0.37854713800000001</v>
       </c>
     </row>
     <row r="12" spans="1:16">
@@ -14095,21 +14160,21 @@
       </c>
     </row>
     <row r="22" spans="1:16">
-      <c r="A22" s="287"/>
-      <c r="B22" s="287"/>
-      <c r="C22" s="287"/>
+      <c r="A22" s="302"/>
+      <c r="B22" s="302"/>
+      <c r="C22" s="302"/>
     </row>
     <row r="23" spans="1:16">
-      <c r="A23" s="288"/>
-      <c r="B23" s="288"/>
-      <c r="C23" s="288"/>
+      <c r="A23" s="304"/>
+      <c r="B23" s="304"/>
+      <c r="C23" s="304"/>
     </row>
     <row r="24" spans="1:16">
-      <c r="A24" s="289" t="s">
+      <c r="A24" s="305" t="s">
         <v>30</v>
       </c>
-      <c r="B24" s="289"/>
-      <c r="C24" s="289"/>
+      <c r="B24" s="305"/>
+      <c r="C24" s="305"/>
     </row>
     <row r="25" spans="1:16">
       <c r="A25" s="6" t="s">
@@ -14143,11 +14208,11 @@
       </c>
     </row>
     <row r="27" spans="1:16">
-      <c r="A27" s="290" t="s">
+      <c r="A27" s="301" t="s">
         <v>77</v>
       </c>
-      <c r="B27" s="290"/>
-      <c r="C27" s="290"/>
+      <c r="B27" s="301"/>
+      <c r="C27" s="301"/>
       <c r="E27" s="6" t="s">
         <v>78</v>
       </c>
@@ -14168,14 +14233,14 @@
       <c r="C28" s="12">
         <v>39.625999999999998</v>
       </c>
-      <c r="E28" s="290" t="s">
+      <c r="E28" s="301" t="s">
         <v>32</v>
       </c>
-      <c r="F28" s="290"/>
-      <c r="G28" s="290"/>
-      <c r="H28" s="287"/>
-      <c r="I28" s="287"/>
-      <c r="J28" s="287"/>
+      <c r="F28" s="301"/>
+      <c r="G28" s="301"/>
+      <c r="H28" s="302"/>
+      <c r="I28" s="302"/>
+      <c r="J28" s="302"/>
     </row>
     <row r="29" spans="1:16">
       <c r="A29" s="6" t="s">
@@ -14198,16 +14263,16 @@
       </c>
     </row>
     <row r="30" spans="1:16">
-      <c r="A30" s="290" t="s">
+      <c r="A30" s="301" t="s">
         <v>84</v>
       </c>
-      <c r="B30" s="290"/>
-      <c r="C30" s="290"/>
-      <c r="E30" s="290" t="s">
+      <c r="B30" s="301"/>
+      <c r="C30" s="301"/>
+      <c r="E30" s="301" t="s">
         <v>85</v>
       </c>
-      <c r="F30" s="290"/>
-      <c r="G30" s="290"/>
+      <c r="F30" s="301"/>
+      <c r="G30" s="301"/>
     </row>
     <row r="31" spans="1:16">
       <c r="A31" s="6" t="s">
@@ -14239,11 +14304,11 @@
       <c r="C32">
         <v>0.442362737444705</v>
       </c>
-      <c r="E32" s="290" t="s">
+      <c r="E32" s="301" t="s">
         <v>89</v>
       </c>
-      <c r="F32" s="290"/>
-      <c r="G32" s="290"/>
+      <c r="F32" s="301"/>
+      <c r="G32" s="301"/>
     </row>
     <row r="33" spans="1:34">
       <c r="A33" s="6" t="s">
@@ -14277,16 +14342,16 @@
       </c>
     </row>
     <row r="36" spans="1:34">
-      <c r="A36" s="290" t="s">
+      <c r="A36" s="301" t="s">
         <v>93</v>
       </c>
-      <c r="B36" s="290"/>
-      <c r="C36" s="290"/>
-      <c r="E36" s="291" t="s">
+      <c r="B36" s="301"/>
+      <c r="C36" s="301"/>
+      <c r="E36" s="297" t="s">
         <v>94</v>
       </c>
-      <c r="F36" s="291"/>
-      <c r="G36" s="291"/>
+      <c r="F36" s="297"/>
+      <c r="G36" s="297"/>
     </row>
     <row r="37" spans="1:34">
       <c r="A37" s="6" t="s">
@@ -14567,13 +14632,13 @@
       <c r="AH49" s="49"/>
     </row>
     <row r="50" spans="1:34">
-      <c r="A50" s="292" t="s">
+      <c r="A50" s="298" t="s">
         <v>115</v>
       </c>
-      <c r="B50" s="293" t="s">
+      <c r="B50" s="295" t="s">
         <v>12</v>
       </c>
-      <c r="C50" s="294">
+      <c r="C50" s="299">
         <v>14500</v>
       </c>
       <c r="D50" s="50" t="s">
@@ -14671,9 +14736,9 @@
       </c>
     </row>
     <row r="51" spans="1:34">
-      <c r="A51" s="292"/>
-      <c r="B51" s="292"/>
-      <c r="C51" s="294"/>
+      <c r="A51" s="298"/>
+      <c r="B51" s="298"/>
+      <c r="C51" s="299"/>
       <c r="D51" s="50" t="s">
         <v>117</v>
       </c>
@@ -14769,13 +14834,13 @@
       </c>
     </row>
     <row r="52" spans="1:34">
-      <c r="A52" s="295" t="s">
+      <c r="A52" s="296" t="s">
         <v>118</v>
       </c>
-      <c r="B52" s="293" t="s">
+      <c r="B52" s="295" t="s">
         <v>12</v>
       </c>
-      <c r="C52" s="296">
+      <c r="C52" s="300">
         <v>10500</v>
       </c>
       <c r="D52" s="50" t="s">
@@ -14857,9 +14922,9 @@
       <c r="AH52" s="57"/>
     </row>
     <row r="53" spans="1:34">
-      <c r="A53" s="295"/>
-      <c r="B53" s="293"/>
-      <c r="C53" s="296"/>
+      <c r="A53" s="296"/>
+      <c r="B53" s="295"/>
+      <c r="C53" s="300"/>
       <c r="D53" s="50" t="s">
         <v>117</v>
       </c>
@@ -14939,13 +15004,13 @@
       <c r="AH53" s="60"/>
     </row>
     <row r="54" spans="1:34">
-      <c r="A54" s="293" t="s">
+      <c r="A54" s="295" t="s">
         <v>119</v>
       </c>
-      <c r="B54" s="297">
+      <c r="B54" s="291">
         <v>0.5</v>
       </c>
-      <c r="C54" s="298">
+      <c r="C54" s="292">
         <v>16800</v>
       </c>
       <c r="D54" s="50" t="s">
@@ -15041,9 +15106,9 @@
       <c r="AH54" s="57"/>
     </row>
     <row r="55" spans="1:34">
-      <c r="A55" s="293"/>
-      <c r="B55" s="297"/>
-      <c r="C55" s="297"/>
+      <c r="A55" s="295"/>
+      <c r="B55" s="291"/>
+      <c r="C55" s="291"/>
       <c r="D55" s="50" t="s">
         <v>117</v>
       </c>
@@ -15175,13 +15240,13 @@
       <c r="AH56" s="49"/>
     </row>
     <row r="57" spans="1:34">
-      <c r="A57" s="293" t="s">
+      <c r="A57" s="295" t="s">
         <v>121</v>
       </c>
-      <c r="B57" s="293" t="s">
+      <c r="B57" s="295" t="s">
         <v>12</v>
       </c>
-      <c r="C57" s="298">
+      <c r="C57" s="292">
         <v>13200</v>
       </c>
       <c r="D57" s="50" t="s">
@@ -15243,9 +15308,9 @@
       <c r="AH57" s="57"/>
     </row>
     <row r="58" spans="1:34">
-      <c r="A58" s="293"/>
-      <c r="B58" s="293"/>
-      <c r="C58" s="298"/>
+      <c r="A58" s="295"/>
+      <c r="B58" s="295"/>
+      <c r="C58" s="292"/>
       <c r="D58" s="50" t="s">
         <v>117</v>
       </c>
@@ -15305,13 +15370,13 @@
       <c r="AH58" s="61"/>
     </row>
     <row r="59" spans="1:34">
-      <c r="A59" s="295" t="s">
+      <c r="A59" s="296" t="s">
         <v>122</v>
       </c>
-      <c r="B59" s="293" t="s">
+      <c r="B59" s="295" t="s">
         <v>12</v>
       </c>
-      <c r="C59" s="298">
+      <c r="C59" s="292">
         <v>14500</v>
       </c>
       <c r="D59" s="50" t="s">
@@ -15409,9 +15474,9 @@
       </c>
     </row>
     <row r="60" spans="1:34">
-      <c r="A60" s="295"/>
-      <c r="B60" s="293"/>
-      <c r="C60" s="298"/>
+      <c r="A60" s="296"/>
+      <c r="B60" s="295"/>
+      <c r="C60" s="292"/>
       <c r="D60" s="50" t="s">
         <v>117</v>
       </c>
@@ -15507,13 +15572,13 @@
       </c>
     </row>
     <row r="61" spans="1:34">
-      <c r="A61" s="293" t="s">
+      <c r="A61" s="295" t="s">
         <v>123</v>
       </c>
-      <c r="B61" s="297">
+      <c r="B61" s="291">
         <v>0.25</v>
       </c>
-      <c r="C61" s="298">
+      <c r="C61" s="292">
         <v>13000</v>
       </c>
       <c r="D61" s="50" t="s">
@@ -15605,9 +15670,9 @@
       <c r="AH61" s="57"/>
     </row>
     <row r="62" spans="1:34">
-      <c r="A62" s="293"/>
-      <c r="B62" s="297"/>
-      <c r="C62" s="297"/>
+      <c r="A62" s="295"/>
+      <c r="B62" s="291"/>
+      <c r="C62" s="291"/>
       <c r="D62" s="50" t="s">
         <v>117</v>
       </c>
@@ -15735,13 +15800,13 @@
       <c r="AH63" s="49"/>
     </row>
     <row r="64" spans="1:34">
-      <c r="A64" s="293" t="s">
+      <c r="A64" s="295" t="s">
         <v>125</v>
       </c>
-      <c r="B64" s="295" t="s">
+      <c r="B64" s="296" t="s">
         <v>12</v>
       </c>
-      <c r="C64" s="298">
+      <c r="C64" s="292">
         <v>22500</v>
       </c>
       <c r="D64" s="50" t="s">
@@ -15811,9 +15876,9 @@
       <c r="AH64" s="57"/>
     </row>
     <row r="65" spans="1:34">
-      <c r="A65" s="293"/>
-      <c r="B65" s="295"/>
-      <c r="C65" s="298"/>
+      <c r="A65" s="295"/>
+      <c r="B65" s="296"/>
+      <c r="C65" s="292"/>
       <c r="D65" s="50" t="s">
         <v>117</v>
       </c>
@@ -15919,13 +15984,13 @@
       <c r="AH66" s="49"/>
     </row>
     <row r="67" spans="1:34">
-      <c r="A67" s="293" t="s">
+      <c r="A67" s="295" t="s">
         <v>127</v>
       </c>
-      <c r="B67" s="293" t="s">
+      <c r="B67" s="295" t="s">
         <v>12</v>
       </c>
-      <c r="C67" s="298">
+      <c r="C67" s="292">
         <v>3700</v>
       </c>
       <c r="D67" s="50" t="s">
@@ -15991,9 +16056,9 @@
       <c r="AH67" s="57"/>
     </row>
     <row r="68" spans="1:34">
-      <c r="A68" s="293"/>
-      <c r="B68" s="293"/>
-      <c r="C68" s="298"/>
+      <c r="A68" s="295"/>
+      <c r="B68" s="295"/>
+      <c r="C68" s="292"/>
       <c r="D68" s="50" t="s">
         <v>117</v>
       </c>
@@ -16057,16 +16122,16 @@
       <c r="AH68" s="61"/>
     </row>
     <row r="71" spans="1:34">
-      <c r="A71" s="300" t="s">
+      <c r="A71" s="290" t="s">
         <v>128</v>
       </c>
-      <c r="B71" s="300"/>
-      <c r="C71" s="300"/>
-      <c r="E71" s="299" t="s">
+      <c r="B71" s="290"/>
+      <c r="C71" s="290"/>
+      <c r="E71" s="293" t="s">
         <v>129</v>
       </c>
-      <c r="F71" s="299"/>
-      <c r="G71" s="299"/>
+      <c r="F71" s="293"/>
+      <c r="G71" s="293"/>
     </row>
     <row r="72" spans="1:34">
       <c r="A72" s="50" t="s">
@@ -16321,10 +16386,10 @@
       </c>
     </row>
     <row r="92" spans="1:23">
-      <c r="A92" s="300" t="s">
+      <c r="A92" s="290" t="s">
         <v>30</v>
       </c>
-      <c r="B92" s="300"/>
+      <c r="B92" s="290"/>
       <c r="C92" s="11">
         <v>1995</v>
       </c>
@@ -21567,6 +21632,9 @@
         <v>82</v>
       </c>
       <c r="C193" s="104">
+        <v>100</v>
+      </c>
+      <c r="D193">
         <v>47</v>
       </c>
     </row>
@@ -21578,7 +21646,7 @@
         <v>82</v>
       </c>
       <c r="C194" s="104">
-        <v>25</v>
+        <v>70</v>
       </c>
     </row>
     <row r="195" spans="1:17">
@@ -21622,11 +21690,11 @@
       </c>
     </row>
     <row r="199" spans="1:17">
-      <c r="A199" s="301" t="s">
+      <c r="A199" s="294" t="s">
         <v>265</v>
       </c>
-      <c r="B199" s="301"/>
-      <c r="C199" s="301"/>
+      <c r="B199" s="294"/>
+      <c r="C199" s="294"/>
     </row>
     <row r="200" spans="1:17">
       <c r="A200" s="103" t="s">
@@ -21706,7 +21774,7 @@
       <c r="A205" s="279" t="s">
         <v>270</v>
       </c>
-      <c r="B205" s="309" t="s">
+      <c r="B205" s="287" t="s">
         <v>271</v>
       </c>
       <c r="C205" s="273">
@@ -21759,7 +21827,7 @@
       <c r="A206" s="278" t="s">
         <v>272</v>
       </c>
-      <c r="B206" s="310"/>
+      <c r="B206" s="288"/>
       <c r="C206" s="270">
         <v>0.5</v>
       </c>
@@ -21810,7 +21878,7 @@
       <c r="A207" s="278" t="s">
         <v>273</v>
       </c>
-      <c r="B207" s="310"/>
+      <c r="B207" s="288"/>
       <c r="C207" s="270">
         <v>0.5</v>
       </c>
@@ -21861,7 +21929,7 @@
       <c r="A208" s="278" t="s">
         <v>274</v>
       </c>
-      <c r="B208" s="310"/>
+      <c r="B208" s="288"/>
       <c r="C208" s="270">
         <v>0.5</v>
       </c>
@@ -21912,7 +21980,7 @@
       <c r="A209" s="277" t="s">
         <v>275</v>
       </c>
-      <c r="B209" s="311"/>
+      <c r="B209" s="289"/>
       <c r="C209" s="270">
         <v>0.5</v>
       </c>
@@ -21963,7 +22031,7 @@
       <c r="A210" s="276" t="s">
         <v>270</v>
       </c>
-      <c r="B210" s="309" t="s">
+      <c r="B210" s="287" t="s">
         <v>276</v>
       </c>
       <c r="C210" s="270">
@@ -22016,7 +22084,7 @@
       <c r="A211" s="271" t="s">
         <v>272</v>
       </c>
-      <c r="B211" s="310"/>
+      <c r="B211" s="288"/>
       <c r="C211" s="273">
         <v>0.5</v>
       </c>
@@ -22067,7 +22135,7 @@
       <c r="A212" s="271" t="s">
         <v>273</v>
       </c>
-      <c r="B212" s="310"/>
+      <c r="B212" s="288"/>
       <c r="C212" s="270">
         <v>0.5</v>
       </c>
@@ -22118,7 +22186,7 @@
       <c r="A213" s="271" t="s">
         <v>274</v>
       </c>
-      <c r="B213" s="310"/>
+      <c r="B213" s="288"/>
       <c r="C213" s="270">
         <v>0.5</v>
       </c>
@@ -22169,7 +22237,7 @@
       <c r="A214" s="269" t="s">
         <v>275</v>
       </c>
-      <c r="B214" s="311"/>
+      <c r="B214" s="289"/>
       <c r="C214" s="270">
         <v>0.5</v>
       </c>
@@ -22220,7 +22288,7 @@
       <c r="A215" s="272" t="s">
         <v>277</v>
       </c>
-      <c r="B215" s="309" t="s">
+      <c r="B215" s="287" t="s">
         <v>278</v>
       </c>
       <c r="C215" s="270">
@@ -22273,7 +22341,7 @@
       <c r="A216" s="271" t="s">
         <v>272</v>
       </c>
-      <c r="B216" s="310"/>
+      <c r="B216" s="288"/>
       <c r="C216" s="270">
         <v>0.5</v>
       </c>
@@ -22324,7 +22392,7 @@
       <c r="A217" s="271" t="s">
         <v>273</v>
       </c>
-      <c r="B217" s="310"/>
+      <c r="B217" s="288"/>
       <c r="C217" s="273">
         <v>0.5</v>
       </c>
@@ -22375,7 +22443,7 @@
       <c r="A218" s="271" t="s">
         <v>274</v>
       </c>
-      <c r="B218" s="310"/>
+      <c r="B218" s="288"/>
       <c r="C218" s="270">
         <v>0.5</v>
       </c>
@@ -22426,7 +22494,7 @@
       <c r="A219" s="269" t="s">
         <v>275</v>
       </c>
-      <c r="B219" s="311"/>
+      <c r="B219" s="289"/>
       <c r="C219" s="270">
         <v>0.5</v>
       </c>
@@ -22477,7 +22545,7 @@
       <c r="A220" s="272" t="s">
         <v>270</v>
       </c>
-      <c r="B220" s="309" t="s">
+      <c r="B220" s="287" t="s">
         <v>279</v>
       </c>
       <c r="C220" s="270">
@@ -22530,7 +22598,7 @@
       <c r="A221" s="271" t="s">
         <v>272</v>
       </c>
-      <c r="B221" s="310"/>
+      <c r="B221" s="288"/>
       <c r="C221" s="270">
         <v>0.5</v>
       </c>
@@ -22581,7 +22649,7 @@
       <c r="A222" s="271" t="s">
         <v>273</v>
       </c>
-      <c r="B222" s="310"/>
+      <c r="B222" s="288"/>
       <c r="C222" s="270">
         <v>0.5</v>
       </c>
@@ -22632,7 +22700,7 @@
       <c r="A223" s="271" t="s">
         <v>274</v>
       </c>
-      <c r="B223" s="310"/>
+      <c r="B223" s="288"/>
       <c r="C223" s="273">
         <v>0.5</v>
       </c>
@@ -22683,7 +22751,7 @@
       <c r="A224" s="269" t="s">
         <v>275</v>
       </c>
-      <c r="B224" s="311"/>
+      <c r="B224" s="289"/>
       <c r="C224" s="270">
         <v>0.5</v>
       </c>
@@ -22734,7 +22802,7 @@
       <c r="A225" s="272" t="s">
         <v>270</v>
       </c>
-      <c r="B225" s="309" t="s">
+      <c r="B225" s="287" t="s">
         <v>280</v>
       </c>
       <c r="C225" s="270">
@@ -22787,7 +22855,7 @@
       <c r="A226" s="271" t="s">
         <v>272</v>
       </c>
-      <c r="B226" s="310"/>
+      <c r="B226" s="288"/>
       <c r="C226" s="270">
         <v>0.5</v>
       </c>
@@ -22838,7 +22906,7 @@
       <c r="A227" s="271" t="s">
         <v>273</v>
       </c>
-      <c r="B227" s="310"/>
+      <c r="B227" s="288"/>
       <c r="C227" s="270">
         <v>0.5</v>
       </c>
@@ -22889,7 +22957,7 @@
       <c r="A228" s="271" t="s">
         <v>274</v>
       </c>
-      <c r="B228" s="310"/>
+      <c r="B228" s="288"/>
       <c r="C228" s="270">
         <v>0.5</v>
       </c>
@@ -22940,7 +23008,7 @@
       <c r="A229" s="269" t="s">
         <v>275</v>
       </c>
-      <c r="B229" s="311"/>
+      <c r="B229" s="289"/>
       <c r="C229" s="268">
         <v>0.5</v>
       </c>
@@ -22987,52 +23055,95 @@
         <v>0.5</v>
       </c>
     </row>
+    <row r="232" spans="1:17">
+      <c r="A232" s="303" t="s">
+        <v>404</v>
+      </c>
+      <c r="B232" s="303"/>
+      <c r="C232" s="303"/>
+    </row>
+    <row r="233" spans="1:17">
+      <c r="A233" t="s">
+        <v>405</v>
+      </c>
+      <c r="B233">
+        <f>0.82*B235</f>
+        <v>0.47313999999999995</v>
+      </c>
+    </row>
+    <row r="234" spans="1:17">
+      <c r="A234" t="s">
+        <v>406</v>
+      </c>
+      <c r="B234">
+        <f>B235*0.65</f>
+        <v>0.37504999999999999</v>
+      </c>
+    </row>
+    <row r="235" spans="1:17">
+      <c r="A235" t="s">
+        <v>407</v>
+      </c>
+      <c r="B235">
+        <v>0.57699999999999996</v>
+      </c>
+    </row>
+    <row r="236" spans="1:17">
+      <c r="A236" t="s">
+        <v>408</v>
+      </c>
+      <c r="B236">
+        <f>0.78*B235</f>
+        <v>0.45005999999999996</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="44">
-    <mergeCell ref="B210:B214"/>
-    <mergeCell ref="B215:B219"/>
-    <mergeCell ref="B220:B224"/>
-    <mergeCell ref="B225:B229"/>
-    <mergeCell ref="A71:C71"/>
+  <mergeCells count="45">
+    <mergeCell ref="A232:C232"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="A36:C36"/>
+    <mergeCell ref="A54:A55"/>
+    <mergeCell ref="B54:B55"/>
+    <mergeCell ref="C54:C55"/>
+    <mergeCell ref="A57:A58"/>
+    <mergeCell ref="B57:B58"/>
+    <mergeCell ref="C57:C58"/>
+    <mergeCell ref="A59:A60"/>
+    <mergeCell ref="B59:B60"/>
+    <mergeCell ref="C59:C60"/>
+    <mergeCell ref="A61:A62"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="H28:J28"/>
+    <mergeCell ref="A30:C30"/>
+    <mergeCell ref="E30:G30"/>
+    <mergeCell ref="E32:G32"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="A50:A51"/>
+    <mergeCell ref="B50:B51"/>
+    <mergeCell ref="C50:C51"/>
+    <mergeCell ref="A52:A53"/>
+    <mergeCell ref="B52:B53"/>
+    <mergeCell ref="C52:C53"/>
+    <mergeCell ref="B61:B62"/>
+    <mergeCell ref="C61:C62"/>
     <mergeCell ref="E71:G71"/>
     <mergeCell ref="A92:B92"/>
     <mergeCell ref="A199:C199"/>
-    <mergeCell ref="B205:B209"/>
     <mergeCell ref="A64:A65"/>
     <mergeCell ref="B64:B65"/>
     <mergeCell ref="C64:C65"/>
     <mergeCell ref="A67:A68"/>
     <mergeCell ref="B67:B68"/>
     <mergeCell ref="C67:C68"/>
-    <mergeCell ref="A59:A60"/>
-    <mergeCell ref="B59:B60"/>
-    <mergeCell ref="C59:C60"/>
-    <mergeCell ref="A61:A62"/>
-    <mergeCell ref="B61:B62"/>
-    <mergeCell ref="C61:C62"/>
-    <mergeCell ref="A54:A55"/>
-    <mergeCell ref="B54:B55"/>
-    <mergeCell ref="C54:C55"/>
-    <mergeCell ref="A57:A58"/>
-    <mergeCell ref="B57:B58"/>
-    <mergeCell ref="C57:C58"/>
-    <mergeCell ref="A50:A51"/>
-    <mergeCell ref="B50:B51"/>
-    <mergeCell ref="C50:C51"/>
-    <mergeCell ref="A52:A53"/>
-    <mergeCell ref="B52:B53"/>
-    <mergeCell ref="C52:C53"/>
-    <mergeCell ref="H28:J28"/>
-    <mergeCell ref="A30:C30"/>
-    <mergeCell ref="E30:G30"/>
-    <mergeCell ref="E32:G32"/>
-    <mergeCell ref="A36:C36"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="A27:C27"/>
-    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="B210:B214"/>
+    <mergeCell ref="B215:B219"/>
+    <mergeCell ref="B220:B224"/>
+    <mergeCell ref="B225:B229"/>
+    <mergeCell ref="A71:C71"/>
+    <mergeCell ref="B205:B209"/>
   </mergeCells>
   <conditionalFormatting sqref="B165:P165">
     <cfRule type="cellIs" dxfId="2" priority="2" operator="lessThan">
@@ -23409,21 +23520,21 @@
       <c r="L21" s="113"/>
     </row>
     <row r="22" spans="1:16">
-      <c r="A22" s="287"/>
-      <c r="B22" s="287"/>
-      <c r="C22" s="287"/>
+      <c r="A22" s="302"/>
+      <c r="B22" s="302"/>
+      <c r="C22" s="302"/>
     </row>
     <row r="23" spans="1:16">
-      <c r="A23" s="288"/>
-      <c r="B23" s="288"/>
-      <c r="C23" s="288"/>
+      <c r="A23" s="304"/>
+      <c r="B23" s="304"/>
+      <c r="C23" s="304"/>
     </row>
     <row r="24" spans="1:16">
-      <c r="A24" s="289" t="s">
+      <c r="A24" s="305" t="s">
         <v>30</v>
       </c>
-      <c r="B24" s="289"/>
-      <c r="C24" s="289"/>
+      <c r="B24" s="305"/>
+      <c r="C24" s="305"/>
     </row>
     <row r="25" spans="1:16">
       <c r="A25" s="6" t="s">
@@ -23457,11 +23568,11 @@
       </c>
     </row>
     <row r="27" spans="1:16">
-      <c r="A27" s="290" t="s">
+      <c r="A27" s="301" t="s">
         <v>77</v>
       </c>
-      <c r="B27" s="290"/>
-      <c r="C27" s="290"/>
+      <c r="B27" s="301"/>
+      <c r="C27" s="301"/>
       <c r="E27" s="6" t="s">
         <v>78</v>
       </c>
@@ -23482,14 +23593,14 @@
       <c r="C28" s="12">
         <v>0</v>
       </c>
-      <c r="E28" s="290" t="s">
+      <c r="E28" s="301" t="s">
         <v>32</v>
       </c>
-      <c r="F28" s="290"/>
-      <c r="G28" s="290"/>
-      <c r="H28" s="287"/>
-      <c r="I28" s="287"/>
-      <c r="J28" s="287"/>
+      <c r="F28" s="301"/>
+      <c r="G28" s="301"/>
+      <c r="H28" s="302"/>
+      <c r="I28" s="302"/>
+      <c r="J28" s="302"/>
     </row>
     <row r="29" spans="1:16">
       <c r="A29" s="6"/>
@@ -23506,16 +23617,16 @@
       </c>
     </row>
     <row r="30" spans="1:16">
-      <c r="A30" s="290" t="s">
+      <c r="A30" s="301" t="s">
         <v>84</v>
       </c>
-      <c r="B30" s="290"/>
-      <c r="C30" s="290"/>
-      <c r="E30" s="290" t="s">
+      <c r="B30" s="301"/>
+      <c r="C30" s="301"/>
+      <c r="E30" s="301" t="s">
         <v>85</v>
       </c>
-      <c r="F30" s="290"/>
-      <c r="G30" s="290"/>
+      <c r="F30" s="301"/>
+      <c r="G30" s="301"/>
     </row>
     <row r="31" spans="1:16">
       <c r="A31" s="6" t="s">
@@ -23548,11 +23659,11 @@
       <c r="C32" s="35">
         <v>0.76834862385321101</v>
       </c>
-      <c r="E32" s="290" t="s">
+      <c r="E32" s="301" t="s">
         <v>89</v>
       </c>
-      <c r="F32" s="290"/>
-      <c r="G32" s="290"/>
+      <c r="F32" s="301"/>
+      <c r="G32" s="301"/>
     </row>
     <row r="33" spans="1:34">
       <c r="A33" s="6" t="s">
@@ -23586,16 +23697,16 @@
       </c>
     </row>
     <row r="36" spans="1:34">
-      <c r="A36" s="290" t="s">
+      <c r="A36" s="301" t="s">
         <v>93</v>
       </c>
-      <c r="B36" s="290"/>
-      <c r="C36" s="290"/>
-      <c r="E36" s="291" t="s">
+      <c r="B36" s="301"/>
+      <c r="C36" s="301"/>
+      <c r="E36" s="297" t="s">
         <v>94</v>
       </c>
-      <c r="F36" s="291"/>
-      <c r="G36" s="291"/>
+      <c r="F36" s="297"/>
+      <c r="G36" s="297"/>
     </row>
     <row r="37" spans="1:34">
       <c r="A37" s="6" t="s">
@@ -23876,13 +23987,13 @@
       <c r="AH49" s="49"/>
     </row>
     <row r="50" spans="1:34">
-      <c r="A50" s="292" t="s">
+      <c r="A50" s="298" t="s">
         <v>115</v>
       </c>
-      <c r="B50" s="293" t="s">
+      <c r="B50" s="295" t="s">
         <v>12</v>
       </c>
-      <c r="C50" s="302">
+      <c r="C50" s="310">
         <v>411.48014529125697</v>
       </c>
       <c r="D50" s="50" t="s">
@@ -23956,9 +24067,9 @@
       <c r="AH50" s="52"/>
     </row>
     <row r="51" spans="1:34">
-      <c r="A51" s="292"/>
-      <c r="B51" s="292"/>
-      <c r="C51" s="302"/>
+      <c r="A51" s="298"/>
+      <c r="B51" s="298"/>
+      <c r="C51" s="310"/>
       <c r="D51" s="50" t="s">
         <v>117</v>
       </c>
@@ -24030,13 +24141,13 @@
       <c r="AH51" s="55"/>
     </row>
     <row r="52" spans="1:34">
-      <c r="A52" s="295" t="s">
+      <c r="A52" s="296" t="s">
         <v>118</v>
       </c>
-      <c r="B52" s="293" t="s">
+      <c r="B52" s="295" t="s">
         <v>12</v>
       </c>
-      <c r="C52" s="302">
+      <c r="C52" s="310">
         <v>77.5139928551</v>
       </c>
       <c r="D52" s="116" t="s">
@@ -24108,9 +24219,9 @@
       <c r="AH52" s="57"/>
     </row>
     <row r="53" spans="1:34">
-      <c r="A53" s="295"/>
-      <c r="B53" s="293"/>
-      <c r="C53" s="302"/>
+      <c r="A53" s="296"/>
+      <c r="B53" s="295"/>
+      <c r="C53" s="310"/>
       <c r="D53" s="116" t="s">
         <v>117</v>
       </c>
@@ -24180,13 +24291,13 @@
       <c r="AH53" s="60"/>
     </row>
     <row r="54" spans="1:34">
-      <c r="A54" s="293" t="s">
+      <c r="A54" s="295" t="s">
         <v>119</v>
       </c>
-      <c r="B54" s="303">
+      <c r="B54" s="312">
         <v>0.5</v>
       </c>
-      <c r="C54" s="304">
+      <c r="C54" s="311">
         <v>14500</v>
       </c>
       <c r="D54" s="116" t="s">
@@ -24284,9 +24395,9 @@
       </c>
     </row>
     <row r="55" spans="1:34">
-      <c r="A55" s="293"/>
-      <c r="B55" s="303"/>
-      <c r="C55" s="303"/>
+      <c r="A55" s="295"/>
+      <c r="B55" s="312"/>
+      <c r="C55" s="312"/>
       <c r="D55" s="116" t="s">
         <v>117</v>
       </c>
@@ -24420,13 +24531,13 @@
       <c r="AH56" s="49"/>
     </row>
     <row r="57" spans="1:34">
-      <c r="A57" s="293" t="s">
+      <c r="A57" s="295" t="s">
         <v>121</v>
       </c>
-      <c r="B57" s="293" t="s">
+      <c r="B57" s="295" t="s">
         <v>12</v>
       </c>
-      <c r="C57" s="302">
+      <c r="C57" s="310">
         <v>538.005973433431</v>
       </c>
       <c r="D57" s="50" t="s">
@@ -24498,9 +24609,9 @@
       <c r="AH57" s="57"/>
     </row>
     <row r="58" spans="1:34">
-      <c r="A58" s="293"/>
-      <c r="B58" s="293"/>
-      <c r="C58" s="302"/>
+      <c r="A58" s="295"/>
+      <c r="B58" s="295"/>
+      <c r="C58" s="310"/>
       <c r="D58" s="50" t="s">
         <v>117</v>
       </c>
@@ -24570,13 +24681,13 @@
       <c r="AH58" s="61"/>
     </row>
     <row r="59" spans="1:34">
-      <c r="A59" s="295" t="s">
+      <c r="A59" s="296" t="s">
         <v>122</v>
       </c>
-      <c r="B59" s="293" t="s">
+      <c r="B59" s="295" t="s">
         <v>12</v>
       </c>
-      <c r="C59" s="302">
+      <c r="C59" s="310">
         <v>70.703999727247606</v>
       </c>
       <c r="D59" s="50" t="s">
@@ -24654,9 +24765,9 @@
       <c r="AH59" s="57"/>
     </row>
     <row r="60" spans="1:34">
-      <c r="A60" s="295"/>
-      <c r="B60" s="293"/>
-      <c r="C60" s="302"/>
+      <c r="A60" s="296"/>
+      <c r="B60" s="295"/>
+      <c r="C60" s="310"/>
       <c r="D60" s="50" t="s">
         <v>117</v>
       </c>
@@ -24732,13 +24843,13 @@
       <c r="AH60" s="60"/>
     </row>
     <row r="61" spans="1:34">
-      <c r="A61" s="293" t="s">
+      <c r="A61" s="295" t="s">
         <v>123</v>
       </c>
-      <c r="B61" s="303">
+      <c r="B61" s="312">
         <v>0.5</v>
       </c>
-      <c r="C61" s="304">
+      <c r="C61" s="311">
         <v>14500</v>
       </c>
       <c r="D61" s="116" t="s">
@@ -24836,9 +24947,9 @@
       </c>
     </row>
     <row r="62" spans="1:34">
-      <c r="A62" s="293"/>
-      <c r="B62" s="303"/>
-      <c r="C62" s="303"/>
+      <c r="A62" s="295"/>
+      <c r="B62" s="312"/>
+      <c r="C62" s="312"/>
       <c r="D62" s="116" t="s">
         <v>117</v>
       </c>
@@ -24972,13 +25083,13 @@
       <c r="AH63" s="49"/>
     </row>
     <row r="64" spans="1:34">
-      <c r="A64" s="293" t="s">
+      <c r="A64" s="295" t="s">
         <v>125</v>
       </c>
-      <c r="B64" s="295" t="s">
+      <c r="B64" s="296" t="s">
         <v>12</v>
       </c>
-      <c r="C64" s="302">
+      <c r="C64" s="310">
         <f>+E64</f>
         <v>2309.2137610162299</v>
       </c>
@@ -25049,9 +25160,9 @@
       <c r="AH64" s="57"/>
     </row>
     <row r="65" spans="1:34">
-      <c r="A65" s="293"/>
-      <c r="B65" s="295"/>
-      <c r="C65" s="302"/>
+      <c r="A65" s="295"/>
+      <c r="B65" s="296"/>
+      <c r="C65" s="310"/>
       <c r="D65" s="50" t="s">
         <v>117</v>
       </c>
@@ -25157,13 +25268,13 @@
       <c r="AH66" s="49"/>
     </row>
     <row r="67" spans="1:34">
-      <c r="A67" s="293" t="s">
+      <c r="A67" s="295" t="s">
         <v>127</v>
       </c>
-      <c r="B67" s="293" t="s">
+      <c r="B67" s="295" t="s">
         <v>12</v>
       </c>
-      <c r="C67" s="304">
+      <c r="C67" s="311">
         <v>14500</v>
       </c>
       <c r="D67" s="50" t="s">
@@ -25261,9 +25372,9 @@
       </c>
     </row>
     <row r="68" spans="1:34">
-      <c r="A68" s="293"/>
-      <c r="B68" s="293"/>
-      <c r="C68" s="304"/>
+      <c r="A68" s="295"/>
+      <c r="B68" s="295"/>
+      <c r="C68" s="311"/>
       <c r="D68" s="50" t="s">
         <v>117</v>
       </c>
@@ -25373,11 +25484,11 @@
       </c>
     </row>
     <row r="72" spans="1:34">
-      <c r="A72" s="305" t="s">
+      <c r="A72" s="309" t="s">
         <v>283</v>
       </c>
-      <c r="B72" s="305"/>
-      <c r="C72" s="305"/>
+      <c r="B72" s="309"/>
+      <c r="C72" s="309"/>
     </row>
     <row r="73" spans="1:34">
       <c r="A73" s="123" t="s">
@@ -25416,16 +25527,16 @@
       </c>
     </row>
     <row r="78" spans="1:34">
-      <c r="A78" s="300" t="s">
+      <c r="A78" s="290" t="s">
         <v>128</v>
       </c>
-      <c r="B78" s="300"/>
-      <c r="C78" s="300"/>
-      <c r="E78" s="299" t="s">
+      <c r="B78" s="290"/>
+      <c r="C78" s="290"/>
+      <c r="E78" s="293" t="s">
         <v>129</v>
       </c>
-      <c r="F78" s="299"/>
-      <c r="G78" s="299"/>
+      <c r="F78" s="293"/>
+      <c r="G78" s="293"/>
     </row>
     <row r="79" spans="1:34">
       <c r="A79" s="64" t="s">
@@ -25680,10 +25791,10 @@
       </c>
     </row>
     <row r="99" spans="1:26">
-      <c r="A99" s="300" t="s">
+      <c r="A99" s="290" t="s">
         <v>30</v>
       </c>
-      <c r="B99" s="300"/>
+      <c r="B99" s="290"/>
       <c r="C99" s="11">
         <v>1995</v>
       </c>
@@ -31565,11 +31676,11 @@
       </c>
     </row>
     <row r="218" spans="1:4">
-      <c r="A218" s="301" t="s">
+      <c r="A218" s="294" t="s">
         <v>265</v>
       </c>
-      <c r="B218" s="301"/>
-      <c r="C218" s="301"/>
+      <c r="B218" s="294"/>
+      <c r="C218" s="294"/>
     </row>
     <row r="219" spans="1:4">
       <c r="A219" s="103" t="s">
@@ -33333,52 +33444,52 @@
     </row>
   </sheetData>
   <mergeCells count="46">
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="H28:J28"/>
+    <mergeCell ref="A30:C30"/>
+    <mergeCell ref="E30:G30"/>
+    <mergeCell ref="E32:G32"/>
+    <mergeCell ref="A36:C36"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="A50:A51"/>
+    <mergeCell ref="B50:B51"/>
+    <mergeCell ref="C50:C51"/>
+    <mergeCell ref="A52:A53"/>
+    <mergeCell ref="B52:B53"/>
+    <mergeCell ref="C52:C53"/>
+    <mergeCell ref="A54:A55"/>
+    <mergeCell ref="B54:B55"/>
+    <mergeCell ref="C54:C55"/>
+    <mergeCell ref="A57:A58"/>
+    <mergeCell ref="B57:B58"/>
+    <mergeCell ref="C57:C58"/>
+    <mergeCell ref="A59:A60"/>
+    <mergeCell ref="B59:B60"/>
+    <mergeCell ref="C59:C60"/>
+    <mergeCell ref="A61:A62"/>
+    <mergeCell ref="B61:B62"/>
+    <mergeCell ref="C61:C62"/>
+    <mergeCell ref="A64:A65"/>
+    <mergeCell ref="B64:B65"/>
+    <mergeCell ref="C64:C65"/>
+    <mergeCell ref="A67:A68"/>
+    <mergeCell ref="B67:B68"/>
+    <mergeCell ref="C67:C68"/>
+    <mergeCell ref="A72:C72"/>
+    <mergeCell ref="A78:C78"/>
+    <mergeCell ref="E78:G78"/>
+    <mergeCell ref="A99:B99"/>
+    <mergeCell ref="A218:C218"/>
     <mergeCell ref="B254:B258"/>
     <mergeCell ref="A233:B233"/>
     <mergeCell ref="B234:B238"/>
     <mergeCell ref="B239:B243"/>
     <mergeCell ref="B244:B248"/>
     <mergeCell ref="B249:B253"/>
-    <mergeCell ref="A72:C72"/>
-    <mergeCell ref="A78:C78"/>
-    <mergeCell ref="E78:G78"/>
-    <mergeCell ref="A99:B99"/>
-    <mergeCell ref="A218:C218"/>
-    <mergeCell ref="A64:A65"/>
-    <mergeCell ref="B64:B65"/>
-    <mergeCell ref="C64:C65"/>
-    <mergeCell ref="A67:A68"/>
-    <mergeCell ref="B67:B68"/>
-    <mergeCell ref="C67:C68"/>
-    <mergeCell ref="A59:A60"/>
-    <mergeCell ref="B59:B60"/>
-    <mergeCell ref="C59:C60"/>
-    <mergeCell ref="A61:A62"/>
-    <mergeCell ref="B61:B62"/>
-    <mergeCell ref="C61:C62"/>
-    <mergeCell ref="A54:A55"/>
-    <mergeCell ref="B54:B55"/>
-    <mergeCell ref="C54:C55"/>
-    <mergeCell ref="A57:A58"/>
-    <mergeCell ref="B57:B58"/>
-    <mergeCell ref="C57:C58"/>
-    <mergeCell ref="A50:A51"/>
-    <mergeCell ref="B50:B51"/>
-    <mergeCell ref="C50:C51"/>
-    <mergeCell ref="A52:A53"/>
-    <mergeCell ref="B52:B53"/>
-    <mergeCell ref="C52:C53"/>
-    <mergeCell ref="H28:J28"/>
-    <mergeCell ref="A30:C30"/>
-    <mergeCell ref="E30:G30"/>
-    <mergeCell ref="E32:G32"/>
-    <mergeCell ref="A36:C36"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="A27:C27"/>
-    <mergeCell ref="E28:G28"/>
   </mergeCells>
   <conditionalFormatting sqref="B183:P183">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
@@ -33755,21 +33866,21 @@
       <c r="L20" s="113"/>
     </row>
     <row r="21" spans="1:12">
-      <c r="A21" s="287"/>
-      <c r="B21" s="287"/>
-      <c r="C21" s="287"/>
+      <c r="A21" s="302"/>
+      <c r="B21" s="302"/>
+      <c r="C21" s="302"/>
     </row>
     <row r="22" spans="1:12">
-      <c r="A22" s="288"/>
-      <c r="B22" s="288"/>
-      <c r="C22" s="288"/>
+      <c r="A22" s="304"/>
+      <c r="B22" s="304"/>
+      <c r="C22" s="304"/>
     </row>
     <row r="23" spans="1:12">
-      <c r="A23" s="289" t="s">
+      <c r="A23" s="305" t="s">
         <v>30</v>
       </c>
-      <c r="B23" s="289"/>
-      <c r="C23" s="289"/>
+      <c r="B23" s="305"/>
+      <c r="C23" s="305"/>
     </row>
     <row r="24" spans="1:12">
       <c r="A24" s="6" t="s">
@@ -33803,11 +33914,11 @@
       </c>
     </row>
     <row r="26" spans="1:12">
-      <c r="A26" s="290" t="s">
+      <c r="A26" s="301" t="s">
         <v>77</v>
       </c>
-      <c r="B26" s="290"/>
-      <c r="C26" s="290"/>
+      <c r="B26" s="301"/>
+      <c r="C26" s="301"/>
       <c r="E26" s="6" t="s">
         <v>78</v>
       </c>
@@ -33828,14 +33939,14 @@
       <c r="C27" s="35">
         <v>0</v>
       </c>
-      <c r="E27" s="290" t="s">
+      <c r="E27" s="301" t="s">
         <v>32</v>
       </c>
-      <c r="F27" s="290"/>
-      <c r="G27" s="290"/>
-      <c r="H27" s="287"/>
-      <c r="I27" s="287"/>
-      <c r="J27" s="287"/>
+      <c r="F27" s="301"/>
+      <c r="G27" s="301"/>
+      <c r="H27" s="302"/>
+      <c r="I27" s="302"/>
+      <c r="J27" s="302"/>
     </row>
     <row r="28" spans="1:12">
       <c r="A28" s="6"/>
@@ -33852,16 +33963,16 @@
       </c>
     </row>
     <row r="29" spans="1:12">
-      <c r="A29" s="290" t="s">
+      <c r="A29" s="301" t="s">
         <v>84</v>
       </c>
-      <c r="B29" s="290"/>
-      <c r="C29" s="290"/>
-      <c r="E29" s="290" t="s">
+      <c r="B29" s="301"/>
+      <c r="C29" s="301"/>
+      <c r="E29" s="301" t="s">
         <v>85</v>
       </c>
-      <c r="F29" s="290"/>
-      <c r="G29" s="290"/>
+      <c r="F29" s="301"/>
+      <c r="G29" s="301"/>
     </row>
     <row r="30" spans="1:12">
       <c r="A30" s="181" t="s">
@@ -33893,11 +34004,11 @@
       <c r="C31" s="104">
         <v>0</v>
       </c>
-      <c r="E31" s="290" t="s">
+      <c r="E31" s="301" t="s">
         <v>89</v>
       </c>
-      <c r="F31" s="290"/>
-      <c r="G31" s="290"/>
+      <c r="F31" s="301"/>
+      <c r="G31" s="301"/>
     </row>
     <row r="32" spans="1:12">
       <c r="A32" s="182" t="s">
@@ -33931,11 +34042,11 @@
       </c>
     </row>
     <row r="35" spans="1:23">
-      <c r="A35" s="290" t="s">
+      <c r="A35" s="301" t="s">
         <v>93</v>
       </c>
-      <c r="B35" s="290"/>
-      <c r="C35" s="290"/>
+      <c r="B35" s="301"/>
+      <c r="C35" s="301"/>
     </row>
     <row r="36" spans="1:23">
       <c r="B36" s="183" t="s">
@@ -35329,13 +35440,13 @@
       <c r="AH63" s="49"/>
     </row>
     <row r="64" spans="1:34">
-      <c r="A64" s="292" t="s">
+      <c r="A64" s="298" t="s">
         <v>115</v>
       </c>
-      <c r="B64" s="293" t="s">
+      <c r="B64" s="295" t="s">
         <v>12</v>
       </c>
-      <c r="C64" s="312">
+      <c r="C64" s="314">
         <v>1.667</v>
       </c>
       <c r="D64" s="50" t="s">
@@ -35433,9 +35544,9 @@
       </c>
     </row>
     <row r="65" spans="1:34">
-      <c r="A65" s="292"/>
-      <c r="B65" s="293"/>
-      <c r="C65" s="312"/>
+      <c r="A65" s="298"/>
+      <c r="B65" s="295"/>
+      <c r="C65" s="314"/>
       <c r="D65" s="50" t="s">
         <v>117</v>
       </c>
@@ -35531,13 +35642,13 @@
       </c>
     </row>
     <row r="66" spans="1:34">
-      <c r="A66" s="295" t="s">
+      <c r="A66" s="296" t="s">
         <v>118</v>
       </c>
-      <c r="B66" s="293" t="s">
+      <c r="B66" s="295" t="s">
         <v>12</v>
       </c>
-      <c r="C66" s="296">
+      <c r="C66" s="300">
         <v>0</v>
       </c>
       <c r="D66" s="50" t="s">
@@ -35635,9 +35746,9 @@
       </c>
     </row>
     <row r="67" spans="1:34">
-      <c r="A67" s="295"/>
-      <c r="B67" s="293"/>
-      <c r="C67" s="296"/>
+      <c r="A67" s="296"/>
+      <c r="B67" s="295"/>
+      <c r="C67" s="300"/>
       <c r="D67" s="50" t="s">
         <v>117</v>
       </c>
@@ -35733,13 +35844,13 @@
       </c>
     </row>
     <row r="68" spans="1:34">
-      <c r="A68" s="293" t="s">
+      <c r="A68" s="295" t="s">
         <v>119</v>
       </c>
-      <c r="B68" s="313">
-        <v>0</v>
-      </c>
-      <c r="C68" s="312">
+      <c r="B68" s="315">
+        <v>0</v>
+      </c>
+      <c r="C68" s="314">
         <v>1.667</v>
       </c>
       <c r="D68" s="50" t="s">
@@ -35837,9 +35948,9 @@
       </c>
     </row>
     <row r="69" spans="1:34">
-      <c r="A69" s="293"/>
-      <c r="B69" s="313"/>
-      <c r="C69" s="312"/>
+      <c r="A69" s="295"/>
+      <c r="B69" s="315"/>
+      <c r="C69" s="314"/>
       <c r="D69" s="50" t="s">
         <v>117</v>
       </c>
@@ -35973,13 +36084,13 @@
       <c r="AH70" s="189"/>
     </row>
     <row r="71" spans="1:34">
-      <c r="A71" s="293" t="s">
+      <c r="A71" s="295" t="s">
         <v>121</v>
       </c>
-      <c r="B71" s="293" t="s">
+      <c r="B71" s="295" t="s">
         <v>12</v>
       </c>
-      <c r="C71" s="312">
+      <c r="C71" s="314">
         <v>0.49125463090459598</v>
       </c>
       <c r="D71" s="50" t="s">
@@ -36077,9 +36188,9 @@
       </c>
     </row>
     <row r="72" spans="1:34">
-      <c r="A72" s="293"/>
-      <c r="B72" s="293"/>
-      <c r="C72" s="312"/>
+      <c r="A72" s="295"/>
+      <c r="B72" s="295"/>
+      <c r="C72" s="314"/>
       <c r="D72" s="50" t="s">
         <v>117</v>
       </c>
@@ -36175,13 +36286,13 @@
       </c>
     </row>
     <row r="73" spans="1:34">
-      <c r="A73" s="295" t="s">
+      <c r="A73" s="296" t="s">
         <v>122</v>
       </c>
-      <c r="B73" s="293" t="s">
+      <c r="B73" s="295" t="s">
         <v>12</v>
       </c>
-      <c r="C73" s="296">
+      <c r="C73" s="300">
         <v>0</v>
       </c>
       <c r="D73" s="50" t="s">
@@ -36279,9 +36390,9 @@
       </c>
     </row>
     <row r="74" spans="1:34">
-      <c r="A74" s="295"/>
-      <c r="B74" s="293"/>
-      <c r="C74" s="296"/>
+      <c r="A74" s="296"/>
+      <c r="B74" s="295"/>
+      <c r="C74" s="300"/>
       <c r="D74" s="50" t="s">
         <v>117</v>
       </c>
@@ -36377,13 +36488,13 @@
       </c>
     </row>
     <row r="75" spans="1:34">
-      <c r="A75" s="293" t="s">
+      <c r="A75" s="295" t="s">
         <v>123</v>
       </c>
-      <c r="B75" s="313">
-        <v>0</v>
-      </c>
-      <c r="C75" s="312">
+      <c r="B75" s="315">
+        <v>0</v>
+      </c>
+      <c r="C75" s="314">
         <v>0.49125463090459598</v>
       </c>
       <c r="D75" s="50" t="s">
@@ -36481,9 +36592,9 @@
       </c>
     </row>
     <row r="76" spans="1:34">
-      <c r="A76" s="293"/>
-      <c r="B76" s="313"/>
-      <c r="C76" s="312"/>
+      <c r="A76" s="295"/>
+      <c r="B76" s="315"/>
+      <c r="C76" s="314"/>
       <c r="D76" s="50" t="s">
         <v>117</v>
       </c>
@@ -36617,13 +36728,13 @@
       <c r="AH77" s="189"/>
     </row>
     <row r="78" spans="1:34">
-      <c r="A78" s="293" t="s">
+      <c r="A78" s="295" t="s">
         <v>125</v>
       </c>
-      <c r="B78" s="295" t="s">
+      <c r="B78" s="296" t="s">
         <v>12</v>
       </c>
-      <c r="C78" s="312">
+      <c r="C78" s="314">
         <v>0.80576346799999998</v>
       </c>
       <c r="D78" s="50" t="s">
@@ -36721,9 +36832,9 @@
       </c>
     </row>
     <row r="79" spans="1:34">
-      <c r="A79" s="293"/>
-      <c r="B79" s="295"/>
-      <c r="C79" s="312"/>
+      <c r="A79" s="295"/>
+      <c r="B79" s="296"/>
+      <c r="C79" s="314"/>
       <c r="D79" s="50" t="s">
         <v>117</v>
       </c>
@@ -36857,13 +36968,13 @@
       <c r="AH80" s="189"/>
     </row>
     <row r="81" spans="1:34">
-      <c r="A81" s="293" t="s">
+      <c r="A81" s="295" t="s">
         <v>127</v>
       </c>
-      <c r="B81" s="293" t="s">
+      <c r="B81" s="295" t="s">
         <v>12</v>
       </c>
-      <c r="C81" s="296">
+      <c r="C81" s="300">
         <v>0</v>
       </c>
       <c r="D81" s="50" t="s">
@@ -36961,9 +37072,9 @@
       </c>
     </row>
     <row r="82" spans="1:34">
-      <c r="A82" s="293"/>
-      <c r="B82" s="293"/>
-      <c r="C82" s="296"/>
+      <c r="A82" s="295"/>
+      <c r="B82" s="295"/>
+      <c r="C82" s="300"/>
       <c r="D82" s="50" t="s">
         <v>117</v>
       </c>
@@ -37073,11 +37184,11 @@
       </c>
     </row>
     <row r="86" spans="1:34">
-      <c r="A86" s="290" t="s">
+      <c r="A86" s="301" t="s">
         <v>283</v>
       </c>
-      <c r="B86" s="290"/>
-      <c r="C86" s="290"/>
+      <c r="B86" s="301"/>
+      <c r="C86" s="301"/>
     </row>
     <row r="87" spans="1:34">
       <c r="A87" s="191" t="s">
@@ -37116,16 +37227,16 @@
       </c>
     </row>
     <row r="92" spans="1:34">
-      <c r="A92" s="289" t="s">
+      <c r="A92" s="305" t="s">
         <v>128</v>
       </c>
-      <c r="B92" s="289"/>
-      <c r="C92" s="289"/>
-      <c r="E92" s="314" t="s">
+      <c r="B92" s="305"/>
+      <c r="C92" s="305"/>
+      <c r="E92" s="313" t="s">
         <v>129</v>
       </c>
-      <c r="F92" s="314"/>
-      <c r="G92" s="314"/>
+      <c r="F92" s="313"/>
+      <c r="G92" s="313"/>
     </row>
     <row r="93" spans="1:34">
       <c r="A93" s="50" t="s">
@@ -37382,10 +37493,10 @@
       </c>
     </row>
     <row r="113" spans="1:27">
-      <c r="A113" s="300" t="s">
+      <c r="A113" s="290" t="s">
         <v>30</v>
       </c>
-      <c r="B113" s="300"/>
+      <c r="B113" s="290"/>
       <c r="C113" s="11">
         <v>1995</v>
       </c>
@@ -43779,11 +43890,11 @@
       </c>
     </row>
     <row r="233" spans="1:27">
-      <c r="A233" s="301" t="s">
+      <c r="A233" s="294" t="s">
         <v>265</v>
       </c>
-      <c r="B233" s="301"/>
-      <c r="C233" s="301"/>
+      <c r="B233" s="294"/>
+      <c r="C233" s="294"/>
     </row>
     <row r="234" spans="1:27">
       <c r="A234" s="103" t="s">
@@ -44848,7 +44959,7 @@
       <c r="A257" s="279" t="s">
         <v>270</v>
       </c>
-      <c r="B257" s="309" t="s">
+      <c r="B257" s="287" t="s">
         <v>243</v>
       </c>
       <c r="C257" s="273">
@@ -44901,7 +45012,7 @@
       <c r="A258" s="278" t="s">
         <v>272</v>
       </c>
-      <c r="B258" s="310"/>
+      <c r="B258" s="288"/>
       <c r="C258" s="270">
         <v>0.9</v>
       </c>
@@ -44952,7 +45063,7 @@
       <c r="A259" s="278" t="s">
         <v>273</v>
       </c>
-      <c r="B259" s="310"/>
+      <c r="B259" s="288"/>
       <c r="C259" s="270">
         <v>0.9</v>
       </c>
@@ -45003,7 +45114,7 @@
       <c r="A260" s="278" t="s">
         <v>274</v>
       </c>
-      <c r="B260" s="310"/>
+      <c r="B260" s="288"/>
       <c r="C260" s="270">
         <v>0.9</v>
       </c>
@@ -45054,7 +45165,7 @@
       <c r="A261" s="277" t="s">
         <v>275</v>
       </c>
-      <c r="B261" s="311"/>
+      <c r="B261" s="289"/>
       <c r="C261" s="270">
         <v>0.9</v>
       </c>
@@ -45105,7 +45216,7 @@
       <c r="A262" s="276" t="s">
         <v>270</v>
       </c>
-      <c r="B262" s="309" t="s">
+      <c r="B262" s="287" t="s">
         <v>244</v>
       </c>
       <c r="C262" s="270">
@@ -45158,7 +45269,7 @@
       <c r="A263" s="271" t="s">
         <v>272</v>
       </c>
-      <c r="B263" s="310"/>
+      <c r="B263" s="288"/>
       <c r="C263" s="273">
         <v>0</v>
       </c>
@@ -45209,7 +45320,7 @@
       <c r="A264" s="271" t="s">
         <v>273</v>
       </c>
-      <c r="B264" s="310"/>
+      <c r="B264" s="288"/>
       <c r="C264" s="270">
         <v>0.2</v>
       </c>
@@ -45260,7 +45371,7 @@
       <c r="A265" s="271" t="s">
         <v>274</v>
       </c>
-      <c r="B265" s="310"/>
+      <c r="B265" s="288"/>
       <c r="C265" s="270">
         <v>0.6</v>
       </c>
@@ -45311,7 +45422,7 @@
       <c r="A266" s="269" t="s">
         <v>275</v>
       </c>
-      <c r="B266" s="311"/>
+      <c r="B266" s="289"/>
       <c r="C266" s="270">
         <v>0.6</v>
       </c>
@@ -45362,7 +45473,7 @@
       <c r="A267" s="272" t="s">
         <v>277</v>
       </c>
-      <c r="B267" s="309" t="s">
+      <c r="B267" s="287" t="s">
         <v>245</v>
       </c>
       <c r="C267" s="270">
@@ -45415,7 +45526,7 @@
       <c r="A268" s="271" t="s">
         <v>272</v>
       </c>
-      <c r="B268" s="310"/>
+      <c r="B268" s="288"/>
       <c r="C268" s="270">
         <v>0.01</v>
       </c>
@@ -45466,7 +45577,7 @@
       <c r="A269" s="271" t="s">
         <v>273</v>
       </c>
-      <c r="B269" s="310"/>
+      <c r="B269" s="288"/>
       <c r="C269" s="273">
         <v>0</v>
       </c>
@@ -45517,7 +45628,7 @@
       <c r="A270" s="271" t="s">
         <v>274</v>
       </c>
-      <c r="B270" s="310"/>
+      <c r="B270" s="288"/>
       <c r="C270" s="270">
         <v>0.4</v>
       </c>
@@ -45568,7 +45679,7 @@
       <c r="A271" s="269" t="s">
         <v>275</v>
       </c>
-      <c r="B271" s="311"/>
+      <c r="B271" s="289"/>
       <c r="C271" s="270">
         <v>0.1</v>
       </c>
@@ -45619,7 +45730,7 @@
       <c r="A272" s="272" t="s">
         <v>270</v>
       </c>
-      <c r="B272" s="309" t="s">
+      <c r="B272" s="287" t="s">
         <v>246</v>
       </c>
       <c r="C272" s="270">
@@ -45672,7 +45783,7 @@
       <c r="A273" s="271" t="s">
         <v>272</v>
       </c>
-      <c r="B273" s="310"/>
+      <c r="B273" s="288"/>
       <c r="C273" s="270">
         <v>0.01</v>
       </c>
@@ -45723,7 +45834,7 @@
       <c r="A274" s="271" t="s">
         <v>273</v>
       </c>
-      <c r="B274" s="310"/>
+      <c r="B274" s="288"/>
       <c r="C274" s="270">
         <v>0.01</v>
       </c>
@@ -45774,7 +45885,7 @@
       <c r="A275" s="271" t="s">
         <v>274</v>
       </c>
-      <c r="B275" s="310"/>
+      <c r="B275" s="288"/>
       <c r="C275" s="273">
         <v>0</v>
       </c>
@@ -45825,7 +45936,7 @@
       <c r="A276" s="269" t="s">
         <v>275</v>
       </c>
-      <c r="B276" s="311"/>
+      <c r="B276" s="289"/>
       <c r="C276" s="270">
         <v>0.01</v>
       </c>
@@ -45876,7 +45987,7 @@
       <c r="A277" s="272" t="s">
         <v>270</v>
       </c>
-      <c r="B277" s="309" t="s">
+      <c r="B277" s="287" t="s">
         <v>247</v>
       </c>
       <c r="C277" s="270">
@@ -45929,7 +46040,7 @@
       <c r="A278" s="271" t="s">
         <v>272</v>
       </c>
-      <c r="B278" s="310"/>
+      <c r="B278" s="288"/>
       <c r="C278" s="270">
         <v>0</v>
       </c>
@@ -45980,7 +46091,7 @@
       <c r="A279" s="271" t="s">
         <v>273</v>
       </c>
-      <c r="B279" s="310"/>
+      <c r="B279" s="288"/>
       <c r="C279" s="270">
         <v>0.1</v>
       </c>
@@ -46031,7 +46142,7 @@
       <c r="A280" s="271" t="s">
         <v>274</v>
       </c>
-      <c r="B280" s="310"/>
+      <c r="B280" s="288"/>
       <c r="C280" s="270">
         <v>0.1</v>
       </c>
@@ -46082,7 +46193,7 @@
       <c r="A281" s="269" t="s">
         <v>275</v>
       </c>
-      <c r="B281" s="311"/>
+      <c r="B281" s="289"/>
       <c r="C281" s="268">
         <v>0</v>
       </c>
@@ -46131,50 +46242,50 @@
     </row>
   </sheetData>
   <mergeCells count="44">
-    <mergeCell ref="A86:C86"/>
-    <mergeCell ref="A92:C92"/>
-    <mergeCell ref="E92:G92"/>
-    <mergeCell ref="A113:B113"/>
-    <mergeCell ref="A233:C233"/>
+    <mergeCell ref="B257:B261"/>
+    <mergeCell ref="B262:B266"/>
+    <mergeCell ref="B267:B271"/>
+    <mergeCell ref="B272:B276"/>
+    <mergeCell ref="B277:B281"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="E27:G27"/>
+    <mergeCell ref="H27:J27"/>
+    <mergeCell ref="A29:C29"/>
+    <mergeCell ref="E29:G29"/>
+    <mergeCell ref="E31:G31"/>
+    <mergeCell ref="A35:C35"/>
+    <mergeCell ref="A64:A65"/>
+    <mergeCell ref="B64:B65"/>
+    <mergeCell ref="C64:C65"/>
+    <mergeCell ref="A66:A67"/>
+    <mergeCell ref="B66:B67"/>
+    <mergeCell ref="C66:C67"/>
+    <mergeCell ref="A68:A69"/>
+    <mergeCell ref="B68:B69"/>
+    <mergeCell ref="C68:C69"/>
+    <mergeCell ref="A71:A72"/>
+    <mergeCell ref="B71:B72"/>
+    <mergeCell ref="C71:C72"/>
+    <mergeCell ref="A73:A74"/>
+    <mergeCell ref="B73:B74"/>
+    <mergeCell ref="C73:C74"/>
+    <mergeCell ref="A75:A76"/>
+    <mergeCell ref="B75:B76"/>
+    <mergeCell ref="C75:C76"/>
     <mergeCell ref="A78:A79"/>
     <mergeCell ref="B78:B79"/>
     <mergeCell ref="C78:C79"/>
     <mergeCell ref="A81:A82"/>
     <mergeCell ref="B81:B82"/>
     <mergeCell ref="C81:C82"/>
-    <mergeCell ref="A73:A74"/>
-    <mergeCell ref="B73:B74"/>
-    <mergeCell ref="C73:C74"/>
-    <mergeCell ref="A75:A76"/>
-    <mergeCell ref="B75:B76"/>
-    <mergeCell ref="C75:C76"/>
-    <mergeCell ref="A68:A69"/>
-    <mergeCell ref="B68:B69"/>
-    <mergeCell ref="C68:C69"/>
-    <mergeCell ref="A71:A72"/>
-    <mergeCell ref="B71:B72"/>
-    <mergeCell ref="C71:C72"/>
-    <mergeCell ref="A64:A65"/>
-    <mergeCell ref="B64:B65"/>
-    <mergeCell ref="C64:C65"/>
-    <mergeCell ref="A66:A67"/>
-    <mergeCell ref="B66:B67"/>
-    <mergeCell ref="C66:C67"/>
-    <mergeCell ref="H27:J27"/>
-    <mergeCell ref="A29:C29"/>
-    <mergeCell ref="E29:G29"/>
-    <mergeCell ref="E31:G31"/>
-    <mergeCell ref="A35:C35"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="E27:G27"/>
-    <mergeCell ref="B257:B261"/>
-    <mergeCell ref="B262:B266"/>
-    <mergeCell ref="B267:B271"/>
-    <mergeCell ref="B272:B276"/>
-    <mergeCell ref="B277:B281"/>
+    <mergeCell ref="A86:C86"/>
+    <mergeCell ref="A92:C92"/>
+    <mergeCell ref="E92:G92"/>
+    <mergeCell ref="A113:B113"/>
+    <mergeCell ref="A233:C233"/>
   </mergeCells>
   <conditionalFormatting sqref="B197:P197">
     <cfRule type="cellIs" dxfId="0" priority="2" operator="lessThan">
@@ -46349,13 +46460,13 @@
       <c r="AM5" s="49"/>
     </row>
     <row r="6" spans="1:39">
-      <c r="A6" s="293" t="s">
+      <c r="A6" s="295" t="s">
         <v>348</v>
       </c>
-      <c r="B6" s="293" t="s">
+      <c r="B6" s="295" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="298">
+      <c r="C6" s="292">
         <v>12500</v>
       </c>
       <c r="D6" s="50" t="s">
@@ -46450,9 +46561,9 @@
       <c r="AM6" s="228"/>
     </row>
     <row r="7" spans="1:39">
-      <c r="A7" s="293"/>
-      <c r="B7" s="293"/>
-      <c r="C7" s="298"/>
+      <c r="A7" s="295"/>
+      <c r="B7" s="295"/>
+      <c r="C7" s="292"/>
       <c r="D7" s="50" t="s">
         <v>117</v>
       </c>
@@ -46545,13 +46656,13 @@
       <c r="AM7" s="229"/>
     </row>
     <row r="8" spans="1:39">
-      <c r="A8" s="292" t="s">
+      <c r="A8" s="298" t="s">
         <v>349</v>
       </c>
-      <c r="B8" s="293" t="s">
+      <c r="B8" s="295" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="294">
+      <c r="C8" s="299">
         <v>14500</v>
       </c>
       <c r="D8" s="50" t="s">
@@ -46654,9 +46765,9 @@
       <c r="AM8" s="231"/>
     </row>
     <row r="9" spans="1:39">
-      <c r="A9" s="292"/>
-      <c r="B9" s="292"/>
-      <c r="C9" s="294"/>
+      <c r="A9" s="298"/>
+      <c r="B9" s="298"/>
+      <c r="C9" s="299"/>
       <c r="D9" s="50" t="s">
         <v>117</v>
       </c>
@@ -46757,13 +46868,13 @@
       <c r="AM9" s="229"/>
     </row>
     <row r="10" spans="1:39">
-      <c r="A10" s="295" t="s">
+      <c r="A10" s="296" t="s">
         <v>350</v>
       </c>
-      <c r="B10" s="293" t="s">
+      <c r="B10" s="295" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="296">
+      <c r="C10" s="300">
         <v>16700</v>
       </c>
       <c r="D10" s="50" t="s">
@@ -46876,9 +46987,9 @@
       </c>
     </row>
     <row r="11" spans="1:39">
-      <c r="A11" s="295"/>
-      <c r="B11" s="293"/>
-      <c r="C11" s="296"/>
+      <c r="A11" s="296"/>
+      <c r="B11" s="295"/>
+      <c r="C11" s="300"/>
       <c r="D11" s="50" t="s">
         <v>117</v>
       </c>
@@ -46989,13 +47100,13 @@
       </c>
     </row>
     <row r="12" spans="1:39">
-      <c r="A12" s="295" t="s">
+      <c r="A12" s="296" t="s">
         <v>351</v>
       </c>
-      <c r="B12" s="293" t="s">
+      <c r="B12" s="295" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="296">
+      <c r="C12" s="300">
         <v>10500</v>
       </c>
       <c r="D12" s="50" t="s">
@@ -47082,9 +47193,9 @@
       <c r="AM12" s="228"/>
     </row>
     <row r="13" spans="1:39">
-      <c r="A13" s="295"/>
-      <c r="B13" s="293"/>
-      <c r="C13" s="296"/>
+      <c r="A13" s="296"/>
+      <c r="B13" s="295"/>
+      <c r="C13" s="300"/>
       <c r="D13" s="50" t="s">
         <v>117</v>
       </c>
@@ -47169,13 +47280,13 @@
       <c r="AM13" s="234"/>
     </row>
     <row r="14" spans="1:39">
-      <c r="A14" s="295" t="s">
+      <c r="A14" s="296" t="s">
         <v>352</v>
       </c>
-      <c r="B14" s="293" t="s">
+      <c r="B14" s="295" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="296">
+      <c r="C14" s="300">
         <v>22000</v>
       </c>
       <c r="D14" s="50" t="s">
@@ -47264,9 +47375,9 @@
       <c r="AM14" s="228"/>
     </row>
     <row r="15" spans="1:39">
-      <c r="A15" s="295"/>
-      <c r="B15" s="293"/>
-      <c r="C15" s="296"/>
+      <c r="A15" s="296"/>
+      <c r="B15" s="295"/>
+      <c r="C15" s="300"/>
       <c r="D15" s="50" t="s">
         <v>117</v>
       </c>
@@ -47353,13 +47464,13 @@
       <c r="AM15" s="234"/>
     </row>
     <row r="16" spans="1:39">
-      <c r="A16" s="295" t="s">
+      <c r="A16" s="296" t="s">
         <v>353</v>
       </c>
-      <c r="B16" s="293" t="s">
+      <c r="B16" s="295" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="296">
+      <c r="C16" s="300">
         <v>6000</v>
       </c>
       <c r="D16" s="50" t="s">
@@ -47428,9 +47539,9 @@
       <c r="AM16" s="228"/>
     </row>
     <row r="17" spans="1:39">
-      <c r="A17" s="295"/>
-      <c r="B17" s="293"/>
-      <c r="C17" s="296"/>
+      <c r="A17" s="296"/>
+      <c r="B17" s="295"/>
+      <c r="C17" s="300"/>
       <c r="D17" s="50" t="s">
         <v>117</v>
       </c>
@@ -47497,13 +47608,13 @@
       <c r="AM17" s="234"/>
     </row>
     <row r="18" spans="1:39">
-      <c r="A18" s="293" t="s">
+      <c r="A18" s="295" t="s">
         <v>354</v>
       </c>
-      <c r="B18" s="297">
+      <c r="B18" s="291">
         <v>0.5</v>
       </c>
-      <c r="C18" s="298">
+      <c r="C18" s="292">
         <v>16800</v>
       </c>
       <c r="D18" s="50" t="s">
@@ -47604,9 +47715,9 @@
       <c r="AM18" s="228"/>
     </row>
     <row r="19" spans="1:39">
-      <c r="A19" s="293"/>
-      <c r="B19" s="297"/>
-      <c r="C19" s="297"/>
+      <c r="A19" s="295"/>
+      <c r="B19" s="291"/>
+      <c r="C19" s="291"/>
       <c r="D19" s="50" t="s">
         <v>117</v>
       </c>
@@ -47748,13 +47859,13 @@
       <c r="AM20" s="49"/>
     </row>
     <row r="21" spans="1:39">
-      <c r="A21" s="293" t="s">
+      <c r="A21" s="295" t="s">
         <v>355</v>
       </c>
-      <c r="B21" s="293" t="s">
+      <c r="B21" s="295" t="s">
         <v>12</v>
       </c>
-      <c r="C21" s="298">
+      <c r="C21" s="292">
         <v>11000</v>
       </c>
       <c r="D21" s="50" t="s">
@@ -47819,9 +47930,9 @@
       <c r="AM21" s="228"/>
     </row>
     <row r="22" spans="1:39">
-      <c r="A22" s="293"/>
-      <c r="B22" s="293"/>
-      <c r="C22" s="298"/>
+      <c r="A22" s="295"/>
+      <c r="B22" s="295"/>
+      <c r="C22" s="292"/>
       <c r="D22" s="50" t="s">
         <v>117</v>
       </c>
@@ -47884,13 +47995,13 @@
       <c r="AM22" s="229"/>
     </row>
     <row r="23" spans="1:39">
-      <c r="A23" s="293" t="s">
+      <c r="A23" s="295" t="s">
         <v>356</v>
       </c>
-      <c r="B23" s="293" t="s">
+      <c r="B23" s="295" t="s">
         <v>12</v>
       </c>
-      <c r="C23" s="298">
+      <c r="C23" s="292">
         <v>22500</v>
       </c>
       <c r="D23" s="50" t="s">
@@ -47965,9 +48076,9 @@
       <c r="AM23" s="228"/>
     </row>
     <row r="24" spans="1:39">
-      <c r="A24" s="293"/>
-      <c r="B24" s="293"/>
-      <c r="C24" s="298"/>
+      <c r="A24" s="295"/>
+      <c r="B24" s="295"/>
+      <c r="C24" s="292"/>
       <c r="D24" s="50" t="s">
         <v>117</v>
       </c>
@@ -48040,13 +48151,13 @@
       <c r="AM24" s="229"/>
     </row>
     <row r="25" spans="1:39">
-      <c r="A25" s="293" t="s">
+      <c r="A25" s="295" t="s">
         <v>357</v>
       </c>
-      <c r="B25" s="293" t="s">
+      <c r="B25" s="295" t="s">
         <v>12</v>
       </c>
-      <c r="C25" s="298">
+      <c r="C25" s="292">
         <v>13200</v>
       </c>
       <c r="D25" s="50" t="s">
@@ -48113,9 +48224,9 @@
       <c r="AM25" s="228"/>
     </row>
     <row r="26" spans="1:39">
-      <c r="A26" s="293"/>
-      <c r="B26" s="293"/>
-      <c r="C26" s="298"/>
+      <c r="A26" s="295"/>
+      <c r="B26" s="295"/>
+      <c r="C26" s="292"/>
       <c r="D26" s="50" t="s">
         <v>117</v>
       </c>
@@ -48180,13 +48291,13 @@
       <c r="AM26" s="229"/>
     </row>
     <row r="27" spans="1:39">
-      <c r="A27" s="295" t="s">
+      <c r="A27" s="296" t="s">
         <v>358</v>
       </c>
-      <c r="B27" s="293" t="s">
+      <c r="B27" s="295" t="s">
         <v>12</v>
       </c>
-      <c r="C27" s="298">
+      <c r="C27" s="292">
         <v>14500</v>
       </c>
       <c r="D27" s="50" t="s">
@@ -48289,9 +48400,9 @@
       <c r="AM27" s="228"/>
     </row>
     <row r="28" spans="1:39">
-      <c r="A28" s="295"/>
-      <c r="B28" s="293"/>
-      <c r="C28" s="298"/>
+      <c r="A28" s="296"/>
+      <c r="B28" s="295"/>
+      <c r="C28" s="292"/>
       <c r="D28" s="50" t="s">
         <v>117</v>
       </c>
@@ -48392,13 +48503,13 @@
       <c r="AM28" s="229"/>
     </row>
     <row r="29" spans="1:39">
-      <c r="A29" s="295" t="s">
+      <c r="A29" s="296" t="s">
         <v>359</v>
       </c>
-      <c r="B29" s="293" t="s">
+      <c r="B29" s="295" t="s">
         <v>12</v>
       </c>
-      <c r="C29" s="298">
+      <c r="C29" s="292">
         <v>24000</v>
       </c>
       <c r="D29" s="50" t="s">
@@ -48475,9 +48586,9 @@
       <c r="AM29" s="228"/>
     </row>
     <row r="30" spans="1:39">
-      <c r="A30" s="295"/>
-      <c r="B30" s="293"/>
-      <c r="C30" s="298"/>
+      <c r="A30" s="296"/>
+      <c r="B30" s="295"/>
+      <c r="C30" s="292"/>
       <c r="D30" s="50" t="s">
         <v>117</v>
       </c>
@@ -48552,13 +48663,13 @@
       <c r="AM30" s="229"/>
     </row>
     <row r="31" spans="1:39">
-      <c r="A31" s="295" t="s">
+      <c r="A31" s="296" t="s">
         <v>360</v>
       </c>
-      <c r="B31" s="293" t="s">
+      <c r="B31" s="295" t="s">
         <v>12</v>
       </c>
-      <c r="C31" s="298">
+      <c r="C31" s="292">
         <v>2800</v>
       </c>
       <c r="D31" s="50" t="s">
@@ -48617,9 +48728,9 @@
       <c r="AM31" s="228"/>
     </row>
     <row r="32" spans="1:39">
-      <c r="A32" s="295"/>
-      <c r="B32" s="293"/>
-      <c r="C32" s="298"/>
+      <c r="A32" s="296"/>
+      <c r="B32" s="295"/>
+      <c r="C32" s="292"/>
       <c r="D32" s="50" t="s">
         <v>117</v>
       </c>
@@ -48676,13 +48787,13 @@
       <c r="AM32" s="229"/>
     </row>
     <row r="33" spans="1:39">
-      <c r="A33" s="293" t="s">
+      <c r="A33" s="295" t="s">
         <v>361</v>
       </c>
-      <c r="B33" s="297">
+      <c r="B33" s="291">
         <v>0.25</v>
       </c>
-      <c r="C33" s="298">
+      <c r="C33" s="292">
         <v>13000</v>
       </c>
       <c r="D33" s="50" t="s">
@@ -48779,9 +48890,9 @@
       <c r="AM33" s="228"/>
     </row>
     <row r="34" spans="1:39">
-      <c r="A34" s="293"/>
-      <c r="B34" s="297"/>
-      <c r="C34" s="297"/>
+      <c r="A34" s="295"/>
+      <c r="B34" s="291"/>
+      <c r="C34" s="291"/>
       <c r="D34" s="50" t="s">
         <v>117</v>
       </c>
@@ -48876,14 +48987,14 @@
       <c r="AM34" s="229"/>
     </row>
     <row r="35" spans="1:39">
-      <c r="A35" s="293" t="s">
+      <c r="A35" s="295" t="s">
         <v>362</v>
       </c>
-      <c r="B35" s="315">
+      <c r="B35" s="320">
         <f>40/150</f>
         <v>0.26666666666666666</v>
       </c>
-      <c r="C35" s="298">
+      <c r="C35" s="292">
         <v>20000</v>
       </c>
       <c r="D35" s="50" t="s">
@@ -48968,9 +49079,9 @@
       <c r="AM35" s="228"/>
     </row>
     <row r="36" spans="1:39">
-      <c r="A36" s="293"/>
-      <c r="B36" s="315"/>
-      <c r="C36" s="298"/>
+      <c r="A36" s="295"/>
+      <c r="B36" s="320"/>
+      <c r="C36" s="292"/>
       <c r="D36" s="50" t="s">
         <v>117</v>
       </c>
@@ -49096,13 +49207,13 @@
       <c r="AM37" s="49"/>
     </row>
     <row r="38" spans="1:39">
-      <c r="A38" s="295" t="s">
+      <c r="A38" s="296" t="s">
         <v>363</v>
       </c>
-      <c r="B38" s="295" t="s">
+      <c r="B38" s="296" t="s">
         <v>12</v>
       </c>
-      <c r="C38" s="296">
+      <c r="C38" s="300">
         <v>27800</v>
       </c>
       <c r="D38" s="50" t="s">
@@ -49175,9 +49286,9 @@
       <c r="AM38" s="228"/>
     </row>
     <row r="39" spans="1:39">
-      <c r="A39" s="295"/>
-      <c r="B39" s="295"/>
-      <c r="C39" s="296"/>
+      <c r="A39" s="296"/>
+      <c r="B39" s="296"/>
+      <c r="C39" s="300"/>
       <c r="D39" s="50" t="s">
         <v>117</v>
       </c>
@@ -49248,13 +49359,13 @@
       <c r="AM39" s="234"/>
     </row>
     <row r="40" spans="1:39">
-      <c r="A40" s="293" t="s">
+      <c r="A40" s="295" t="s">
         <v>364</v>
       </c>
-      <c r="B40" s="295" t="s">
+      <c r="B40" s="296" t="s">
         <v>12</v>
       </c>
-      <c r="C40" s="298">
+      <c r="C40" s="292">
         <v>14500</v>
       </c>
       <c r="D40" s="50" t="s">
@@ -49357,9 +49468,9 @@
       <c r="AM40" s="228"/>
     </row>
     <row r="41" spans="1:39">
-      <c r="A41" s="293"/>
-      <c r="B41" s="295"/>
-      <c r="C41" s="298"/>
+      <c r="A41" s="295"/>
+      <c r="B41" s="296"/>
+      <c r="C41" s="292"/>
       <c r="D41" s="50" t="s">
         <v>117</v>
       </c>
@@ -49460,13 +49571,13 @@
       <c r="AM41" s="229"/>
     </row>
     <row r="42" spans="1:39">
-      <c r="A42" s="293" t="s">
+      <c r="A42" s="295" t="s">
         <v>365</v>
       </c>
-      <c r="B42" s="295" t="s">
+      <c r="B42" s="296" t="s">
         <v>12</v>
       </c>
-      <c r="C42" s="298">
+      <c r="C42" s="292">
         <v>22500</v>
       </c>
       <c r="D42" s="50" t="s">
@@ -49541,9 +49652,9 @@
       <c r="AM42" s="228"/>
     </row>
     <row r="43" spans="1:39">
-      <c r="A43" s="293"/>
-      <c r="B43" s="295"/>
-      <c r="C43" s="298"/>
+      <c r="A43" s="295"/>
+      <c r="B43" s="296"/>
+      <c r="C43" s="292"/>
       <c r="D43" s="50" t="s">
         <v>117</v>
       </c>
@@ -49616,13 +49727,13 @@
       <c r="AM43" s="229"/>
     </row>
     <row r="44" spans="1:39">
-      <c r="A44" s="293" t="s">
+      <c r="A44" s="295" t="s">
         <v>366</v>
       </c>
-      <c r="B44" s="295" t="s">
+      <c r="B44" s="296" t="s">
         <v>12</v>
       </c>
-      <c r="C44" s="298">
+      <c r="C44" s="292">
         <v>31500</v>
       </c>
       <c r="D44" s="50" t="s">
@@ -49709,9 +49820,9 @@
       <c r="AM44" s="228"/>
     </row>
     <row r="45" spans="1:39">
-      <c r="A45" s="293"/>
-      <c r="B45" s="295"/>
-      <c r="C45" s="298"/>
+      <c r="A45" s="295"/>
+      <c r="B45" s="296"/>
+      <c r="C45" s="292"/>
       <c r="D45" s="50" t="s">
         <v>117</v>
       </c>
@@ -49839,13 +49950,13 @@
       <c r="AM46" s="49"/>
     </row>
     <row r="47" spans="1:39">
-      <c r="A47" s="293" t="s">
+      <c r="A47" s="295" t="s">
         <v>367</v>
       </c>
-      <c r="B47" s="293" t="s">
+      <c r="B47" s="295" t="s">
         <v>12</v>
       </c>
-      <c r="C47" s="298">
+      <c r="C47" s="292">
         <v>3700</v>
       </c>
       <c r="D47" s="50" t="s">
@@ -49916,9 +50027,9 @@
       <c r="AM47" s="228"/>
     </row>
     <row r="48" spans="1:39">
-      <c r="A48" s="293"/>
-      <c r="B48" s="293"/>
-      <c r="C48" s="298"/>
+      <c r="A48" s="295"/>
+      <c r="B48" s="295"/>
+      <c r="C48" s="292"/>
       <c r="D48" s="50" t="s">
         <v>117</v>
       </c>
@@ -49987,13 +50098,13 @@
       <c r="AM48" s="229"/>
     </row>
     <row r="49" spans="1:39">
-      <c r="A49" s="293" t="s">
+      <c r="A49" s="295" t="s">
         <v>368</v>
       </c>
-      <c r="B49" s="293" t="s">
+      <c r="B49" s="295" t="s">
         <v>12</v>
       </c>
-      <c r="C49" s="298">
+      <c r="C49" s="292">
         <v>4000</v>
       </c>
       <c r="D49" s="50" t="s">
@@ -50064,9 +50175,9 @@
       <c r="AM49" s="228"/>
     </row>
     <row r="50" spans="1:39">
-      <c r="A50" s="293"/>
-      <c r="B50" s="293"/>
-      <c r="C50" s="298"/>
+      <c r="A50" s="295"/>
+      <c r="B50" s="295"/>
+      <c r="C50" s="292"/>
       <c r="D50" s="50" t="s">
         <v>117</v>
       </c>
@@ -50266,10 +50377,10 @@
       <c r="A56" s="316" t="s">
         <v>370</v>
       </c>
-      <c r="B56" s="293" t="s">
+      <c r="B56" s="295" t="s">
         <v>12</v>
       </c>
-      <c r="C56" s="298">
+      <c r="C56" s="292">
         <f>+E56</f>
         <v>299.97278596475797</v>
       </c>
@@ -50342,8 +50453,8 @@
     </row>
     <row r="57" spans="1:39">
       <c r="A57" s="316"/>
-      <c r="B57" s="293"/>
-      <c r="C57" s="298"/>
+      <c r="B57" s="295"/>
+      <c r="C57" s="292"/>
       <c r="D57" s="50" t="s">
         <v>117</v>
       </c>
@@ -50415,10 +50526,10 @@
       <c r="A58" s="316" t="s">
         <v>371</v>
       </c>
-      <c r="B58" s="293" t="s">
+      <c r="B58" s="295" t="s">
         <v>12</v>
       </c>
-      <c r="C58" s="298">
+      <c r="C58" s="292">
         <f>+I58</f>
         <v>304.471539948898</v>
       </c>
@@ -50482,8 +50593,8 @@
     </row>
     <row r="59" spans="1:39">
       <c r="A59" s="316"/>
-      <c r="B59" s="293"/>
-      <c r="C59" s="298"/>
+      <c r="B59" s="295"/>
+      <c r="C59" s="292"/>
       <c r="D59" s="50" t="s">
         <v>117</v>
       </c>
@@ -50546,10 +50657,10 @@
       <c r="A60" s="316" t="s">
         <v>372</v>
       </c>
-      <c r="B60" s="293" t="s">
+      <c r="B60" s="295" t="s">
         <v>12</v>
       </c>
-      <c r="C60" s="298">
+      <c r="C60" s="292">
         <f>+K60</f>
         <v>411.48014529125697</v>
       </c>
@@ -50613,8 +50724,8 @@
     </row>
     <row r="61" spans="1:39">
       <c r="A61" s="316"/>
-      <c r="B61" s="293"/>
-      <c r="C61" s="298"/>
+      <c r="B61" s="295"/>
+      <c r="C61" s="292"/>
       <c r="D61" s="50" t="s">
         <v>117</v>
       </c>
@@ -50677,10 +50788,10 @@
       <c r="A62" s="316" t="s">
         <v>373</v>
       </c>
-      <c r="B62" s="293" t="s">
+      <c r="B62" s="295" t="s">
         <v>12</v>
       </c>
-      <c r="C62" s="298">
+      <c r="C62" s="292">
         <f>+E62</f>
         <v>14.1809996187</v>
       </c>
@@ -50759,8 +50870,8 @@
     </row>
     <row r="63" spans="1:39">
       <c r="A63" s="316"/>
-      <c r="B63" s="293"/>
-      <c r="C63" s="298"/>
+      <c r="B63" s="295"/>
+      <c r="C63" s="292"/>
       <c r="D63" s="50" t="s">
         <v>117</v>
       </c>
@@ -50838,10 +50949,10 @@
       <c r="A64" s="316" t="s">
         <v>374</v>
       </c>
-      <c r="B64" s="293" t="s">
+      <c r="B64" s="295" t="s">
         <v>12</v>
       </c>
-      <c r="C64" s="298">
+      <c r="C64" s="292">
         <f>+E64</f>
         <v>77.5139928551</v>
       </c>
@@ -50899,8 +51010,8 @@
     </row>
     <row r="65" spans="1:39">
       <c r="A65" s="316"/>
-      <c r="B65" s="293"/>
-      <c r="C65" s="298"/>
+      <c r="B65" s="295"/>
+      <c r="C65" s="292"/>
       <c r="D65" s="116" t="s">
         <v>117</v>
       </c>
@@ -50957,10 +51068,10 @@
       <c r="A66" s="316" t="s">
         <v>375</v>
       </c>
-      <c r="B66" s="293" t="s">
+      <c r="B66" s="295" t="s">
         <v>12</v>
       </c>
-      <c r="C66" s="298">
+      <c r="C66" s="292">
         <f>+E66</f>
         <v>103.654610475</v>
       </c>
@@ -51035,8 +51146,8 @@
     </row>
     <row r="67" spans="1:39">
       <c r="A67" s="316"/>
-      <c r="B67" s="293"/>
-      <c r="C67" s="298"/>
+      <c r="B67" s="295"/>
+      <c r="C67" s="292"/>
       <c r="D67" s="50" t="s">
         <v>117</v>
       </c>
@@ -51110,11 +51221,11 @@
       <c r="A68" s="317" t="s">
         <v>12</v>
       </c>
-      <c r="B68" s="297">
+      <c r="B68" s="291">
         <f>+E68</f>
         <v>0</v>
       </c>
-      <c r="C68" s="298">
+      <c r="C68" s="292">
         <v>0</v>
       </c>
       <c r="D68" s="50" t="s">
@@ -51158,8 +51269,8 @@
     </row>
     <row r="69" spans="1:39">
       <c r="A69" s="317"/>
-      <c r="B69" s="297"/>
-      <c r="C69" s="298"/>
+      <c r="B69" s="291"/>
+      <c r="C69" s="292"/>
       <c r="D69" s="50" t="s">
         <v>117</v>
       </c>
@@ -51236,10 +51347,10 @@
       <c r="A71" s="316" t="s">
         <v>376</v>
       </c>
-      <c r="B71" s="293" t="s">
+      <c r="B71" s="295" t="s">
         <v>12</v>
       </c>
-      <c r="C71" s="298">
+      <c r="C71" s="292">
         <f>+E71</f>
         <v>542.01797255752001</v>
       </c>
@@ -51318,8 +51429,8 @@
     </row>
     <row r="72" spans="1:39">
       <c r="A72" s="316"/>
-      <c r="B72" s="293"/>
-      <c r="C72" s="298"/>
+      <c r="B72" s="295"/>
+      <c r="C72" s="292"/>
       <c r="D72" s="50" t="s">
         <v>117</v>
       </c>
@@ -51397,10 +51508,10 @@
       <c r="A73" s="316" t="s">
         <v>377</v>
       </c>
-      <c r="B73" s="293" t="s">
+      <c r="B73" s="295" t="s">
         <v>12</v>
       </c>
-      <c r="C73" s="298">
+      <c r="C73" s="292">
         <f>+G73</f>
         <v>538.005973433431</v>
       </c>
@@ -51467,8 +51578,8 @@
     </row>
     <row r="74" spans="1:39">
       <c r="A74" s="316"/>
-      <c r="B74" s="293"/>
-      <c r="C74" s="298"/>
+      <c r="B74" s="295"/>
+      <c r="C74" s="292"/>
       <c r="D74" s="50" t="s">
         <v>117</v>
       </c>
@@ -51534,10 +51645,10 @@
       <c r="A75" s="316" t="s">
         <v>378</v>
       </c>
-      <c r="B75" s="293" t="s">
+      <c r="B75" s="295" t="s">
         <v>12</v>
       </c>
-      <c r="C75" s="298">
+      <c r="C75" s="292">
         <f>+H75</f>
         <v>540.81199952922702</v>
       </c>
@@ -51604,8 +51715,8 @@
     </row>
     <row r="76" spans="1:39">
       <c r="A76" s="316"/>
-      <c r="B76" s="293"/>
-      <c r="C76" s="298"/>
+      <c r="B76" s="295"/>
+      <c r="C76" s="292"/>
       <c r="D76" s="50" t="s">
         <v>117</v>
       </c>
@@ -51671,10 +51782,10 @@
       <c r="A77" s="316" t="s">
         <v>379</v>
       </c>
-      <c r="B77" s="293" t="s">
+      <c r="B77" s="295" t="s">
         <v>12</v>
       </c>
-      <c r="C77" s="298">
+      <c r="C77" s="292">
         <f>+E77</f>
         <v>70.703999727247606</v>
       </c>
@@ -51757,8 +51868,8 @@
     </row>
     <row r="78" spans="1:39">
       <c r="A78" s="316"/>
-      <c r="B78" s="293"/>
-      <c r="C78" s="298"/>
+      <c r="B78" s="295"/>
+      <c r="C78" s="292"/>
       <c r="D78" s="50" t="s">
         <v>117</v>
       </c>
@@ -51840,10 +51951,10 @@
       <c r="A79" s="316" t="s">
         <v>380</v>
       </c>
-      <c r="B79" s="293" t="s">
+      <c r="B79" s="295" t="s">
         <v>12</v>
       </c>
-      <c r="C79" s="298">
+      <c r="C79" s="292">
         <f>+E79</f>
         <v>487.78598291406001</v>
       </c>
@@ -51928,8 +52039,8 @@
     </row>
     <row r="80" spans="1:39">
       <c r="A80" s="316"/>
-      <c r="B80" s="293"/>
-      <c r="C80" s="298"/>
+      <c r="B80" s="295"/>
+      <c r="C80" s="292"/>
       <c r="D80" s="50" t="s">
         <v>117</v>
       </c>
@@ -52013,10 +52124,10 @@
       <c r="A81" s="316" t="s">
         <v>381</v>
       </c>
-      <c r="B81" s="293" t="s">
+      <c r="B81" s="295" t="s">
         <v>12</v>
       </c>
-      <c r="C81" s="298">
+      <c r="C81" s="292">
         <f>+E81</f>
         <v>881.48595333719004</v>
       </c>
@@ -52095,8 +52206,8 @@
     </row>
     <row r="82" spans="1:39">
       <c r="A82" s="316"/>
-      <c r="B82" s="293"/>
-      <c r="C82" s="298"/>
+      <c r="B82" s="295"/>
+      <c r="C82" s="292"/>
       <c r="D82" s="50" t="s">
         <v>117</v>
       </c>
@@ -52174,11 +52285,11 @@
       <c r="A83" s="317" t="s">
         <v>12</v>
       </c>
-      <c r="B83" s="297">
+      <c r="B83" s="291">
         <f>+E83</f>
         <v>0</v>
       </c>
-      <c r="C83" s="298">
+      <c r="C83" s="292">
         <v>0</v>
       </c>
       <c r="D83" s="50" t="s">
@@ -52222,8 +52333,8 @@
     </row>
     <row r="84" spans="1:39">
       <c r="A84" s="317"/>
-      <c r="B84" s="297"/>
-      <c r="C84" s="297"/>
+      <c r="B84" s="291"/>
+      <c r="C84" s="291"/>
       <c r="D84" s="50" t="s">
         <v>117</v>
       </c>
@@ -52267,11 +52378,11 @@
       <c r="A85" s="317" t="s">
         <v>12</v>
       </c>
-      <c r="B85" s="315">
+      <c r="B85" s="320">
         <f>+E85</f>
         <v>0</v>
       </c>
-      <c r="C85" s="298">
+      <c r="C85" s="292">
         <v>0</v>
       </c>
       <c r="D85" s="50" t="s">
@@ -52315,8 +52426,8 @@
     </row>
     <row r="86" spans="1:39">
       <c r="A86" s="317"/>
-      <c r="B86" s="315"/>
-      <c r="C86" s="298"/>
+      <c r="B86" s="320"/>
+      <c r="C86" s="292"/>
       <c r="D86" s="50" t="s">
         <v>117</v>
       </c>
@@ -52390,13 +52501,13 @@
       <c r="AC87" s="48"/>
     </row>
     <row r="88" spans="1:39">
-      <c r="A88" s="318" t="s">
+      <c r="A88" s="319" t="s">
         <v>12</v>
       </c>
-      <c r="B88" s="295" t="s">
+      <c r="B88" s="296" t="s">
         <v>12</v>
       </c>
-      <c r="C88" s="296">
+      <c r="C88" s="300">
         <v>0</v>
       </c>
       <c r="D88" s="50" t="s">
@@ -52439,9 +52550,9 @@
       <c r="AM88" s="228"/>
     </row>
     <row r="89" spans="1:39">
-      <c r="A89" s="318"/>
-      <c r="B89" s="295"/>
-      <c r="C89" s="296"/>
+      <c r="A89" s="319"/>
+      <c r="B89" s="296"/>
+      <c r="C89" s="300"/>
       <c r="D89" s="50" t="s">
         <v>117</v>
       </c>
@@ -52485,10 +52596,10 @@
       <c r="A90" s="316" t="s">
         <v>382</v>
       </c>
-      <c r="B90" s="295" t="s">
+      <c r="B90" s="296" t="s">
         <v>12</v>
       </c>
-      <c r="C90" s="298">
+      <c r="C90" s="292">
         <f>+E90</f>
         <v>2314.1137144060499</v>
       </c>
@@ -52543,8 +52654,8 @@
     </row>
     <row r="91" spans="1:39">
       <c r="A91" s="316"/>
-      <c r="B91" s="295"/>
-      <c r="C91" s="298"/>
+      <c r="B91" s="296"/>
+      <c r="C91" s="292"/>
       <c r="D91" s="50" t="s">
         <v>117</v>
       </c>
@@ -52598,10 +52709,10 @@
       <c r="A92" s="316" t="s">
         <v>383</v>
       </c>
-      <c r="B92" s="295" t="s">
+      <c r="B92" s="296" t="s">
         <v>12</v>
       </c>
-      <c r="C92" s="298">
+      <c r="C92" s="292">
         <f>+E92</f>
         <v>2309.2137610162299</v>
       </c>
@@ -52678,8 +52789,8 @@
     </row>
     <row r="93" spans="1:39">
       <c r="A93" s="316"/>
-      <c r="B93" s="295"/>
-      <c r="C93" s="298"/>
+      <c r="B93" s="296"/>
+      <c r="C93" s="292"/>
       <c r="D93" s="50" t="s">
         <v>117</v>
       </c>
@@ -52755,10 +52866,10 @@
       <c r="A94" s="316" t="s">
         <v>384</v>
       </c>
-      <c r="B94" s="295" t="s">
+      <c r="B94" s="296" t="s">
         <v>12</v>
       </c>
-      <c r="C94" s="298">
+      <c r="C94" s="292">
         <f>+E94</f>
         <v>2588.6587743893901</v>
       </c>
@@ -52833,8 +52944,8 @@
     </row>
     <row r="95" spans="1:39">
       <c r="A95" s="316"/>
-      <c r="B95" s="295"/>
-      <c r="C95" s="298"/>
+      <c r="B95" s="296"/>
+      <c r="C95" s="292"/>
       <c r="D95" s="50" t="s">
         <v>117</v>
       </c>
@@ -52939,10 +53050,10 @@
     </row>
     <row r="97" spans="1:39">
       <c r="A97" s="317"/>
-      <c r="B97" s="293" t="s">
+      <c r="B97" s="295" t="s">
         <v>12</v>
       </c>
-      <c r="C97" s="298">
+      <c r="C97" s="292">
         <f>+E97</f>
         <v>0</v>
       </c>
@@ -52987,8 +53098,8 @@
     </row>
     <row r="98" spans="1:39">
       <c r="A98" s="317"/>
-      <c r="B98" s="293"/>
-      <c r="C98" s="298"/>
+      <c r="B98" s="295"/>
+      <c r="C98" s="292"/>
       <c r="D98" s="50" t="s">
         <v>117</v>
       </c>
@@ -53030,10 +53141,10 @@
     </row>
     <row r="99" spans="1:39">
       <c r="A99" s="317"/>
-      <c r="B99" s="293" t="s">
+      <c r="B99" s="295" t="s">
         <v>12</v>
       </c>
-      <c r="C99" s="319">
+      <c r="C99" s="318">
         <f>+E99</f>
         <v>0</v>
       </c>
@@ -53078,8 +53189,8 @@
     </row>
     <row r="100" spans="1:39">
       <c r="A100" s="317"/>
-      <c r="B100" s="293"/>
-      <c r="C100" s="319"/>
+      <c r="B100" s="295"/>
+      <c r="C100" s="318"/>
       <c r="D100" s="50" t="s">
         <v>117</v>
       </c>
@@ -53251,10 +53362,10 @@
       <c r="A107" s="316" t="s">
         <v>386</v>
       </c>
-      <c r="B107" s="293" t="s">
+      <c r="B107" s="295" t="s">
         <v>12</v>
       </c>
-      <c r="C107" s="298">
+      <c r="C107" s="292">
         <f>+E107</f>
         <v>5.8600034000000001</v>
       </c>
@@ -53303,8 +53414,8 @@
     </row>
     <row r="108" spans="1:39">
       <c r="A108" s="316"/>
-      <c r="B108" s="293"/>
-      <c r="C108" s="298"/>
+      <c r="B108" s="295"/>
+      <c r="C108" s="292"/>
       <c r="D108" s="50" t="s">
         <v>117</v>
       </c>
@@ -53352,10 +53463,10 @@
       <c r="A109" s="316" t="s">
         <v>387</v>
       </c>
-      <c r="B109" s="293" t="s">
+      <c r="B109" s="295" t="s">
         <v>12</v>
       </c>
-      <c r="C109" s="298">
+      <c r="C109" s="292">
         <f>+E109</f>
         <v>5.86</v>
       </c>
@@ -53406,8 +53517,8 @@
     </row>
     <row r="110" spans="1:39">
       <c r="A110" s="316"/>
-      <c r="B110" s="293"/>
-      <c r="C110" s="298"/>
+      <c r="B110" s="295"/>
+      <c r="C110" s="292"/>
       <c r="D110" s="50" t="s">
         <v>117</v>
       </c>
@@ -53457,10 +53568,10 @@
       <c r="A111" s="316" t="s">
         <v>388</v>
       </c>
-      <c r="B111" s="293" t="s">
+      <c r="B111" s="295" t="s">
         <v>12</v>
       </c>
-      <c r="C111" s="298">
+      <c r="C111" s="292">
         <f>+E111</f>
         <v>7.2400155000000002</v>
       </c>
@@ -53537,8 +53648,8 @@
     </row>
     <row r="112" spans="1:39">
       <c r="A112" s="316"/>
-      <c r="B112" s="293"/>
-      <c r="C112" s="298"/>
+      <c r="B112" s="295"/>
+      <c r="C112" s="292"/>
       <c r="D112" s="50" t="s">
         <v>117</v>
       </c>
@@ -53614,10 +53725,10 @@
       <c r="A113" s="316" t="s">
         <v>389</v>
       </c>
-      <c r="B113" s="293" t="s">
+      <c r="B113" s="295" t="s">
         <v>12</v>
       </c>
-      <c r="C113" s="298">
+      <c r="C113" s="292">
         <f>+E113</f>
         <v>0</v>
       </c>
@@ -53664,8 +53775,8 @@
     </row>
     <row r="114" spans="1:39">
       <c r="A114" s="316"/>
-      <c r="B114" s="293"/>
-      <c r="C114" s="298"/>
+      <c r="B114" s="295"/>
+      <c r="C114" s="292"/>
       <c r="D114" s="50" t="s">
         <v>117</v>
       </c>
@@ -53711,10 +53822,10 @@
       <c r="A115" s="316" t="s">
         <v>390</v>
       </c>
-      <c r="B115" s="293" t="s">
+      <c r="B115" s="295" t="s">
         <v>12</v>
       </c>
-      <c r="C115" s="298">
+      <c r="C115" s="292">
         <f>+E115</f>
         <v>0</v>
       </c>
@@ -53761,8 +53872,8 @@
     </row>
     <row r="116" spans="1:39">
       <c r="A116" s="316"/>
-      <c r="B116" s="293"/>
-      <c r="C116" s="298"/>
+      <c r="B116" s="295"/>
+      <c r="C116" s="292"/>
       <c r="D116" s="50" t="s">
         <v>117</v>
       </c>
@@ -53808,10 +53919,10 @@
       <c r="A117" s="316" t="s">
         <v>391</v>
       </c>
-      <c r="B117" s="293" t="s">
+      <c r="B117" s="295" t="s">
         <v>12</v>
       </c>
-      <c r="C117" s="298">
+      <c r="C117" s="292">
         <f>+E117</f>
         <v>0</v>
       </c>
@@ -53858,8 +53969,8 @@
     </row>
     <row r="118" spans="1:39">
       <c r="A118" s="316"/>
-      <c r="B118" s="293"/>
-      <c r="C118" s="298"/>
+      <c r="B118" s="295"/>
+      <c r="C118" s="292"/>
       <c r="D118" s="50" t="s">
         <v>117</v>
       </c>
@@ -53905,11 +54016,11 @@
       <c r="A119" s="317" t="s">
         <v>12</v>
       </c>
-      <c r="B119" s="297">
+      <c r="B119" s="291">
         <f>+E119</f>
         <v>0</v>
       </c>
-      <c r="C119" s="298">
+      <c r="C119" s="292">
         <v>0</v>
       </c>
       <c r="D119" s="50" t="s">
@@ -53953,8 +54064,8 @@
     </row>
     <row r="120" spans="1:39">
       <c r="A120" s="317"/>
-      <c r="B120" s="297"/>
-      <c r="C120" s="298"/>
+      <c r="B120" s="291"/>
+      <c r="C120" s="292"/>
       <c r="D120" s="50" t="s">
         <v>117</v>
       </c>
@@ -54031,10 +54142,10 @@
       <c r="A122" s="316" t="s">
         <v>392</v>
       </c>
-      <c r="B122" s="293" t="s">
+      <c r="B122" s="295" t="s">
         <v>12</v>
       </c>
-      <c r="C122" s="298">
+      <c r="C122" s="292">
         <f>+E122</f>
         <v>4.2299990999999997</v>
       </c>
@@ -54105,8 +54216,8 @@
     </row>
     <row r="123" spans="1:39">
       <c r="A123" s="316"/>
-      <c r="B123" s="293"/>
-      <c r="C123" s="298"/>
+      <c r="B123" s="295"/>
+      <c r="C123" s="292"/>
       <c r="D123" s="50" t="s">
         <v>117</v>
       </c>
@@ -54176,10 +54287,10 @@
       <c r="A124" s="316" t="s">
         <v>393</v>
       </c>
-      <c r="B124" s="293" t="s">
+      <c r="B124" s="295" t="s">
         <v>12</v>
       </c>
-      <c r="C124" s="298">
+      <c r="C124" s="292">
         <f>+E124</f>
         <v>5.3000118000000001</v>
       </c>
@@ -54252,8 +54363,8 @@
     </row>
     <row r="125" spans="1:39">
       <c r="A125" s="316"/>
-      <c r="B125" s="293"/>
-      <c r="C125" s="298"/>
+      <c r="B125" s="295"/>
+      <c r="C125" s="292"/>
       <c r="D125" s="50" t="s">
         <v>117</v>
       </c>
@@ -54325,10 +54436,10 @@
       <c r="A126" s="316" t="s">
         <v>394</v>
       </c>
-      <c r="B126" s="293" t="s">
+      <c r="B126" s="295" t="s">
         <v>12</v>
       </c>
-      <c r="C126" s="298">
+      <c r="C126" s="292">
         <f>+E126</f>
         <v>5.3000049000000002</v>
       </c>
@@ -54403,8 +54514,8 @@
     </row>
     <row r="127" spans="1:39">
       <c r="A127" s="316"/>
-      <c r="B127" s="293"/>
-      <c r="C127" s="298"/>
+      <c r="B127" s="295"/>
+      <c r="C127" s="292"/>
       <c r="D127" s="50" t="s">
         <v>117</v>
       </c>
@@ -54478,10 +54589,10 @@
       <c r="A128" s="316" t="s">
         <v>395</v>
       </c>
-      <c r="B128" s="293" t="s">
+      <c r="B128" s="295" t="s">
         <v>12</v>
       </c>
-      <c r="C128" s="298">
+      <c r="C128" s="292">
         <f>+E128</f>
         <v>0</v>
       </c>
@@ -54528,8 +54639,8 @@
     </row>
     <row r="129" spans="1:39">
       <c r="A129" s="316"/>
-      <c r="B129" s="293"/>
-      <c r="C129" s="298"/>
+      <c r="B129" s="295"/>
+      <c r="C129" s="292"/>
       <c r="D129" s="50" t="s">
         <v>117</v>
       </c>
@@ -54575,10 +54686,10 @@
       <c r="A130" s="316" t="s">
         <v>396</v>
       </c>
-      <c r="B130" s="293" t="s">
+      <c r="B130" s="295" t="s">
         <v>12</v>
       </c>
-      <c r="C130" s="298">
+      <c r="C130" s="292">
         <f>+E130</f>
         <v>0</v>
       </c>
@@ -54625,8 +54736,8 @@
     </row>
     <row r="131" spans="1:39">
       <c r="A131" s="316"/>
-      <c r="B131" s="293"/>
-      <c r="C131" s="298"/>
+      <c r="B131" s="295"/>
+      <c r="C131" s="292"/>
       <c r="D131" s="50" t="s">
         <v>117</v>
       </c>
@@ -54672,10 +54783,10 @@
       <c r="A132" s="316" t="s">
         <v>397</v>
       </c>
-      <c r="B132" s="293" t="s">
+      <c r="B132" s="295" t="s">
         <v>12</v>
       </c>
-      <c r="C132" s="298">
+      <c r="C132" s="292">
         <f>+E132</f>
         <v>0</v>
       </c>
@@ -54722,8 +54833,8 @@
     </row>
     <row r="133" spans="1:39">
       <c r="A133" s="316"/>
-      <c r="B133" s="293"/>
-      <c r="C133" s="298"/>
+      <c r="B133" s="295"/>
+      <c r="C133" s="292"/>
       <c r="D133" s="50" t="s">
         <v>117</v>
       </c>
@@ -54769,11 +54880,11 @@
       <c r="A134" s="317" t="s">
         <v>12</v>
       </c>
-      <c r="B134" s="297">
+      <c r="B134" s="291">
         <f>+E134</f>
         <v>0</v>
       </c>
-      <c r="C134" s="298">
+      <c r="C134" s="292">
         <v>0</v>
       </c>
       <c r="D134" s="248" t="s">
@@ -54817,8 +54928,8 @@
     </row>
     <row r="135" spans="1:39">
       <c r="A135" s="317"/>
-      <c r="B135" s="297"/>
-      <c r="C135" s="298"/>
+      <c r="B135" s="291"/>
+      <c r="C135" s="292"/>
       <c r="D135" s="50" t="s">
         <v>117</v>
       </c>
@@ -54862,11 +54973,11 @@
       <c r="A136" s="317" t="s">
         <v>12</v>
       </c>
-      <c r="B136" s="315">
+      <c r="B136" s="320">
         <f>+E136</f>
         <v>0</v>
       </c>
-      <c r="C136" s="298">
+      <c r="C136" s="292">
         <v>0</v>
       </c>
       <c r="D136" s="50" t="s">
@@ -54910,8 +55021,8 @@
     </row>
     <row r="137" spans="1:39">
       <c r="A137" s="317"/>
-      <c r="B137" s="315"/>
-      <c r="C137" s="298"/>
+      <c r="B137" s="320"/>
+      <c r="C137" s="292"/>
       <c r="D137" s="50" t="s">
         <v>117</v>
       </c>
@@ -54985,13 +55096,13 @@
       <c r="AC138" s="247"/>
     </row>
     <row r="139" spans="1:39">
-      <c r="A139" s="318" t="s">
+      <c r="A139" s="319" t="s">
         <v>12</v>
       </c>
-      <c r="B139" s="295" t="s">
+      <c r="B139" s="296" t="s">
         <v>12</v>
       </c>
-      <c r="C139" s="298">
+      <c r="C139" s="292">
         <v>0</v>
       </c>
       <c r="D139" s="50" t="s">
@@ -55034,9 +55145,9 @@
       <c r="AM139" s="228"/>
     </row>
     <row r="140" spans="1:39">
-      <c r="A140" s="318"/>
-      <c r="B140" s="295"/>
-      <c r="C140" s="298"/>
+      <c r="A140" s="319"/>
+      <c r="B140" s="296"/>
+      <c r="C140" s="292"/>
       <c r="D140" s="202" t="s">
         <v>117</v>
       </c>
@@ -55080,10 +55191,10 @@
       <c r="A141" s="316" t="s">
         <v>398</v>
       </c>
-      <c r="B141" s="295" t="s">
+      <c r="B141" s="296" t="s">
         <v>12</v>
       </c>
-      <c r="C141" s="298">
+      <c r="C141" s="292">
         <f>+E141</f>
         <v>3.8630089000000001</v>
       </c>
@@ -55110,8 +55221,8 @@
     </row>
     <row r="142" spans="1:39">
       <c r="A142" s="316"/>
-      <c r="B142" s="295"/>
-      <c r="C142" s="298"/>
+      <c r="B142" s="296"/>
+      <c r="C142" s="292"/>
       <c r="D142" s="50" t="s">
         <v>117</v>
       </c>
@@ -55137,10 +55248,10 @@
       <c r="A143" s="316" t="s">
         <v>399</v>
       </c>
-      <c r="B143" s="295" t="s">
+      <c r="B143" s="296" t="s">
         <v>12</v>
       </c>
-      <c r="C143" s="298">
+      <c r="C143" s="292">
         <f>+E143</f>
         <v>3.8630089600000002</v>
       </c>
@@ -55187,8 +55298,8 @@
     </row>
     <row r="144" spans="1:39">
       <c r="A144" s="316"/>
-      <c r="B144" s="295"/>
-      <c r="C144" s="298"/>
+      <c r="B144" s="296"/>
+      <c r="C144" s="292"/>
       <c r="D144" s="50" t="s">
         <v>117</v>
       </c>
@@ -55234,10 +55345,10 @@
       <c r="A145" s="316" t="s">
         <v>400</v>
       </c>
-      <c r="B145" s="295" t="s">
+      <c r="B145" s="296" t="s">
         <v>12</v>
       </c>
-      <c r="C145" s="298">
+      <c r="C145" s="292">
         <f>+E145</f>
         <v>7.0260103999999997</v>
       </c>
@@ -55308,8 +55419,8 @@
     </row>
     <row r="146" spans="1:39">
       <c r="A146" s="316"/>
-      <c r="B146" s="295"/>
-      <c r="C146" s="298"/>
+      <c r="B146" s="296"/>
+      <c r="C146" s="292"/>
       <c r="D146" s="50" t="s">
         <v>117</v>
       </c>
@@ -55410,10 +55521,10 @@
     </row>
     <row r="148" spans="1:39">
       <c r="A148" s="317"/>
-      <c r="B148" s="293" t="s">
+      <c r="B148" s="295" t="s">
         <v>12</v>
       </c>
-      <c r="C148" s="298">
+      <c r="C148" s="292">
         <f>+E148</f>
         <v>0</v>
       </c>
@@ -55458,8 +55569,8 @@
     </row>
     <row r="149" spans="1:39">
       <c r="A149" s="317"/>
-      <c r="B149" s="293"/>
-      <c r="C149" s="298"/>
+      <c r="B149" s="295"/>
+      <c r="C149" s="292"/>
       <c r="D149" s="50" t="s">
         <v>117</v>
       </c>
@@ -55501,10 +55612,10 @@
     </row>
     <row r="150" spans="1:39">
       <c r="A150" s="317"/>
-      <c r="B150" s="293" t="s">
+      <c r="B150" s="295" t="s">
         <v>12</v>
       </c>
-      <c r="C150" s="319">
+      <c r="C150" s="318">
         <f>+E150</f>
         <v>0</v>
       </c>
@@ -55549,8 +55660,8 @@
     </row>
     <row r="151" spans="1:39">
       <c r="A151" s="317"/>
-      <c r="B151" s="293"/>
-      <c r="C151" s="319"/>
+      <c r="B151" s="295"/>
+      <c r="C151" s="318"/>
       <c r="D151" s="50" t="s">
         <v>117</v>
       </c>
@@ -55592,6 +55703,186 @@
     </row>
   </sheetData>
   <mergeCells count="189">
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="A40:A41"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="C40:C41"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="A44:A45"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="C47:C48"/>
+    <mergeCell ref="A49:A50"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="C49:C50"/>
+    <mergeCell ref="A56:A57"/>
+    <mergeCell ref="B56:B57"/>
+    <mergeCell ref="C56:C57"/>
+    <mergeCell ref="A58:A59"/>
+    <mergeCell ref="B58:B59"/>
+    <mergeCell ref="C58:C59"/>
+    <mergeCell ref="A60:A61"/>
+    <mergeCell ref="B60:B61"/>
+    <mergeCell ref="C60:C61"/>
+    <mergeCell ref="A62:A63"/>
+    <mergeCell ref="B62:B63"/>
+    <mergeCell ref="C62:C63"/>
+    <mergeCell ref="A64:A65"/>
+    <mergeCell ref="B64:B65"/>
+    <mergeCell ref="C64:C65"/>
+    <mergeCell ref="A66:A67"/>
+    <mergeCell ref="B66:B67"/>
+    <mergeCell ref="C66:C67"/>
+    <mergeCell ref="A68:A69"/>
+    <mergeCell ref="B68:B69"/>
+    <mergeCell ref="C68:C69"/>
+    <mergeCell ref="A71:A72"/>
+    <mergeCell ref="B71:B72"/>
+    <mergeCell ref="C71:C72"/>
+    <mergeCell ref="A73:A74"/>
+    <mergeCell ref="B73:B74"/>
+    <mergeCell ref="C73:C74"/>
+    <mergeCell ref="A75:A76"/>
+    <mergeCell ref="B75:B76"/>
+    <mergeCell ref="C75:C76"/>
+    <mergeCell ref="A77:A78"/>
+    <mergeCell ref="B77:B78"/>
+    <mergeCell ref="C77:C78"/>
+    <mergeCell ref="A79:A80"/>
+    <mergeCell ref="B79:B80"/>
+    <mergeCell ref="C79:C80"/>
+    <mergeCell ref="A81:A82"/>
+    <mergeCell ref="B81:B82"/>
+    <mergeCell ref="C81:C82"/>
+    <mergeCell ref="A83:A84"/>
+    <mergeCell ref="B83:B84"/>
+    <mergeCell ref="C83:C84"/>
+    <mergeCell ref="A85:A86"/>
+    <mergeCell ref="B85:B86"/>
+    <mergeCell ref="C85:C86"/>
+    <mergeCell ref="A88:A89"/>
+    <mergeCell ref="B88:B89"/>
+    <mergeCell ref="C88:C89"/>
+    <mergeCell ref="A90:A91"/>
+    <mergeCell ref="B90:B91"/>
+    <mergeCell ref="C90:C91"/>
+    <mergeCell ref="A92:A93"/>
+    <mergeCell ref="B92:B93"/>
+    <mergeCell ref="C92:C93"/>
+    <mergeCell ref="A94:A95"/>
+    <mergeCell ref="B94:B95"/>
+    <mergeCell ref="C94:C95"/>
+    <mergeCell ref="A97:A98"/>
+    <mergeCell ref="B97:B98"/>
+    <mergeCell ref="C97:C98"/>
+    <mergeCell ref="A99:A100"/>
+    <mergeCell ref="B99:B100"/>
+    <mergeCell ref="C99:C100"/>
+    <mergeCell ref="A107:A108"/>
+    <mergeCell ref="B107:B108"/>
+    <mergeCell ref="C107:C108"/>
+    <mergeCell ref="A109:A110"/>
+    <mergeCell ref="B109:B110"/>
+    <mergeCell ref="C109:C110"/>
+    <mergeCell ref="A111:A112"/>
+    <mergeCell ref="B111:B112"/>
+    <mergeCell ref="C111:C112"/>
+    <mergeCell ref="A113:A114"/>
+    <mergeCell ref="B113:B114"/>
+    <mergeCell ref="C113:C114"/>
+    <mergeCell ref="A115:A116"/>
+    <mergeCell ref="B115:B116"/>
+    <mergeCell ref="C115:C116"/>
+    <mergeCell ref="A117:A118"/>
+    <mergeCell ref="B117:B118"/>
+    <mergeCell ref="C117:C118"/>
+    <mergeCell ref="A119:A120"/>
+    <mergeCell ref="B119:B120"/>
+    <mergeCell ref="C119:C120"/>
+    <mergeCell ref="A122:A123"/>
+    <mergeCell ref="B122:B123"/>
+    <mergeCell ref="C122:C123"/>
+    <mergeCell ref="A124:A125"/>
+    <mergeCell ref="B124:B125"/>
+    <mergeCell ref="C124:C125"/>
+    <mergeCell ref="A126:A127"/>
+    <mergeCell ref="B126:B127"/>
+    <mergeCell ref="C126:C127"/>
+    <mergeCell ref="A128:A129"/>
+    <mergeCell ref="B128:B129"/>
+    <mergeCell ref="C128:C129"/>
+    <mergeCell ref="A130:A131"/>
+    <mergeCell ref="B130:B131"/>
+    <mergeCell ref="C130:C131"/>
+    <mergeCell ref="A132:A133"/>
+    <mergeCell ref="B132:B133"/>
+    <mergeCell ref="C132:C133"/>
+    <mergeCell ref="A134:A135"/>
+    <mergeCell ref="B134:B135"/>
+    <mergeCell ref="C134:C135"/>
+    <mergeCell ref="A136:A137"/>
+    <mergeCell ref="B136:B137"/>
+    <mergeCell ref="C136:C137"/>
+    <mergeCell ref="A139:A140"/>
+    <mergeCell ref="B139:B140"/>
+    <mergeCell ref="C139:C140"/>
+    <mergeCell ref="A141:A142"/>
+    <mergeCell ref="B141:B142"/>
+    <mergeCell ref="C141:C142"/>
+    <mergeCell ref="A143:A144"/>
+    <mergeCell ref="B143:B144"/>
+    <mergeCell ref="C143:C144"/>
     <mergeCell ref="A145:A146"/>
     <mergeCell ref="B145:B146"/>
     <mergeCell ref="C145:C146"/>
@@ -55601,186 +55892,6 @@
     <mergeCell ref="A150:A151"/>
     <mergeCell ref="B150:B151"/>
     <mergeCell ref="C150:C151"/>
-    <mergeCell ref="A139:A140"/>
-    <mergeCell ref="B139:B140"/>
-    <mergeCell ref="C139:C140"/>
-    <mergeCell ref="A141:A142"/>
-    <mergeCell ref="B141:B142"/>
-    <mergeCell ref="C141:C142"/>
-    <mergeCell ref="A143:A144"/>
-    <mergeCell ref="B143:B144"/>
-    <mergeCell ref="C143:C144"/>
-    <mergeCell ref="A132:A133"/>
-    <mergeCell ref="B132:B133"/>
-    <mergeCell ref="C132:C133"/>
-    <mergeCell ref="A134:A135"/>
-    <mergeCell ref="B134:B135"/>
-    <mergeCell ref="C134:C135"/>
-    <mergeCell ref="A136:A137"/>
-    <mergeCell ref="B136:B137"/>
-    <mergeCell ref="C136:C137"/>
-    <mergeCell ref="A126:A127"/>
-    <mergeCell ref="B126:B127"/>
-    <mergeCell ref="C126:C127"/>
-    <mergeCell ref="A128:A129"/>
-    <mergeCell ref="B128:B129"/>
-    <mergeCell ref="C128:C129"/>
-    <mergeCell ref="A130:A131"/>
-    <mergeCell ref="B130:B131"/>
-    <mergeCell ref="C130:C131"/>
-    <mergeCell ref="A119:A120"/>
-    <mergeCell ref="B119:B120"/>
-    <mergeCell ref="C119:C120"/>
-    <mergeCell ref="A122:A123"/>
-    <mergeCell ref="B122:B123"/>
-    <mergeCell ref="C122:C123"/>
-    <mergeCell ref="A124:A125"/>
-    <mergeCell ref="B124:B125"/>
-    <mergeCell ref="C124:C125"/>
-    <mergeCell ref="A113:A114"/>
-    <mergeCell ref="B113:B114"/>
-    <mergeCell ref="C113:C114"/>
-    <mergeCell ref="A115:A116"/>
-    <mergeCell ref="B115:B116"/>
-    <mergeCell ref="C115:C116"/>
-    <mergeCell ref="A117:A118"/>
-    <mergeCell ref="B117:B118"/>
-    <mergeCell ref="C117:C118"/>
-    <mergeCell ref="A107:A108"/>
-    <mergeCell ref="B107:B108"/>
-    <mergeCell ref="C107:C108"/>
-    <mergeCell ref="A109:A110"/>
-    <mergeCell ref="B109:B110"/>
-    <mergeCell ref="C109:C110"/>
-    <mergeCell ref="A111:A112"/>
-    <mergeCell ref="B111:B112"/>
-    <mergeCell ref="C111:C112"/>
-    <mergeCell ref="A94:A95"/>
-    <mergeCell ref="B94:B95"/>
-    <mergeCell ref="C94:C95"/>
-    <mergeCell ref="A97:A98"/>
-    <mergeCell ref="B97:B98"/>
-    <mergeCell ref="C97:C98"/>
-    <mergeCell ref="A99:A100"/>
-    <mergeCell ref="B99:B100"/>
-    <mergeCell ref="C99:C100"/>
-    <mergeCell ref="A88:A89"/>
-    <mergeCell ref="B88:B89"/>
-    <mergeCell ref="C88:C89"/>
-    <mergeCell ref="A90:A91"/>
-    <mergeCell ref="B90:B91"/>
-    <mergeCell ref="C90:C91"/>
-    <mergeCell ref="A92:A93"/>
-    <mergeCell ref="B92:B93"/>
-    <mergeCell ref="C92:C93"/>
-    <mergeCell ref="A81:A82"/>
-    <mergeCell ref="B81:B82"/>
-    <mergeCell ref="C81:C82"/>
-    <mergeCell ref="A83:A84"/>
-    <mergeCell ref="B83:B84"/>
-    <mergeCell ref="C83:C84"/>
-    <mergeCell ref="A85:A86"/>
-    <mergeCell ref="B85:B86"/>
-    <mergeCell ref="C85:C86"/>
-    <mergeCell ref="A75:A76"/>
-    <mergeCell ref="B75:B76"/>
-    <mergeCell ref="C75:C76"/>
-    <mergeCell ref="A77:A78"/>
-    <mergeCell ref="B77:B78"/>
-    <mergeCell ref="C77:C78"/>
-    <mergeCell ref="A79:A80"/>
-    <mergeCell ref="B79:B80"/>
-    <mergeCell ref="C79:C80"/>
-    <mergeCell ref="A68:A69"/>
-    <mergeCell ref="B68:B69"/>
-    <mergeCell ref="C68:C69"/>
-    <mergeCell ref="A71:A72"/>
-    <mergeCell ref="B71:B72"/>
-    <mergeCell ref="C71:C72"/>
-    <mergeCell ref="A73:A74"/>
-    <mergeCell ref="B73:B74"/>
-    <mergeCell ref="C73:C74"/>
-    <mergeCell ref="A62:A63"/>
-    <mergeCell ref="B62:B63"/>
-    <mergeCell ref="C62:C63"/>
-    <mergeCell ref="A64:A65"/>
-    <mergeCell ref="B64:B65"/>
-    <mergeCell ref="C64:C65"/>
-    <mergeCell ref="A66:A67"/>
-    <mergeCell ref="B66:B67"/>
-    <mergeCell ref="C66:C67"/>
-    <mergeCell ref="A56:A57"/>
-    <mergeCell ref="B56:B57"/>
-    <mergeCell ref="C56:C57"/>
-    <mergeCell ref="A58:A59"/>
-    <mergeCell ref="B58:B59"/>
-    <mergeCell ref="C58:C59"/>
-    <mergeCell ref="A60:A61"/>
-    <mergeCell ref="B60:B61"/>
-    <mergeCell ref="C60:C61"/>
-    <mergeCell ref="A44:A45"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="A47:A48"/>
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="C47:C48"/>
-    <mergeCell ref="A49:A50"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="C49:C50"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="C38:C39"/>
-    <mergeCell ref="A40:A41"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="C40:C41"/>
-    <mergeCell ref="A42:A43"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="C42:C43"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="A35:A36"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Updates in the CAT model
</commit_message>
<xml_diff>
--- a/models/14sectors_cat/energy.xlsx
+++ b/models/14sectors_cat/energy.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\OneDrive\01.Feina_CREAF\07.Vensim_models\pymedeas2_vensim\models_for_pymedeas2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4908EF5C-46E9-4639-BC97-D747EF94C618}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FE9EE85-6A32-43DE-9224-D0E051A8472A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="11028" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1884" yWindow="1884" windowWidth="17280" windowHeight="8196" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Global" sheetId="1" r:id="rId1"/>
@@ -11190,17 +11190,50 @@
     <xf numFmtId="0" fontId="0" fillId="25" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -11211,40 +11244,22 @@
     <xf numFmtId="0" fontId="3" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="22" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -11259,25 +11274,16 @@
     <xf numFmtId="0" fontId="1" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="25" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="59" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -11286,17 +11292,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -11637,20 +11637,20 @@
       <c r="G2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="287" t="s">
+      <c r="H2" s="288" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="287"/>
-      <c r="J2" s="287"/>
-      <c r="K2" s="287"/>
-      <c r="L2" s="287"/>
-      <c r="M2" s="287"/>
-      <c r="N2" s="287"/>
-      <c r="O2" s="287"/>
-      <c r="P2" s="287"/>
-      <c r="Q2" s="287"/>
-      <c r="R2" s="287"/>
-      <c r="S2" s="287"/>
+      <c r="I2" s="288"/>
+      <c r="J2" s="288"/>
+      <c r="K2" s="288"/>
+      <c r="L2" s="288"/>
+      <c r="M2" s="288"/>
+      <c r="N2" s="288"/>
+      <c r="O2" s="288"/>
+      <c r="P2" s="288"/>
+      <c r="Q2" s="288"/>
+      <c r="R2" s="288"/>
+      <c r="S2" s="288"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" s="5"/>
@@ -12718,11 +12718,11 @@
       <c r="A44" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="E44" s="288" t="s">
+      <c r="E44" s="289" t="s">
         <v>55</v>
       </c>
-      <c r="F44" s="288"/>
-      <c r="G44" s="288"/>
+      <c r="F44" s="289"/>
+      <c r="G44" s="289"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="10" t="s">
@@ -13191,21 +13191,21 @@
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A22" s="301"/>
-      <c r="B22" s="301"/>
-      <c r="C22" s="301"/>
+      <c r="A22" s="290"/>
+      <c r="B22" s="290"/>
+      <c r="C22" s="290"/>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A23" s="304"/>
-      <c r="B23" s="304"/>
-      <c r="C23" s="304"/>
+      <c r="A23" s="291"/>
+      <c r="B23" s="291"/>
+      <c r="C23" s="291"/>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A24" s="305" t="s">
+      <c r="A24" s="292" t="s">
         <v>30</v>
       </c>
-      <c r="B24" s="305"/>
-      <c r="C24" s="305"/>
+      <c r="B24" s="292"/>
+      <c r="C24" s="292"/>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25" s="10" t="s">
@@ -13239,11 +13239,11 @@
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A27" s="302" t="s">
+      <c r="A27" s="293" t="s">
         <v>77</v>
       </c>
-      <c r="B27" s="302"/>
-      <c r="C27" s="302"/>
+      <c r="B27" s="293"/>
+      <c r="C27" s="293"/>
       <c r="E27" s="10" t="s">
         <v>78</v>
       </c>
@@ -13264,14 +13264,14 @@
       <c r="C28" s="16">
         <v>39.625999999999998</v>
       </c>
-      <c r="E28" s="302" t="s">
+      <c r="E28" s="293" t="s">
         <v>32</v>
       </c>
-      <c r="F28" s="302"/>
-      <c r="G28" s="302"/>
-      <c r="H28" s="301"/>
-      <c r="I28" s="301"/>
-      <c r="J28" s="301"/>
+      <c r="F28" s="293"/>
+      <c r="G28" s="293"/>
+      <c r="H28" s="290"/>
+      <c r="I28" s="290"/>
+      <c r="J28" s="290"/>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A29" s="10" t="s">
@@ -13294,16 +13294,16 @@
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A30" s="302" t="s">
+      <c r="A30" s="293" t="s">
         <v>84</v>
       </c>
-      <c r="B30" s="302"/>
-      <c r="C30" s="302"/>
-      <c r="E30" s="302" t="s">
+      <c r="B30" s="293"/>
+      <c r="C30" s="293"/>
+      <c r="E30" s="293" t="s">
         <v>85</v>
       </c>
-      <c r="F30" s="302"/>
-      <c r="G30" s="302"/>
+      <c r="F30" s="293"/>
+      <c r="G30" s="293"/>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A31" s="10" t="s">
@@ -13335,11 +13335,11 @@
       <c r="C32">
         <v>0.442362737444705</v>
       </c>
-      <c r="E32" s="302" t="s">
+      <c r="E32" s="293" t="s">
         <v>89</v>
       </c>
-      <c r="F32" s="302"/>
-      <c r="G32" s="302"/>
+      <c r="F32" s="293"/>
+      <c r="G32" s="293"/>
     </row>
     <row r="33" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A33" s="10" t="s">
@@ -13373,16 +13373,16 @@
       </c>
     </row>
     <row r="36" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A36" s="302" t="s">
+      <c r="A36" s="293" t="s">
         <v>93</v>
       </c>
-      <c r="B36" s="302"/>
-      <c r="C36" s="302"/>
-      <c r="E36" s="303" t="s">
+      <c r="B36" s="293"/>
+      <c r="C36" s="293"/>
+      <c r="E36" s="294" t="s">
         <v>94</v>
       </c>
-      <c r="F36" s="303"/>
-      <c r="G36" s="303"/>
+      <c r="F36" s="294"/>
+      <c r="G36" s="294"/>
     </row>
     <row r="37" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A37" s="10" t="s">
@@ -13663,13 +13663,13 @@
       <c r="AH49" s="51"/>
     </row>
     <row r="50" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A50" s="298" t="s">
+      <c r="A50" s="295" t="s">
         <v>115</v>
       </c>
-      <c r="B50" s="294" t="s">
+      <c r="B50" s="296" t="s">
         <v>12</v>
       </c>
-      <c r="C50" s="299">
+      <c r="C50" s="297">
         <v>14500</v>
       </c>
       <c r="D50" s="52" t="s">
@@ -13767,9 +13767,9 @@
       </c>
     </row>
     <row r="51" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A51" s="298"/>
-      <c r="B51" s="298"/>
-      <c r="C51" s="299"/>
+      <c r="A51" s="295"/>
+      <c r="B51" s="295"/>
+      <c r="C51" s="297"/>
       <c r="D51" s="52" t="s">
         <v>117</v>
       </c>
@@ -13865,13 +13865,13 @@
       </c>
     </row>
     <row r="52" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A52" s="295" t="s">
+      <c r="A52" s="298" t="s">
         <v>118</v>
       </c>
-      <c r="B52" s="294" t="s">
+      <c r="B52" s="296" t="s">
         <v>12</v>
       </c>
-      <c r="C52" s="300">
+      <c r="C52" s="299">
         <v>10500</v>
       </c>
       <c r="D52" s="52" t="s">
@@ -13953,9 +13953,9 @@
       <c r="AH52" s="59"/>
     </row>
     <row r="53" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A53" s="295"/>
-      <c r="B53" s="294"/>
-      <c r="C53" s="300"/>
+      <c r="A53" s="298"/>
+      <c r="B53" s="296"/>
+      <c r="C53" s="299"/>
       <c r="D53" s="52" t="s">
         <v>117</v>
       </c>
@@ -14035,13 +14035,13 @@
       <c r="AH53" s="62"/>
     </row>
     <row r="54" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A54" s="294" t="s">
+      <c r="A54" s="296" t="s">
         <v>119</v>
       </c>
-      <c r="B54" s="297">
+      <c r="B54" s="300">
         <v>0.5</v>
       </c>
-      <c r="C54" s="296">
+      <c r="C54" s="301">
         <v>16800</v>
       </c>
       <c r="D54" s="52" t="s">
@@ -14137,9 +14137,9 @@
       <c r="AH54" s="59"/>
     </row>
     <row r="55" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A55" s="294"/>
-      <c r="B55" s="297"/>
-      <c r="C55" s="297"/>
+      <c r="A55" s="296"/>
+      <c r="B55" s="300"/>
+      <c r="C55" s="300"/>
       <c r="D55" s="52" t="s">
         <v>117</v>
       </c>
@@ -14271,13 +14271,13 @@
       <c r="AH56" s="51"/>
     </row>
     <row r="57" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A57" s="294" t="s">
+      <c r="A57" s="296" t="s">
         <v>121</v>
       </c>
-      <c r="B57" s="294" t="s">
+      <c r="B57" s="296" t="s">
         <v>12</v>
       </c>
-      <c r="C57" s="296">
+      <c r="C57" s="301">
         <v>13200</v>
       </c>
       <c r="D57" s="52" t="s">
@@ -14339,9 +14339,9 @@
       <c r="AH57" s="59"/>
     </row>
     <row r="58" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A58" s="294"/>
-      <c r="B58" s="294"/>
-      <c r="C58" s="296"/>
+      <c r="A58" s="296"/>
+      <c r="B58" s="296"/>
+      <c r="C58" s="301"/>
       <c r="D58" s="52" t="s">
         <v>117</v>
       </c>
@@ -14401,13 +14401,13 @@
       <c r="AH58" s="63"/>
     </row>
     <row r="59" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A59" s="295" t="s">
+      <c r="A59" s="298" t="s">
         <v>122</v>
       </c>
-      <c r="B59" s="294" t="s">
+      <c r="B59" s="296" t="s">
         <v>12</v>
       </c>
-      <c r="C59" s="296">
+      <c r="C59" s="301">
         <v>14500</v>
       </c>
       <c r="D59" s="52" t="s">
@@ -14505,9 +14505,9 @@
       </c>
     </row>
     <row r="60" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A60" s="295"/>
-      <c r="B60" s="294"/>
-      <c r="C60" s="296"/>
+      <c r="A60" s="298"/>
+      <c r="B60" s="296"/>
+      <c r="C60" s="301"/>
       <c r="D60" s="52" t="s">
         <v>117</v>
       </c>
@@ -14603,13 +14603,13 @@
       </c>
     </row>
     <row r="61" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A61" s="294" t="s">
+      <c r="A61" s="296" t="s">
         <v>123</v>
       </c>
-      <c r="B61" s="297">
+      <c r="B61" s="300">
         <v>0.25</v>
       </c>
-      <c r="C61" s="296">
+      <c r="C61" s="301">
         <v>13000</v>
       </c>
       <c r="D61" s="52" t="s">
@@ -14701,9 +14701,9 @@
       <c r="AH61" s="59"/>
     </row>
     <row r="62" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A62" s="294"/>
-      <c r="B62" s="297"/>
-      <c r="C62" s="297"/>
+      <c r="A62" s="296"/>
+      <c r="B62" s="300"/>
+      <c r="C62" s="300"/>
       <c r="D62" s="52" t="s">
         <v>117</v>
       </c>
@@ -14831,13 +14831,13 @@
       <c r="AH63" s="51"/>
     </row>
     <row r="64" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A64" s="294" t="s">
+      <c r="A64" s="296" t="s">
         <v>125</v>
       </c>
-      <c r="B64" s="295" t="s">
+      <c r="B64" s="298" t="s">
         <v>12</v>
       </c>
-      <c r="C64" s="296">
+      <c r="C64" s="301">
         <v>22500</v>
       </c>
       <c r="D64" s="52" t="s">
@@ -14907,9 +14907,9 @@
       <c r="AH64" s="59"/>
     </row>
     <row r="65" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A65" s="294"/>
-      <c r="B65" s="295"/>
-      <c r="C65" s="296"/>
+      <c r="A65" s="296"/>
+      <c r="B65" s="298"/>
+      <c r="C65" s="301"/>
       <c r="D65" s="52" t="s">
         <v>117</v>
       </c>
@@ -15015,13 +15015,13 @@
       <c r="AH66" s="51"/>
     </row>
     <row r="67" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A67" s="294" t="s">
+      <c r="A67" s="296" t="s">
         <v>127</v>
       </c>
-      <c r="B67" s="294" t="s">
+      <c r="B67" s="296" t="s">
         <v>12</v>
       </c>
-      <c r="C67" s="296">
+      <c r="C67" s="301">
         <v>3700</v>
       </c>
       <c r="D67" s="52" t="s">
@@ -15087,9 +15087,9 @@
       <c r="AH67" s="59"/>
     </row>
     <row r="68" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A68" s="294"/>
-      <c r="B68" s="294"/>
-      <c r="C68" s="296"/>
+      <c r="A68" s="296"/>
+      <c r="B68" s="296"/>
+      <c r="C68" s="301"/>
       <c r="D68" s="52" t="s">
         <v>117</v>
       </c>
@@ -15153,16 +15153,16 @@
       <c r="AH68" s="63"/>
     </row>
     <row r="71" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A71" s="291" t="s">
+      <c r="A71" s="302" t="s">
         <v>128</v>
       </c>
-      <c r="B71" s="291"/>
-      <c r="C71" s="291"/>
-      <c r="E71" s="292" t="s">
+      <c r="B71" s="302"/>
+      <c r="C71" s="302"/>
+      <c r="E71" s="303" t="s">
         <v>129</v>
       </c>
-      <c r="F71" s="292"/>
-      <c r="G71" s="292"/>
+      <c r="F71" s="303"/>
+      <c r="G71" s="303"/>
     </row>
     <row r="72" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A72" s="52" t="s">
@@ -15417,10 +15417,10 @@
       </c>
     </row>
     <row r="92" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A92" s="291" t="s">
+      <c r="A92" s="302" t="s">
         <v>30</v>
       </c>
-      <c r="B92" s="291"/>
+      <c r="B92" s="302"/>
       <c r="C92" s="15">
         <v>1995</v>
       </c>
@@ -20802,11 +20802,11 @@
       </c>
     </row>
     <row r="199" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A199" s="293" t="s">
+      <c r="A199" s="304" t="s">
         <v>266</v>
       </c>
-      <c r="B199" s="293"/>
-      <c r="C199" s="293"/>
+      <c r="B199" s="304"/>
+      <c r="C199" s="304"/>
     </row>
     <row r="200" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A200" s="106" t="s">
@@ -20885,7 +20885,7 @@
       <c r="A205" s="119" t="s">
         <v>271</v>
       </c>
-      <c r="B205" s="289" t="s">
+      <c r="B205" s="305" t="s">
         <v>272</v>
       </c>
       <c r="C205" s="120">
@@ -20938,7 +20938,7 @@
       <c r="A206" s="123" t="s">
         <v>273</v>
       </c>
-      <c r="B206" s="289"/>
+      <c r="B206" s="305"/>
       <c r="C206" s="124">
         <v>0.5</v>
       </c>
@@ -20989,7 +20989,7 @@
       <c r="A207" s="123" t="s">
         <v>274</v>
       </c>
-      <c r="B207" s="289"/>
+      <c r="B207" s="305"/>
       <c r="C207" s="124">
         <v>0.5</v>
       </c>
@@ -21040,7 +21040,7 @@
       <c r="A208" s="123" t="s">
         <v>275</v>
       </c>
-      <c r="B208" s="289"/>
+      <c r="B208" s="305"/>
       <c r="C208" s="124">
         <v>0.5</v>
       </c>
@@ -21091,7 +21091,7 @@
       <c r="A209" s="125" t="s">
         <v>276</v>
       </c>
-      <c r="B209" s="289"/>
+      <c r="B209" s="305"/>
       <c r="C209" s="124">
         <v>0.5</v>
       </c>
@@ -21142,7 +21142,7 @@
       <c r="A210" s="126" t="s">
         <v>271</v>
       </c>
-      <c r="B210" s="289" t="s">
+      <c r="B210" s="305" t="s">
         <v>277</v>
       </c>
       <c r="C210" s="124">
@@ -21195,7 +21195,7 @@
       <c r="A211" s="127" t="s">
         <v>273</v>
       </c>
-      <c r="B211" s="289"/>
+      <c r="B211" s="305"/>
       <c r="C211" s="120">
         <v>0.5</v>
       </c>
@@ -21246,7 +21246,7 @@
       <c r="A212" s="127" t="s">
         <v>274</v>
       </c>
-      <c r="B212" s="289"/>
+      <c r="B212" s="305"/>
       <c r="C212" s="124">
         <v>0.5</v>
       </c>
@@ -21297,7 +21297,7 @@
       <c r="A213" s="127" t="s">
         <v>275</v>
       </c>
-      <c r="B213" s="289"/>
+      <c r="B213" s="305"/>
       <c r="C213" s="124">
         <v>0.5</v>
       </c>
@@ -21348,7 +21348,7 @@
       <c r="A214" s="128" t="s">
         <v>276</v>
       </c>
-      <c r="B214" s="289"/>
+      <c r="B214" s="305"/>
       <c r="C214" s="124">
         <v>0.5</v>
       </c>
@@ -21399,7 +21399,7 @@
       <c r="A215" s="129" t="s">
         <v>278</v>
       </c>
-      <c r="B215" s="289" t="s">
+      <c r="B215" s="305" t="s">
         <v>279</v>
       </c>
       <c r="C215" s="124">
@@ -21452,7 +21452,7 @@
       <c r="A216" s="127" t="s">
         <v>273</v>
       </c>
-      <c r="B216" s="289"/>
+      <c r="B216" s="305"/>
       <c r="C216" s="124">
         <v>0.5</v>
       </c>
@@ -21503,7 +21503,7 @@
       <c r="A217" s="127" t="s">
         <v>274</v>
       </c>
-      <c r="B217" s="289"/>
+      <c r="B217" s="305"/>
       <c r="C217" s="120">
         <v>0.5</v>
       </c>
@@ -21554,7 +21554,7 @@
       <c r="A218" s="127" t="s">
         <v>275</v>
       </c>
-      <c r="B218" s="289"/>
+      <c r="B218" s="305"/>
       <c r="C218" s="124">
         <v>0.5</v>
       </c>
@@ -21605,7 +21605,7 @@
       <c r="A219" s="128" t="s">
         <v>276</v>
       </c>
-      <c r="B219" s="289"/>
+      <c r="B219" s="305"/>
       <c r="C219" s="124">
         <v>0.5</v>
       </c>
@@ -21656,7 +21656,7 @@
       <c r="A220" s="129" t="s">
         <v>271</v>
       </c>
-      <c r="B220" s="289" t="s">
+      <c r="B220" s="305" t="s">
         <v>280</v>
       </c>
       <c r="C220" s="124">
@@ -21709,7 +21709,7 @@
       <c r="A221" s="127" t="s">
         <v>273</v>
       </c>
-      <c r="B221" s="289"/>
+      <c r="B221" s="305"/>
       <c r="C221" s="124">
         <v>0.5</v>
       </c>
@@ -21760,7 +21760,7 @@
       <c r="A222" s="127" t="s">
         <v>274</v>
       </c>
-      <c r="B222" s="289"/>
+      <c r="B222" s="305"/>
       <c r="C222" s="124">
         <v>0.5</v>
       </c>
@@ -21811,7 +21811,7 @@
       <c r="A223" s="127" t="s">
         <v>275</v>
       </c>
-      <c r="B223" s="289"/>
+      <c r="B223" s="305"/>
       <c r="C223" s="120">
         <v>0.5</v>
       </c>
@@ -21862,7 +21862,7 @@
       <c r="A224" s="128" t="s">
         <v>276</v>
       </c>
-      <c r="B224" s="289"/>
+      <c r="B224" s="305"/>
       <c r="C224" s="124">
         <v>0.5</v>
       </c>
@@ -21913,7 +21913,7 @@
       <c r="A225" s="129" t="s">
         <v>271</v>
       </c>
-      <c r="B225" s="289" t="s">
+      <c r="B225" s="305" t="s">
         <v>281</v>
       </c>
       <c r="C225" s="124">
@@ -21966,7 +21966,7 @@
       <c r="A226" s="127" t="s">
         <v>273</v>
       </c>
-      <c r="B226" s="289"/>
+      <c r="B226" s="305"/>
       <c r="C226" s="124">
         <v>0.5</v>
       </c>
@@ -22017,7 +22017,7 @@
       <c r="A227" s="127" t="s">
         <v>274</v>
       </c>
-      <c r="B227" s="289"/>
+      <c r="B227" s="305"/>
       <c r="C227" s="124">
         <v>0.5</v>
       </c>
@@ -22068,7 +22068,7 @@
       <c r="A228" s="127" t="s">
         <v>275</v>
       </c>
-      <c r="B228" s="289"/>
+      <c r="B228" s="305"/>
       <c r="C228" s="124">
         <v>0.5</v>
       </c>
@@ -22119,7 +22119,7 @@
       <c r="A229" s="128" t="s">
         <v>276</v>
       </c>
-      <c r="B229" s="289"/>
+      <c r="B229" s="305"/>
       <c r="C229" s="130">
         <v>0.5</v>
       </c>
@@ -22167,11 +22167,11 @@
       </c>
     </row>
     <row r="232" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A232" s="290" t="s">
+      <c r="A232" s="306" t="s">
         <v>282</v>
       </c>
-      <c r="B232" s="290"/>
-      <c r="C232" s="290"/>
+      <c r="B232" s="306"/>
+      <c r="C232" s="306"/>
     </row>
     <row r="233" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
@@ -22210,51 +22210,51 @@
     </row>
   </sheetData>
   <mergeCells count="45">
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="A27:C27"/>
-    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="B210:B214"/>
+    <mergeCell ref="B215:B219"/>
+    <mergeCell ref="B220:B224"/>
+    <mergeCell ref="B225:B229"/>
+    <mergeCell ref="A232:C232"/>
+    <mergeCell ref="A71:C71"/>
+    <mergeCell ref="E71:G71"/>
+    <mergeCell ref="A92:B92"/>
+    <mergeCell ref="A199:C199"/>
+    <mergeCell ref="B205:B209"/>
+    <mergeCell ref="A64:A65"/>
+    <mergeCell ref="B64:B65"/>
+    <mergeCell ref="C64:C65"/>
+    <mergeCell ref="A67:A68"/>
+    <mergeCell ref="B67:B68"/>
+    <mergeCell ref="C67:C68"/>
+    <mergeCell ref="A59:A60"/>
+    <mergeCell ref="B59:B60"/>
+    <mergeCell ref="C59:C60"/>
+    <mergeCell ref="A61:A62"/>
+    <mergeCell ref="B61:B62"/>
+    <mergeCell ref="C61:C62"/>
+    <mergeCell ref="A54:A55"/>
+    <mergeCell ref="B54:B55"/>
+    <mergeCell ref="C54:C55"/>
+    <mergeCell ref="A57:A58"/>
+    <mergeCell ref="B57:B58"/>
+    <mergeCell ref="C57:C58"/>
+    <mergeCell ref="A50:A51"/>
+    <mergeCell ref="B50:B51"/>
+    <mergeCell ref="C50:C51"/>
+    <mergeCell ref="A52:A53"/>
+    <mergeCell ref="B52:B53"/>
+    <mergeCell ref="C52:C53"/>
     <mergeCell ref="H28:J28"/>
     <mergeCell ref="A30:C30"/>
     <mergeCell ref="E30:G30"/>
     <mergeCell ref="E32:G32"/>
     <mergeCell ref="A36:C36"/>
     <mergeCell ref="E36:G36"/>
-    <mergeCell ref="A50:A51"/>
-    <mergeCell ref="B50:B51"/>
-    <mergeCell ref="C50:C51"/>
-    <mergeCell ref="A52:A53"/>
-    <mergeCell ref="B52:B53"/>
-    <mergeCell ref="C52:C53"/>
-    <mergeCell ref="A54:A55"/>
-    <mergeCell ref="B54:B55"/>
-    <mergeCell ref="C54:C55"/>
-    <mergeCell ref="A57:A58"/>
-    <mergeCell ref="B57:B58"/>
-    <mergeCell ref="C57:C58"/>
-    <mergeCell ref="A59:A60"/>
-    <mergeCell ref="B59:B60"/>
-    <mergeCell ref="C59:C60"/>
-    <mergeCell ref="A61:A62"/>
-    <mergeCell ref="B61:B62"/>
-    <mergeCell ref="C61:C62"/>
-    <mergeCell ref="A64:A65"/>
-    <mergeCell ref="B64:B65"/>
-    <mergeCell ref="C64:C65"/>
-    <mergeCell ref="A67:A68"/>
-    <mergeCell ref="B67:B68"/>
-    <mergeCell ref="C67:C68"/>
-    <mergeCell ref="A71:C71"/>
-    <mergeCell ref="E71:G71"/>
-    <mergeCell ref="A92:B92"/>
-    <mergeCell ref="A199:C199"/>
-    <mergeCell ref="B205:B209"/>
-    <mergeCell ref="B210:B214"/>
-    <mergeCell ref="B215:B219"/>
-    <mergeCell ref="B220:B224"/>
-    <mergeCell ref="B225:B229"/>
-    <mergeCell ref="A232:C232"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="E28:G28"/>
   </mergeCells>
   <conditionalFormatting sqref="B165:P165">
     <cfRule type="cellIs" dxfId="2" priority="2" operator="lessThan">
@@ -22631,21 +22631,21 @@
       <c r="L21" s="136"/>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A22" s="301"/>
-      <c r="B22" s="301"/>
-      <c r="C22" s="301"/>
+      <c r="A22" s="290"/>
+      <c r="B22" s="290"/>
+      <c r="C22" s="290"/>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A23" s="304"/>
-      <c r="B23" s="304"/>
-      <c r="C23" s="304"/>
+      <c r="A23" s="291"/>
+      <c r="B23" s="291"/>
+      <c r="C23" s="291"/>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A24" s="305" t="s">
+      <c r="A24" s="292" t="s">
         <v>30</v>
       </c>
-      <c r="B24" s="305"/>
-      <c r="C24" s="305"/>
+      <c r="B24" s="292"/>
+      <c r="C24" s="292"/>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25" s="10" t="s">
@@ -22679,11 +22679,11 @@
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A27" s="302" t="s">
+      <c r="A27" s="293" t="s">
         <v>77</v>
       </c>
-      <c r="B27" s="302"/>
-      <c r="C27" s="302"/>
+      <c r="B27" s="293"/>
+      <c r="C27" s="293"/>
       <c r="E27" s="10" t="s">
         <v>78</v>
       </c>
@@ -22704,14 +22704,14 @@
       <c r="C28" s="16">
         <v>0</v>
       </c>
-      <c r="E28" s="302" t="s">
+      <c r="E28" s="293" t="s">
         <v>32</v>
       </c>
-      <c r="F28" s="302"/>
-      <c r="G28" s="302"/>
-      <c r="H28" s="301"/>
-      <c r="I28" s="301"/>
-      <c r="J28" s="301"/>
+      <c r="F28" s="293"/>
+      <c r="G28" s="293"/>
+      <c r="H28" s="290"/>
+      <c r="I28" s="290"/>
+      <c r="J28" s="290"/>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A29" s="10"/>
@@ -22728,16 +22728,16 @@
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A30" s="302" t="s">
+      <c r="A30" s="293" t="s">
         <v>84</v>
       </c>
-      <c r="B30" s="302"/>
-      <c r="C30" s="302"/>
-      <c r="E30" s="302" t="s">
+      <c r="B30" s="293"/>
+      <c r="C30" s="293"/>
+      <c r="E30" s="293" t="s">
         <v>85</v>
       </c>
-      <c r="F30" s="302"/>
-      <c r="G30" s="302"/>
+      <c r="F30" s="293"/>
+      <c r="G30" s="293"/>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A31" s="10" t="s">
@@ -22770,11 +22770,11 @@
       <c r="C32" s="39">
         <v>0.76834862385321101</v>
       </c>
-      <c r="E32" s="302" t="s">
+      <c r="E32" s="293" t="s">
         <v>89</v>
       </c>
-      <c r="F32" s="302"/>
-      <c r="G32" s="302"/>
+      <c r="F32" s="293"/>
+      <c r="G32" s="293"/>
     </row>
     <row r="33" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A33" s="10" t="s">
@@ -22808,16 +22808,16 @@
       </c>
     </row>
     <row r="36" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A36" s="302" t="s">
+      <c r="A36" s="293" t="s">
         <v>93</v>
       </c>
-      <c r="B36" s="302"/>
-      <c r="C36" s="302"/>
-      <c r="E36" s="303" t="s">
+      <c r="B36" s="293"/>
+      <c r="C36" s="293"/>
+      <c r="E36" s="294" t="s">
         <v>94</v>
       </c>
-      <c r="F36" s="303"/>
-      <c r="G36" s="303"/>
+      <c r="F36" s="294"/>
+      <c r="G36" s="294"/>
     </row>
     <row r="37" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A37" s="10" t="s">
@@ -23098,13 +23098,13 @@
       <c r="AH49" s="51"/>
     </row>
     <row r="50" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A50" s="298" t="s">
+      <c r="A50" s="295" t="s">
         <v>115</v>
       </c>
-      <c r="B50" s="294" t="s">
+      <c r="B50" s="296" t="s">
         <v>12</v>
       </c>
-      <c r="C50" s="311">
+      <c r="C50" s="307">
         <v>411.48014529125697</v>
       </c>
       <c r="D50" s="52" t="s">
@@ -23178,9 +23178,9 @@
       <c r="AH50" s="54"/>
     </row>
     <row r="51" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A51" s="298"/>
-      <c r="B51" s="298"/>
-      <c r="C51" s="311"/>
+      <c r="A51" s="295"/>
+      <c r="B51" s="295"/>
+      <c r="C51" s="307"/>
       <c r="D51" s="52" t="s">
         <v>117</v>
       </c>
@@ -23252,13 +23252,13 @@
       <c r="AH51" s="57"/>
     </row>
     <row r="52" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A52" s="295" t="s">
+      <c r="A52" s="298" t="s">
         <v>118</v>
       </c>
-      <c r="B52" s="294" t="s">
+      <c r="B52" s="296" t="s">
         <v>12</v>
       </c>
-      <c r="C52" s="311">
+      <c r="C52" s="307">
         <v>77.5139928551</v>
       </c>
       <c r="D52" s="139" t="s">
@@ -23330,9 +23330,9 @@
       <c r="AH52" s="59"/>
     </row>
     <row r="53" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A53" s="295"/>
-      <c r="B53" s="294"/>
-      <c r="C53" s="311"/>
+      <c r="A53" s="298"/>
+      <c r="B53" s="296"/>
+      <c r="C53" s="307"/>
       <c r="D53" s="139" t="s">
         <v>117</v>
       </c>
@@ -23402,13 +23402,13 @@
       <c r="AH53" s="62"/>
     </row>
     <row r="54" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A54" s="294" t="s">
+      <c r="A54" s="296" t="s">
         <v>119</v>
       </c>
-      <c r="B54" s="313">
+      <c r="B54" s="308">
         <v>0.5</v>
       </c>
-      <c r="C54" s="312">
+      <c r="C54" s="309">
         <v>14500</v>
       </c>
       <c r="D54" s="139" t="s">
@@ -23506,9 +23506,9 @@
       </c>
     </row>
     <row r="55" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A55" s="294"/>
-      <c r="B55" s="313"/>
-      <c r="C55" s="313"/>
+      <c r="A55" s="296"/>
+      <c r="B55" s="308"/>
+      <c r="C55" s="308"/>
       <c r="D55" s="139" t="s">
         <v>117</v>
       </c>
@@ -23642,13 +23642,13 @@
       <c r="AH56" s="51"/>
     </row>
     <row r="57" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A57" s="294" t="s">
+      <c r="A57" s="296" t="s">
         <v>121</v>
       </c>
-      <c r="B57" s="294" t="s">
+      <c r="B57" s="296" t="s">
         <v>12</v>
       </c>
-      <c r="C57" s="311">
+      <c r="C57" s="307">
         <v>538.005973433431</v>
       </c>
       <c r="D57" s="52" t="s">
@@ -23720,9 +23720,9 @@
       <c r="AH57" s="59"/>
     </row>
     <row r="58" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A58" s="294"/>
-      <c r="B58" s="294"/>
-      <c r="C58" s="311"/>
+      <c r="A58" s="296"/>
+      <c r="B58" s="296"/>
+      <c r="C58" s="307"/>
       <c r="D58" s="52" t="s">
         <v>117</v>
       </c>
@@ -23792,13 +23792,13 @@
       <c r="AH58" s="63"/>
     </row>
     <row r="59" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A59" s="295" t="s">
+      <c r="A59" s="298" t="s">
         <v>122</v>
       </c>
-      <c r="B59" s="294" t="s">
+      <c r="B59" s="296" t="s">
         <v>12</v>
       </c>
-      <c r="C59" s="311">
+      <c r="C59" s="307">
         <v>70.703999727247606</v>
       </c>
       <c r="D59" s="52" t="s">
@@ -23876,9 +23876,9 @@
       <c r="AH59" s="59"/>
     </row>
     <row r="60" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A60" s="295"/>
-      <c r="B60" s="294"/>
-      <c r="C60" s="311"/>
+      <c r="A60" s="298"/>
+      <c r="B60" s="296"/>
+      <c r="C60" s="307"/>
       <c r="D60" s="52" t="s">
         <v>117</v>
       </c>
@@ -23954,13 +23954,13 @@
       <c r="AH60" s="62"/>
     </row>
     <row r="61" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A61" s="294" t="s">
+      <c r="A61" s="296" t="s">
         <v>123</v>
       </c>
-      <c r="B61" s="313">
+      <c r="B61" s="308">
         <v>0.5</v>
       </c>
-      <c r="C61" s="312">
+      <c r="C61" s="309">
         <v>14500</v>
       </c>
       <c r="D61" s="139" t="s">
@@ -24058,9 +24058,9 @@
       </c>
     </row>
     <row r="62" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A62" s="294"/>
-      <c r="B62" s="313"/>
-      <c r="C62" s="313"/>
+      <c r="A62" s="296"/>
+      <c r="B62" s="308"/>
+      <c r="C62" s="308"/>
       <c r="D62" s="139" t="s">
         <v>117</v>
       </c>
@@ -24194,13 +24194,13 @@
       <c r="AH63" s="51"/>
     </row>
     <row r="64" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A64" s="294" t="s">
+      <c r="A64" s="296" t="s">
         <v>125</v>
       </c>
-      <c r="B64" s="295" t="s">
+      <c r="B64" s="298" t="s">
         <v>12</v>
       </c>
-      <c r="C64" s="311">
+      <c r="C64" s="307">
         <f>+E64</f>
         <v>2309.2137610162299</v>
       </c>
@@ -24271,9 +24271,9 @@
       <c r="AH64" s="59"/>
     </row>
     <row r="65" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A65" s="294"/>
-      <c r="B65" s="295"/>
-      <c r="C65" s="311"/>
+      <c r="A65" s="296"/>
+      <c r="B65" s="298"/>
+      <c r="C65" s="307"/>
       <c r="D65" s="52" t="s">
         <v>117</v>
       </c>
@@ -24379,13 +24379,13 @@
       <c r="AH66" s="51"/>
     </row>
     <row r="67" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A67" s="294" t="s">
+      <c r="A67" s="296" t="s">
         <v>127</v>
       </c>
-      <c r="B67" s="294" t="s">
+      <c r="B67" s="296" t="s">
         <v>12</v>
       </c>
-      <c r="C67" s="312">
+      <c r="C67" s="309">
         <v>14500</v>
       </c>
       <c r="D67" s="52" t="s">
@@ -24483,9 +24483,9 @@
       </c>
     </row>
     <row r="68" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A68" s="294"/>
-      <c r="B68" s="294"/>
-      <c r="C68" s="312"/>
+      <c r="A68" s="296"/>
+      <c r="B68" s="296"/>
+      <c r="C68" s="309"/>
       <c r="D68" s="52" t="s">
         <v>117</v>
       </c>
@@ -24638,16 +24638,16 @@
       </c>
     </row>
     <row r="78" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A78" s="291" t="s">
+      <c r="A78" s="302" t="s">
         <v>128</v>
       </c>
-      <c r="B78" s="291"/>
-      <c r="C78" s="291"/>
-      <c r="E78" s="292" t="s">
+      <c r="B78" s="302"/>
+      <c r="C78" s="302"/>
+      <c r="E78" s="303" t="s">
         <v>129</v>
       </c>
-      <c r="F78" s="292"/>
-      <c r="G78" s="292"/>
+      <c r="F78" s="303"/>
+      <c r="G78" s="303"/>
     </row>
     <row r="79" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A79" s="66" t="s">
@@ -24902,10 +24902,10 @@
       </c>
     </row>
     <row r="99" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A99" s="291" t="s">
+      <c r="A99" s="302" t="s">
         <v>30</v>
       </c>
-      <c r="B99" s="291"/>
+      <c r="B99" s="302"/>
       <c r="C99" s="15">
         <v>1995</v>
       </c>
@@ -30787,11 +30787,11 @@
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A218" s="293" t="s">
+      <c r="A218" s="304" t="s">
         <v>266</v>
       </c>
-      <c r="B218" s="293"/>
-      <c r="C218" s="293"/>
+      <c r="B218" s="304"/>
+      <c r="C218" s="304"/>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A219" s="106" t="s">
@@ -30884,10 +30884,10 @@
     </row>
     <row r="232" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="233" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A233" s="308" t="s">
+      <c r="A233" s="313" t="s">
         <v>270</v>
       </c>
-      <c r="B233" s="308"/>
+      <c r="B233" s="313"/>
       <c r="C233" s="181" t="s">
         <v>229</v>
       </c>
@@ -30938,7 +30938,7 @@
       <c r="A234" s="184" t="s">
         <v>271</v>
       </c>
-      <c r="B234" s="309" t="s">
+      <c r="B234" s="314" t="s">
         <v>244</v>
       </c>
       <c r="C234" s="185" t="s">
@@ -30991,7 +30991,7 @@
       <c r="A235" s="184" t="s">
         <v>273</v>
       </c>
-      <c r="B235" s="309"/>
+      <c r="B235" s="314"/>
       <c r="C235" s="185" t="s">
         <v>324</v>
       </c>
@@ -31042,7 +31042,7 @@
       <c r="A236" s="184" t="s">
         <v>274</v>
       </c>
-      <c r="B236" s="309"/>
+      <c r="B236" s="314"/>
       <c r="C236" s="185" t="s">
         <v>324</v>
       </c>
@@ -31093,7 +31093,7 @@
       <c r="A237" s="184" t="s">
         <v>275</v>
       </c>
-      <c r="B237" s="309"/>
+      <c r="B237" s="314"/>
       <c r="C237" s="185" t="s">
         <v>324</v>
       </c>
@@ -31144,7 +31144,7 @@
       <c r="A238" s="184" t="s">
         <v>276</v>
       </c>
-      <c r="B238" s="309"/>
+      <c r="B238" s="314"/>
       <c r="C238" s="185" t="s">
         <v>324</v>
       </c>
@@ -31195,7 +31195,7 @@
       <c r="A239" s="184" t="s">
         <v>271</v>
       </c>
-      <c r="B239" s="309" t="s">
+      <c r="B239" s="314" t="s">
         <v>245</v>
       </c>
       <c r="C239" s="185" t="s">
@@ -31248,7 +31248,7 @@
       <c r="A240" s="184" t="s">
         <v>273</v>
       </c>
-      <c r="B240" s="309"/>
+      <c r="B240" s="314"/>
       <c r="C240" s="185" t="s">
         <v>324</v>
       </c>
@@ -31299,7 +31299,7 @@
       <c r="A241" s="184" t="s">
         <v>274</v>
       </c>
-      <c r="B241" s="309"/>
+      <c r="B241" s="314"/>
       <c r="C241" s="185" t="s">
         <v>324</v>
       </c>
@@ -31350,7 +31350,7 @@
       <c r="A242" s="184" t="s">
         <v>275</v>
       </c>
-      <c r="B242" s="309"/>
+      <c r="B242" s="314"/>
       <c r="C242" s="185" t="s">
         <v>324</v>
       </c>
@@ -31401,7 +31401,7 @@
       <c r="A243" s="184" t="s">
         <v>276</v>
       </c>
-      <c r="B243" s="309"/>
+      <c r="B243" s="314"/>
       <c r="C243" s="185" t="s">
         <v>324</v>
       </c>
@@ -31452,7 +31452,7 @@
       <c r="A244" s="184" t="s">
         <v>278</v>
       </c>
-      <c r="B244" s="309" t="s">
+      <c r="B244" s="314" t="s">
         <v>246</v>
       </c>
       <c r="C244" s="185" t="s">
@@ -31505,7 +31505,7 @@
       <c r="A245" s="184" t="s">
         <v>273</v>
       </c>
-      <c r="B245" s="309"/>
+      <c r="B245" s="314"/>
       <c r="C245" s="185" t="s">
         <v>324</v>
       </c>
@@ -31556,7 +31556,7 @@
       <c r="A246" s="184" t="s">
         <v>274</v>
       </c>
-      <c r="B246" s="309"/>
+      <c r="B246" s="314"/>
       <c r="C246" s="185" t="s">
         <v>324</v>
       </c>
@@ -31607,7 +31607,7 @@
       <c r="A247" s="184" t="s">
         <v>275</v>
       </c>
-      <c r="B247" s="309"/>
+      <c r="B247" s="314"/>
       <c r="C247" s="185" t="s">
         <v>324</v>
       </c>
@@ -31658,7 +31658,7 @@
       <c r="A248" s="184" t="s">
         <v>276</v>
       </c>
-      <c r="B248" s="309"/>
+      <c r="B248" s="314"/>
       <c r="C248" s="185" t="s">
         <v>324</v>
       </c>
@@ -31709,7 +31709,7 @@
       <c r="A249" s="184" t="s">
         <v>271</v>
       </c>
-      <c r="B249" s="309" t="s">
+      <c r="B249" s="314" t="s">
         <v>247</v>
       </c>
       <c r="C249" s="185" t="s">
@@ -31762,7 +31762,7 @@
       <c r="A250" s="184" t="s">
         <v>273</v>
       </c>
-      <c r="B250" s="309"/>
+      <c r="B250" s="314"/>
       <c r="C250" s="185" t="s">
         <v>324</v>
       </c>
@@ -31813,7 +31813,7 @@
       <c r="A251" s="184" t="s">
         <v>274</v>
       </c>
-      <c r="B251" s="309"/>
+      <c r="B251" s="314"/>
       <c r="C251" s="185" t="s">
         <v>324</v>
       </c>
@@ -31864,7 +31864,7 @@
       <c r="A252" s="184" t="s">
         <v>275</v>
       </c>
-      <c r="B252" s="309"/>
+      <c r="B252" s="314"/>
       <c r="C252" s="185" t="s">
         <v>324</v>
       </c>
@@ -31915,7 +31915,7 @@
       <c r="A253" s="184" t="s">
         <v>276</v>
       </c>
-      <c r="B253" s="309"/>
+      <c r="B253" s="314"/>
       <c r="C253" s="185" t="s">
         <v>324</v>
       </c>
@@ -31966,7 +31966,7 @@
       <c r="A254" s="184" t="s">
         <v>271</v>
       </c>
-      <c r="B254" s="306" t="s">
+      <c r="B254" s="311" t="s">
         <v>248</v>
       </c>
       <c r="C254" s="185" t="s">
@@ -32019,7 +32019,7 @@
       <c r="A255" s="184" t="s">
         <v>273</v>
       </c>
-      <c r="B255" s="306"/>
+      <c r="B255" s="311"/>
       <c r="C255" s="185" t="s">
         <v>324</v>
       </c>
@@ -32070,7 +32070,7 @@
       <c r="A256" s="184" t="s">
         <v>274</v>
       </c>
-      <c r="B256" s="306"/>
+      <c r="B256" s="311"/>
       <c r="C256" s="185" t="s">
         <v>324</v>
       </c>
@@ -32121,7 +32121,7 @@
       <c r="A257" s="184" t="s">
         <v>275</v>
       </c>
-      <c r="B257" s="306"/>
+      <c r="B257" s="311"/>
       <c r="C257" s="185" t="s">
         <v>324</v>
       </c>
@@ -32172,7 +32172,7 @@
       <c r="A258" s="186" t="s">
         <v>276</v>
       </c>
-      <c r="B258" s="306"/>
+      <c r="B258" s="311"/>
       <c r="C258" s="185" t="s">
         <v>324</v>
       </c>
@@ -32554,10 +32554,10 @@
       </c>
     </row>
     <row r="267" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A267" s="307" t="s">
+      <c r="A267" s="312" t="s">
         <v>282</v>
       </c>
-      <c r="B267" s="307"/>
+      <c r="B267" s="312"/>
       <c r="C267" s="200"/>
     </row>
     <row r="268" spans="1:27" x14ac:dyDescent="0.3">
@@ -32597,46 +32597,6 @@
     </row>
   </sheetData>
   <mergeCells count="47">
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="A27:C27"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="H28:J28"/>
-    <mergeCell ref="A30:C30"/>
-    <mergeCell ref="E30:G30"/>
-    <mergeCell ref="E32:G32"/>
-    <mergeCell ref="A36:C36"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="A50:A51"/>
-    <mergeCell ref="B50:B51"/>
-    <mergeCell ref="C50:C51"/>
-    <mergeCell ref="A52:A53"/>
-    <mergeCell ref="B52:B53"/>
-    <mergeCell ref="C52:C53"/>
-    <mergeCell ref="A54:A55"/>
-    <mergeCell ref="B54:B55"/>
-    <mergeCell ref="C54:C55"/>
-    <mergeCell ref="A57:A58"/>
-    <mergeCell ref="B57:B58"/>
-    <mergeCell ref="C57:C58"/>
-    <mergeCell ref="A59:A60"/>
-    <mergeCell ref="B59:B60"/>
-    <mergeCell ref="C59:C60"/>
-    <mergeCell ref="A61:A62"/>
-    <mergeCell ref="B61:B62"/>
-    <mergeCell ref="C61:C62"/>
-    <mergeCell ref="A64:A65"/>
-    <mergeCell ref="B64:B65"/>
-    <mergeCell ref="C64:C65"/>
-    <mergeCell ref="A67:A68"/>
-    <mergeCell ref="B67:B68"/>
-    <mergeCell ref="C67:C68"/>
-    <mergeCell ref="A72:C72"/>
-    <mergeCell ref="A78:C78"/>
-    <mergeCell ref="E78:G78"/>
-    <mergeCell ref="A99:B99"/>
-    <mergeCell ref="A218:C218"/>
     <mergeCell ref="B254:B258"/>
     <mergeCell ref="A267:B267"/>
     <mergeCell ref="A233:B233"/>
@@ -32644,6 +32604,46 @@
     <mergeCell ref="B239:B243"/>
     <mergeCell ref="B244:B248"/>
     <mergeCell ref="B249:B253"/>
+    <mergeCell ref="A72:C72"/>
+    <mergeCell ref="A78:C78"/>
+    <mergeCell ref="E78:G78"/>
+    <mergeCell ref="A99:B99"/>
+    <mergeCell ref="A218:C218"/>
+    <mergeCell ref="A64:A65"/>
+    <mergeCell ref="B64:B65"/>
+    <mergeCell ref="C64:C65"/>
+    <mergeCell ref="A67:A68"/>
+    <mergeCell ref="B67:B68"/>
+    <mergeCell ref="C67:C68"/>
+    <mergeCell ref="A59:A60"/>
+    <mergeCell ref="B59:B60"/>
+    <mergeCell ref="C59:C60"/>
+    <mergeCell ref="A61:A62"/>
+    <mergeCell ref="B61:B62"/>
+    <mergeCell ref="C61:C62"/>
+    <mergeCell ref="A54:A55"/>
+    <mergeCell ref="B54:B55"/>
+    <mergeCell ref="C54:C55"/>
+    <mergeCell ref="A57:A58"/>
+    <mergeCell ref="B57:B58"/>
+    <mergeCell ref="C57:C58"/>
+    <mergeCell ref="A50:A51"/>
+    <mergeCell ref="B50:B51"/>
+    <mergeCell ref="C50:C51"/>
+    <mergeCell ref="A52:A53"/>
+    <mergeCell ref="B52:B53"/>
+    <mergeCell ref="C52:C53"/>
+    <mergeCell ref="H28:J28"/>
+    <mergeCell ref="A30:C30"/>
+    <mergeCell ref="E30:G30"/>
+    <mergeCell ref="E32:G32"/>
+    <mergeCell ref="A36:C36"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="E28:G28"/>
   </mergeCells>
   <conditionalFormatting sqref="B183:P183">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
@@ -32670,7 +32670,7 @@
   <dimension ref="A2:AH288"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F10" sqref="F1:F10"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -32726,7 +32726,7 @@
         <v>0.15</v>
       </c>
       <c r="C4">
-        <v>0.27331499999999997</v>
+        <v>0.2306</v>
       </c>
       <c r="E4">
         <v>0.231662100456621</v>
@@ -32745,7 +32745,7 @@
       <c r="E5" s="21">
         <v>0</v>
       </c>
-      <c r="F5" s="322"/>
+      <c r="F5" s="287"/>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
@@ -32761,7 +32761,7 @@
       <c r="E6">
         <v>0.46046614548285097</v>
       </c>
-      <c r="F6" s="322"/>
+      <c r="F6" s="287"/>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
@@ -32814,10 +32814,10 @@
       </c>
       <c r="B10" s="8">
         <f>C10/4</f>
-        <v>4.5718190862338998E-2</v>
+        <v>4.5172499999999997E-2</v>
       </c>
       <c r="C10" s="202">
-        <v>0.18287276344935599</v>
+        <v>0.18068999999999999</v>
       </c>
       <c r="E10" s="201">
         <v>0.10100000000000001</v>
@@ -33022,21 +33022,21 @@
       <c r="L20" s="136"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A21" s="301"/>
-      <c r="B21" s="301"/>
-      <c r="C21" s="301"/>
+      <c r="A21" s="290"/>
+      <c r="B21" s="290"/>
+      <c r="C21" s="290"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A22" s="304"/>
-      <c r="B22" s="304"/>
-      <c r="C22" s="304"/>
+      <c r="A22" s="291"/>
+      <c r="B22" s="291"/>
+      <c r="C22" s="291"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A23" s="305" t="s">
+      <c r="A23" s="292" t="s">
         <v>30</v>
       </c>
-      <c r="B23" s="305"/>
-      <c r="C23" s="305"/>
+      <c r="B23" s="292"/>
+      <c r="C23" s="292"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" s="10" t="s">
@@ -33070,11 +33070,11 @@
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A26" s="302" t="s">
+      <c r="A26" s="293" t="s">
         <v>77</v>
       </c>
-      <c r="B26" s="302"/>
-      <c r="C26" s="302"/>
+      <c r="B26" s="293"/>
+      <c r="C26" s="293"/>
       <c r="E26" s="10" t="s">
         <v>78</v>
       </c>
@@ -33095,14 +33095,14 @@
       <c r="C27" s="39">
         <v>0</v>
       </c>
-      <c r="E27" s="302" t="s">
+      <c r="E27" s="293" t="s">
         <v>32</v>
       </c>
-      <c r="F27" s="302"/>
-      <c r="G27" s="302"/>
-      <c r="H27" s="301"/>
-      <c r="I27" s="301"/>
-      <c r="J27" s="301"/>
+      <c r="F27" s="293"/>
+      <c r="G27" s="293"/>
+      <c r="H27" s="290"/>
+      <c r="I27" s="290"/>
+      <c r="J27" s="290"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" s="10"/>
@@ -33119,16 +33119,16 @@
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A29" s="302" t="s">
+      <c r="A29" s="293" t="s">
         <v>84</v>
       </c>
-      <c r="B29" s="302"/>
-      <c r="C29" s="302"/>
-      <c r="E29" s="302" t="s">
+      <c r="B29" s="293"/>
+      <c r="C29" s="293"/>
+      <c r="E29" s="293" t="s">
         <v>85</v>
       </c>
-      <c r="F29" s="302"/>
-      <c r="G29" s="302"/>
+      <c r="F29" s="293"/>
+      <c r="G29" s="293"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" s="205" t="s">
@@ -33160,11 +33160,11 @@
       <c r="C31" s="108">
         <v>0</v>
       </c>
-      <c r="E31" s="302" t="s">
+      <c r="E31" s="293" t="s">
         <v>89</v>
       </c>
-      <c r="F31" s="302"/>
-      <c r="G31" s="302"/>
+      <c r="F31" s="293"/>
+      <c r="G31" s="293"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" s="206" t="s">
@@ -33198,11 +33198,11 @@
       </c>
     </row>
     <row r="35" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A35" s="302" t="s">
+      <c r="A35" s="293" t="s">
         <v>93</v>
       </c>
-      <c r="B35" s="302"/>
-      <c r="C35" s="302"/>
+      <c r="B35" s="293"/>
+      <c r="C35" s="293"/>
     </row>
     <row r="36" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B36" s="207" t="s">
@@ -34596,10 +34596,10 @@
       <c r="AH63" s="51"/>
     </row>
     <row r="64" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A64" s="298" t="s">
+      <c r="A64" s="295" t="s">
         <v>115</v>
       </c>
-      <c r="B64" s="294" t="s">
+      <c r="B64" s="296" t="s">
         <v>12</v>
       </c>
       <c r="C64" s="315">
@@ -34700,8 +34700,8 @@
       </c>
     </row>
     <row r="65" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A65" s="298"/>
-      <c r="B65" s="294"/>
+      <c r="A65" s="295"/>
+      <c r="B65" s="296"/>
       <c r="C65" s="315"/>
       <c r="D65" s="52" t="s">
         <v>117</v>
@@ -34798,13 +34798,13 @@
       </c>
     </row>
     <row r="66" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A66" s="295" t="s">
+      <c r="A66" s="298" t="s">
         <v>118</v>
       </c>
-      <c r="B66" s="294" t="s">
+      <c r="B66" s="296" t="s">
         <v>12</v>
       </c>
-      <c r="C66" s="300">
+      <c r="C66" s="299">
         <v>0</v>
       </c>
       <c r="D66" s="52" t="s">
@@ -34902,9 +34902,9 @@
       </c>
     </row>
     <row r="67" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A67" s="295"/>
-      <c r="B67" s="294"/>
-      <c r="C67" s="300"/>
+      <c r="A67" s="298"/>
+      <c r="B67" s="296"/>
+      <c r="C67" s="299"/>
       <c r="D67" s="52" t="s">
         <v>117</v>
       </c>
@@ -35000,7 +35000,7 @@
       </c>
     </row>
     <row r="68" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A68" s="294" t="s">
+      <c r="A68" s="296" t="s">
         <v>119</v>
       </c>
       <c r="B68" s="316">
@@ -35104,7 +35104,7 @@
       </c>
     </row>
     <row r="69" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A69" s="294"/>
+      <c r="A69" s="296"/>
       <c r="B69" s="316"/>
       <c r="C69" s="315"/>
       <c r="D69" s="52" t="s">
@@ -35240,10 +35240,10 @@
       <c r="AH70" s="213"/>
     </row>
     <row r="71" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A71" s="294" t="s">
+      <c r="A71" s="296" t="s">
         <v>121</v>
       </c>
-      <c r="B71" s="294" t="s">
+      <c r="B71" s="296" t="s">
         <v>12</v>
       </c>
       <c r="C71" s="315">
@@ -35344,8 +35344,8 @@
       </c>
     </row>
     <row r="72" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A72" s="294"/>
-      <c r="B72" s="294"/>
+      <c r="A72" s="296"/>
+      <c r="B72" s="296"/>
       <c r="C72" s="315"/>
       <c r="D72" s="52" t="s">
         <v>117</v>
@@ -35442,13 +35442,13 @@
       </c>
     </row>
     <row r="73" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A73" s="295" t="s">
+      <c r="A73" s="298" t="s">
         <v>122</v>
       </c>
-      <c r="B73" s="294" t="s">
+      <c r="B73" s="296" t="s">
         <v>12</v>
       </c>
-      <c r="C73" s="300">
+      <c r="C73" s="299">
         <v>0</v>
       </c>
       <c r="D73" s="52" t="s">
@@ -35546,9 +35546,9 @@
       </c>
     </row>
     <row r="74" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A74" s="295"/>
-      <c r="B74" s="294"/>
-      <c r="C74" s="300"/>
+      <c r="A74" s="298"/>
+      <c r="B74" s="296"/>
+      <c r="C74" s="299"/>
       <c r="D74" s="52" t="s">
         <v>117</v>
       </c>
@@ -35644,7 +35644,7 @@
       </c>
     </row>
     <row r="75" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A75" s="294" t="s">
+      <c r="A75" s="296" t="s">
         <v>123</v>
       </c>
       <c r="B75" s="316">
@@ -35748,7 +35748,7 @@
       </c>
     </row>
     <row r="76" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A76" s="294"/>
+      <c r="A76" s="296"/>
       <c r="B76" s="316"/>
       <c r="C76" s="315"/>
       <c r="D76" s="52" t="s">
@@ -35884,10 +35884,10 @@
       <c r="AH77" s="213"/>
     </row>
     <row r="78" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A78" s="294" t="s">
+      <c r="A78" s="296" t="s">
         <v>125</v>
       </c>
-      <c r="B78" s="295" t="s">
+      <c r="B78" s="298" t="s">
         <v>12</v>
       </c>
       <c r="C78" s="315">
@@ -35988,8 +35988,8 @@
       </c>
     </row>
     <row r="79" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A79" s="294"/>
-      <c r="B79" s="295"/>
+      <c r="A79" s="296"/>
+      <c r="B79" s="298"/>
       <c r="C79" s="315"/>
       <c r="D79" s="52" t="s">
         <v>117</v>
@@ -36124,13 +36124,13 @@
       <c r="AH80" s="213"/>
     </row>
     <row r="81" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A81" s="294" t="s">
+      <c r="A81" s="296" t="s">
         <v>127</v>
       </c>
-      <c r="B81" s="294" t="s">
+      <c r="B81" s="296" t="s">
         <v>12</v>
       </c>
-      <c r="C81" s="300">
+      <c r="C81" s="299">
         <v>0</v>
       </c>
       <c r="D81" s="52" t="s">
@@ -36228,9 +36228,9 @@
       </c>
     </row>
     <row r="82" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A82" s="294"/>
-      <c r="B82" s="294"/>
-      <c r="C82" s="300"/>
+      <c r="A82" s="296"/>
+      <c r="B82" s="296"/>
+      <c r="C82" s="299"/>
       <c r="D82" s="52" t="s">
         <v>117</v>
       </c>
@@ -36340,11 +36340,11 @@
       </c>
     </row>
     <row r="86" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A86" s="302" t="s">
+      <c r="A86" s="293" t="s">
         <v>291</v>
       </c>
-      <c r="B86" s="302"/>
-      <c r="C86" s="302"/>
+      <c r="B86" s="293"/>
+      <c r="C86" s="293"/>
     </row>
     <row r="87" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A87" s="215" t="s">
@@ -36383,16 +36383,16 @@
       </c>
     </row>
     <row r="92" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A92" s="305" t="s">
+      <c r="A92" s="292" t="s">
         <v>128</v>
       </c>
-      <c r="B92" s="305"/>
-      <c r="C92" s="305"/>
-      <c r="E92" s="314" t="s">
+      <c r="B92" s="292"/>
+      <c r="C92" s="292"/>
+      <c r="E92" s="317" t="s">
         <v>129</v>
       </c>
-      <c r="F92" s="314"/>
-      <c r="G92" s="314"/>
+      <c r="F92" s="317"/>
+      <c r="G92" s="317"/>
     </row>
     <row r="93" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A93" s="52" t="s">
@@ -36649,10 +36649,10 @@
       </c>
     </row>
     <row r="113" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A113" s="291" t="s">
+      <c r="A113" s="302" t="s">
         <v>30</v>
       </c>
-      <c r="B113" s="291"/>
+      <c r="B113" s="302"/>
       <c r="C113" s="15">
         <v>1995</v>
       </c>
@@ -43046,11 +43046,11 @@
       </c>
     </row>
     <row r="233" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A233" s="293" t="s">
+      <c r="A233" s="304" t="s">
         <v>266</v>
       </c>
-      <c r="B233" s="293"/>
-      <c r="C233" s="293"/>
+      <c r="B233" s="304"/>
+      <c r="C233" s="304"/>
     </row>
     <row r="234" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A234" s="106" t="s">
@@ -44113,7 +44113,7 @@
       <c r="A257" s="119" t="s">
         <v>271</v>
       </c>
-      <c r="B257" s="289" t="s">
+      <c r="B257" s="305" t="s">
         <v>244</v>
       </c>
       <c r="C257" s="120">
@@ -44166,7 +44166,7 @@
       <c r="A258" s="123" t="s">
         <v>273</v>
       </c>
-      <c r="B258" s="289"/>
+      <c r="B258" s="305"/>
       <c r="C258" s="124">
         <v>0.9</v>
       </c>
@@ -44217,7 +44217,7 @@
       <c r="A259" s="123" t="s">
         <v>274</v>
       </c>
-      <c r="B259" s="289"/>
+      <c r="B259" s="305"/>
       <c r="C259" s="124">
         <v>0.9</v>
       </c>
@@ -44268,7 +44268,7 @@
       <c r="A260" s="123" t="s">
         <v>275</v>
       </c>
-      <c r="B260" s="289"/>
+      <c r="B260" s="305"/>
       <c r="C260" s="124">
         <v>0.9</v>
       </c>
@@ -44319,7 +44319,7 @@
       <c r="A261" s="125" t="s">
         <v>276</v>
       </c>
-      <c r="B261" s="289"/>
+      <c r="B261" s="305"/>
       <c r="C261" s="124">
         <v>0.9</v>
       </c>
@@ -44370,7 +44370,7 @@
       <c r="A262" s="126" t="s">
         <v>271</v>
       </c>
-      <c r="B262" s="289" t="s">
+      <c r="B262" s="305" t="s">
         <v>245</v>
       </c>
       <c r="C262" s="124">
@@ -44423,7 +44423,7 @@
       <c r="A263" s="127" t="s">
         <v>273</v>
       </c>
-      <c r="B263" s="289"/>
+      <c r="B263" s="305"/>
       <c r="C263" s="120">
         <v>0</v>
       </c>
@@ -44474,7 +44474,7 @@
       <c r="A264" s="127" t="s">
         <v>274</v>
       </c>
-      <c r="B264" s="289"/>
+      <c r="B264" s="305"/>
       <c r="C264" s="124">
         <v>0.2</v>
       </c>
@@ -44525,7 +44525,7 @@
       <c r="A265" s="127" t="s">
         <v>275</v>
       </c>
-      <c r="B265" s="289"/>
+      <c r="B265" s="305"/>
       <c r="C265" s="124">
         <v>0.6</v>
       </c>
@@ -44576,7 +44576,7 @@
       <c r="A266" s="128" t="s">
         <v>276</v>
       </c>
-      <c r="B266" s="289"/>
+      <c r="B266" s="305"/>
       <c r="C266" s="124">
         <v>0.6</v>
       </c>
@@ -44627,7 +44627,7 @@
       <c r="A267" s="129" t="s">
         <v>278</v>
       </c>
-      <c r="B267" s="289" t="s">
+      <c r="B267" s="305" t="s">
         <v>246</v>
       </c>
       <c r="C267" s="124">
@@ -44680,7 +44680,7 @@
       <c r="A268" s="127" t="s">
         <v>273</v>
       </c>
-      <c r="B268" s="289"/>
+      <c r="B268" s="305"/>
       <c r="C268" s="124">
         <v>0.01</v>
       </c>
@@ -44731,7 +44731,7 @@
       <c r="A269" s="127" t="s">
         <v>274</v>
       </c>
-      <c r="B269" s="289"/>
+      <c r="B269" s="305"/>
       <c r="C269" s="120">
         <v>0</v>
       </c>
@@ -44782,7 +44782,7 @@
       <c r="A270" s="127" t="s">
         <v>275</v>
       </c>
-      <c r="B270" s="289"/>
+      <c r="B270" s="305"/>
       <c r="C270" s="124">
         <v>0.4</v>
       </c>
@@ -44833,7 +44833,7 @@
       <c r="A271" s="128" t="s">
         <v>276</v>
       </c>
-      <c r="B271" s="289"/>
+      <c r="B271" s="305"/>
       <c r="C271" s="124">
         <v>0.1</v>
       </c>
@@ -44884,7 +44884,7 @@
       <c r="A272" s="129" t="s">
         <v>271</v>
       </c>
-      <c r="B272" s="289" t="s">
+      <c r="B272" s="305" t="s">
         <v>247</v>
       </c>
       <c r="C272" s="124">
@@ -44937,7 +44937,7 @@
       <c r="A273" s="127" t="s">
         <v>273</v>
       </c>
-      <c r="B273" s="289"/>
+      <c r="B273" s="305"/>
       <c r="C273" s="124">
         <v>0.01</v>
       </c>
@@ -44988,7 +44988,7 @@
       <c r="A274" s="127" t="s">
         <v>274</v>
       </c>
-      <c r="B274" s="289"/>
+      <c r="B274" s="305"/>
       <c r="C274" s="124">
         <v>0.01</v>
       </c>
@@ -45039,7 +45039,7 @@
       <c r="A275" s="127" t="s">
         <v>275</v>
       </c>
-      <c r="B275" s="289"/>
+      <c r="B275" s="305"/>
       <c r="C275" s="120">
         <v>0</v>
       </c>
@@ -45090,7 +45090,7 @@
       <c r="A276" s="128" t="s">
         <v>276</v>
       </c>
-      <c r="B276" s="289"/>
+      <c r="B276" s="305"/>
       <c r="C276" s="124">
         <v>0.01</v>
       </c>
@@ -45141,7 +45141,7 @@
       <c r="A277" s="129" t="s">
         <v>271</v>
       </c>
-      <c r="B277" s="289" t="s">
+      <c r="B277" s="305" t="s">
         <v>248</v>
       </c>
       <c r="C277" s="124">
@@ -45194,7 +45194,7 @@
       <c r="A278" s="127" t="s">
         <v>273</v>
       </c>
-      <c r="B278" s="289"/>
+      <c r="B278" s="305"/>
       <c r="C278" s="124">
         <v>0</v>
       </c>
@@ -45245,7 +45245,7 @@
       <c r="A279" s="127" t="s">
         <v>274</v>
       </c>
-      <c r="B279" s="289"/>
+      <c r="B279" s="305"/>
       <c r="C279" s="124">
         <v>0.1</v>
       </c>
@@ -45296,7 +45296,7 @@
       <c r="A280" s="127" t="s">
         <v>275</v>
       </c>
-      <c r="B280" s="289"/>
+      <c r="B280" s="305"/>
       <c r="C280" s="124">
         <v>0.1</v>
       </c>
@@ -45347,7 +45347,7 @@
       <c r="A281" s="128" t="s">
         <v>276</v>
       </c>
-      <c r="B281" s="289"/>
+      <c r="B281" s="305"/>
       <c r="C281" s="130">
         <v>0</v>
       </c>
@@ -45395,10 +45395,10 @@
       </c>
     </row>
     <row r="284" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A284" s="307" t="s">
+      <c r="A284" s="312" t="s">
         <v>282</v>
       </c>
-      <c r="B284" s="307"/>
+      <c r="B284" s="312"/>
     </row>
     <row r="285" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A285" t="s">
@@ -45437,51 +45437,51 @@
     </row>
   </sheetData>
   <mergeCells count="45">
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="E27:G27"/>
-    <mergeCell ref="H27:J27"/>
-    <mergeCell ref="A29:C29"/>
-    <mergeCell ref="E29:G29"/>
-    <mergeCell ref="E31:G31"/>
-    <mergeCell ref="A35:C35"/>
+    <mergeCell ref="A284:B284"/>
+    <mergeCell ref="B257:B261"/>
+    <mergeCell ref="B262:B266"/>
+    <mergeCell ref="B267:B271"/>
+    <mergeCell ref="B272:B276"/>
+    <mergeCell ref="B277:B281"/>
+    <mergeCell ref="A86:C86"/>
+    <mergeCell ref="A92:C92"/>
+    <mergeCell ref="E92:G92"/>
+    <mergeCell ref="A113:B113"/>
+    <mergeCell ref="A233:C233"/>
+    <mergeCell ref="A78:A79"/>
+    <mergeCell ref="B78:B79"/>
+    <mergeCell ref="C78:C79"/>
+    <mergeCell ref="A81:A82"/>
+    <mergeCell ref="B81:B82"/>
+    <mergeCell ref="C81:C82"/>
+    <mergeCell ref="A73:A74"/>
+    <mergeCell ref="B73:B74"/>
+    <mergeCell ref="C73:C74"/>
+    <mergeCell ref="A75:A76"/>
+    <mergeCell ref="B75:B76"/>
+    <mergeCell ref="C75:C76"/>
+    <mergeCell ref="A68:A69"/>
+    <mergeCell ref="B68:B69"/>
+    <mergeCell ref="C68:C69"/>
+    <mergeCell ref="A71:A72"/>
+    <mergeCell ref="B71:B72"/>
+    <mergeCell ref="C71:C72"/>
     <mergeCell ref="A64:A65"/>
     <mergeCell ref="B64:B65"/>
     <mergeCell ref="C64:C65"/>
     <mergeCell ref="A66:A67"/>
     <mergeCell ref="B66:B67"/>
     <mergeCell ref="C66:C67"/>
-    <mergeCell ref="A68:A69"/>
-    <mergeCell ref="B68:B69"/>
-    <mergeCell ref="C68:C69"/>
-    <mergeCell ref="A71:A72"/>
-    <mergeCell ref="B71:B72"/>
-    <mergeCell ref="C71:C72"/>
-    <mergeCell ref="A73:A74"/>
-    <mergeCell ref="B73:B74"/>
-    <mergeCell ref="C73:C74"/>
-    <mergeCell ref="A75:A76"/>
-    <mergeCell ref="B75:B76"/>
-    <mergeCell ref="C75:C76"/>
-    <mergeCell ref="A78:A79"/>
-    <mergeCell ref="B78:B79"/>
-    <mergeCell ref="C78:C79"/>
-    <mergeCell ref="A81:A82"/>
-    <mergeCell ref="B81:B82"/>
-    <mergeCell ref="C81:C82"/>
-    <mergeCell ref="A86:C86"/>
-    <mergeCell ref="A92:C92"/>
-    <mergeCell ref="E92:G92"/>
-    <mergeCell ref="A113:B113"/>
-    <mergeCell ref="A233:C233"/>
-    <mergeCell ref="A284:B284"/>
-    <mergeCell ref="B257:B261"/>
-    <mergeCell ref="B262:B266"/>
-    <mergeCell ref="B267:B271"/>
-    <mergeCell ref="B272:B276"/>
-    <mergeCell ref="B277:B281"/>
+    <mergeCell ref="H27:J27"/>
+    <mergeCell ref="A29:C29"/>
+    <mergeCell ref="E29:G29"/>
+    <mergeCell ref="E31:G31"/>
+    <mergeCell ref="A35:C35"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="E27:G27"/>
   </mergeCells>
   <conditionalFormatting sqref="B197:P197">
     <cfRule type="cellIs" dxfId="0" priority="2" operator="lessThan">
@@ -45656,13 +45656,13 @@
       <c r="AM5" s="51"/>
     </row>
     <row r="6" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A6" s="294" t="s">
+      <c r="A6" s="296" t="s">
         <v>357</v>
       </c>
-      <c r="B6" s="294" t="s">
+      <c r="B6" s="296" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="296">
+      <c r="C6" s="301">
         <v>12500</v>
       </c>
       <c r="D6" s="52" t="s">
@@ -45757,9 +45757,9 @@
       <c r="AM6" s="258"/>
     </row>
     <row r="7" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A7" s="294"/>
-      <c r="B7" s="294"/>
-      <c r="C7" s="296"/>
+      <c r="A7" s="296"/>
+      <c r="B7" s="296"/>
+      <c r="C7" s="301"/>
       <c r="D7" s="52" t="s">
         <v>117</v>
       </c>
@@ -45852,13 +45852,13 @@
       <c r="AM7" s="259"/>
     </row>
     <row r="8" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A8" s="298" t="s">
+      <c r="A8" s="295" t="s">
         <v>358</v>
       </c>
-      <c r="B8" s="294" t="s">
+      <c r="B8" s="296" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="299">
+      <c r="C8" s="297">
         <v>14500</v>
       </c>
       <c r="D8" s="52" t="s">
@@ -45961,9 +45961,9 @@
       <c r="AM8" s="261"/>
     </row>
     <row r="9" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A9" s="298"/>
-      <c r="B9" s="298"/>
-      <c r="C9" s="299"/>
+      <c r="A9" s="295"/>
+      <c r="B9" s="295"/>
+      <c r="C9" s="297"/>
       <c r="D9" s="52" t="s">
         <v>117</v>
       </c>
@@ -46064,13 +46064,13 @@
       <c r="AM9" s="259"/>
     </row>
     <row r="10" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A10" s="295" t="s">
+      <c r="A10" s="298" t="s">
         <v>359</v>
       </c>
-      <c r="B10" s="294" t="s">
+      <c r="B10" s="296" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="300">
+      <c r="C10" s="299">
         <v>16700</v>
       </c>
       <c r="D10" s="52" t="s">
@@ -46183,9 +46183,9 @@
       </c>
     </row>
     <row r="11" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A11" s="295"/>
-      <c r="B11" s="294"/>
-      <c r="C11" s="300"/>
+      <c r="A11" s="298"/>
+      <c r="B11" s="296"/>
+      <c r="C11" s="299"/>
       <c r="D11" s="52" t="s">
         <v>117</v>
       </c>
@@ -46296,13 +46296,13 @@
       </c>
     </row>
     <row r="12" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A12" s="295" t="s">
+      <c r="A12" s="298" t="s">
         <v>360</v>
       </c>
-      <c r="B12" s="294" t="s">
+      <c r="B12" s="296" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="300">
+      <c r="C12" s="299">
         <v>10500</v>
       </c>
       <c r="D12" s="52" t="s">
@@ -46389,9 +46389,9 @@
       <c r="AM12" s="258"/>
     </row>
     <row r="13" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A13" s="295"/>
-      <c r="B13" s="294"/>
-      <c r="C13" s="300"/>
+      <c r="A13" s="298"/>
+      <c r="B13" s="296"/>
+      <c r="C13" s="299"/>
       <c r="D13" s="52" t="s">
         <v>117</v>
       </c>
@@ -46476,13 +46476,13 @@
       <c r="AM13" s="264"/>
     </row>
     <row r="14" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A14" s="295" t="s">
+      <c r="A14" s="298" t="s">
         <v>361</v>
       </c>
-      <c r="B14" s="294" t="s">
+      <c r="B14" s="296" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="300">
+      <c r="C14" s="299">
         <v>22000</v>
       </c>
       <c r="D14" s="52" t="s">
@@ -46571,9 +46571,9 @@
       <c r="AM14" s="258"/>
     </row>
     <row r="15" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A15" s="295"/>
-      <c r="B15" s="294"/>
-      <c r="C15" s="300"/>
+      <c r="A15" s="298"/>
+      <c r="B15" s="296"/>
+      <c r="C15" s="299"/>
       <c r="D15" s="52" t="s">
         <v>117</v>
       </c>
@@ -46660,13 +46660,13 @@
       <c r="AM15" s="264"/>
     </row>
     <row r="16" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A16" s="295" t="s">
+      <c r="A16" s="298" t="s">
         <v>362</v>
       </c>
-      <c r="B16" s="294" t="s">
+      <c r="B16" s="296" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="300">
+      <c r="C16" s="299">
         <v>6000</v>
       </c>
       <c r="D16" s="52" t="s">
@@ -46735,9 +46735,9 @@
       <c r="AM16" s="258"/>
     </row>
     <row r="17" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A17" s="295"/>
-      <c r="B17" s="294"/>
-      <c r="C17" s="300"/>
+      <c r="A17" s="298"/>
+      <c r="B17" s="296"/>
+      <c r="C17" s="299"/>
       <c r="D17" s="52" t="s">
         <v>117</v>
       </c>
@@ -46804,13 +46804,13 @@
       <c r="AM17" s="264"/>
     </row>
     <row r="18" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A18" s="294" t="s">
+      <c r="A18" s="296" t="s">
         <v>363</v>
       </c>
-      <c r="B18" s="297">
+      <c r="B18" s="300">
         <v>0.5</v>
       </c>
-      <c r="C18" s="296">
+      <c r="C18" s="301">
         <v>16800</v>
       </c>
       <c r="D18" s="52" t="s">
@@ -46911,9 +46911,9 @@
       <c r="AM18" s="258"/>
     </row>
     <row r="19" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A19" s="294"/>
-      <c r="B19" s="297"/>
-      <c r="C19" s="297"/>
+      <c r="A19" s="296"/>
+      <c r="B19" s="300"/>
+      <c r="C19" s="300"/>
       <c r="D19" s="52" t="s">
         <v>117</v>
       </c>
@@ -47055,13 +47055,13 @@
       <c r="AM20" s="51"/>
     </row>
     <row r="21" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A21" s="294" t="s">
+      <c r="A21" s="296" t="s">
         <v>364</v>
       </c>
-      <c r="B21" s="294" t="s">
+      <c r="B21" s="296" t="s">
         <v>12</v>
       </c>
-      <c r="C21" s="296">
+      <c r="C21" s="301">
         <v>11000</v>
       </c>
       <c r="D21" s="52" t="s">
@@ -47126,9 +47126,9 @@
       <c r="AM21" s="258"/>
     </row>
     <row r="22" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A22" s="294"/>
-      <c r="B22" s="294"/>
-      <c r="C22" s="296"/>
+      <c r="A22" s="296"/>
+      <c r="B22" s="296"/>
+      <c r="C22" s="301"/>
       <c r="D22" s="52" t="s">
         <v>117</v>
       </c>
@@ -47191,13 +47191,13 @@
       <c r="AM22" s="259"/>
     </row>
     <row r="23" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A23" s="294" t="s">
+      <c r="A23" s="296" t="s">
         <v>365</v>
       </c>
-      <c r="B23" s="294" t="s">
+      <c r="B23" s="296" t="s">
         <v>12</v>
       </c>
-      <c r="C23" s="296">
+      <c r="C23" s="301">
         <v>22500</v>
       </c>
       <c r="D23" s="52" t="s">
@@ -47272,9 +47272,9 @@
       <c r="AM23" s="258"/>
     </row>
     <row r="24" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A24" s="294"/>
-      <c r="B24" s="294"/>
-      <c r="C24" s="296"/>
+      <c r="A24" s="296"/>
+      <c r="B24" s="296"/>
+      <c r="C24" s="301"/>
       <c r="D24" s="52" t="s">
         <v>117</v>
       </c>
@@ -47347,13 +47347,13 @@
       <c r="AM24" s="259"/>
     </row>
     <row r="25" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A25" s="294" t="s">
+      <c r="A25" s="296" t="s">
         <v>366</v>
       </c>
-      <c r="B25" s="294" t="s">
+      <c r="B25" s="296" t="s">
         <v>12</v>
       </c>
-      <c r="C25" s="296">
+      <c r="C25" s="301">
         <v>13200</v>
       </c>
       <c r="D25" s="52" t="s">
@@ -47420,9 +47420,9 @@
       <c r="AM25" s="258"/>
     </row>
     <row r="26" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A26" s="294"/>
-      <c r="B26" s="294"/>
-      <c r="C26" s="296"/>
+      <c r="A26" s="296"/>
+      <c r="B26" s="296"/>
+      <c r="C26" s="301"/>
       <c r="D26" s="52" t="s">
         <v>117</v>
       </c>
@@ -47487,13 +47487,13 @@
       <c r="AM26" s="259"/>
     </row>
     <row r="27" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A27" s="295" t="s">
+      <c r="A27" s="298" t="s">
         <v>367</v>
       </c>
-      <c r="B27" s="294" t="s">
+      <c r="B27" s="296" t="s">
         <v>12</v>
       </c>
-      <c r="C27" s="296">
+      <c r="C27" s="301">
         <v>14500</v>
       </c>
       <c r="D27" s="52" t="s">
@@ -47596,9 +47596,9 @@
       <c r="AM27" s="258"/>
     </row>
     <row r="28" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A28" s="295"/>
-      <c r="B28" s="294"/>
-      <c r="C28" s="296"/>
+      <c r="A28" s="298"/>
+      <c r="B28" s="296"/>
+      <c r="C28" s="301"/>
       <c r="D28" s="52" t="s">
         <v>117</v>
       </c>
@@ -47699,13 +47699,13 @@
       <c r="AM28" s="259"/>
     </row>
     <row r="29" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A29" s="295" t="s">
+      <c r="A29" s="298" t="s">
         <v>368</v>
       </c>
-      <c r="B29" s="294" t="s">
+      <c r="B29" s="296" t="s">
         <v>12</v>
       </c>
-      <c r="C29" s="296">
+      <c r="C29" s="301">
         <v>24000</v>
       </c>
       <c r="D29" s="52" t="s">
@@ -47782,9 +47782,9 @@
       <c r="AM29" s="258"/>
     </row>
     <row r="30" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A30" s="295"/>
-      <c r="B30" s="294"/>
-      <c r="C30" s="296"/>
+      <c r="A30" s="298"/>
+      <c r="B30" s="296"/>
+      <c r="C30" s="301"/>
       <c r="D30" s="52" t="s">
         <v>117</v>
       </c>
@@ -47859,13 +47859,13 @@
       <c r="AM30" s="259"/>
     </row>
     <row r="31" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A31" s="295" t="s">
+      <c r="A31" s="298" t="s">
         <v>369</v>
       </c>
-      <c r="B31" s="294" t="s">
+      <c r="B31" s="296" t="s">
         <v>12</v>
       </c>
-      <c r="C31" s="296">
+      <c r="C31" s="301">
         <v>2800</v>
       </c>
       <c r="D31" s="52" t="s">
@@ -47924,9 +47924,9 @@
       <c r="AM31" s="258"/>
     </row>
     <row r="32" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A32" s="295"/>
-      <c r="B32" s="294"/>
-      <c r="C32" s="296"/>
+      <c r="A32" s="298"/>
+      <c r="B32" s="296"/>
+      <c r="C32" s="301"/>
       <c r="D32" s="52" t="s">
         <v>117</v>
       </c>
@@ -47983,13 +47983,13 @@
       <c r="AM32" s="259"/>
     </row>
     <row r="33" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A33" s="294" t="s">
+      <c r="A33" s="296" t="s">
         <v>370</v>
       </c>
-      <c r="B33" s="297">
+      <c r="B33" s="300">
         <v>0.25</v>
       </c>
-      <c r="C33" s="296">
+      <c r="C33" s="301">
         <v>13000</v>
       </c>
       <c r="D33" s="52" t="s">
@@ -48086,9 +48086,9 @@
       <c r="AM33" s="258"/>
     </row>
     <row r="34" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A34" s="294"/>
-      <c r="B34" s="297"/>
-      <c r="C34" s="297"/>
+      <c r="A34" s="296"/>
+      <c r="B34" s="300"/>
+      <c r="C34" s="300"/>
       <c r="D34" s="52" t="s">
         <v>117</v>
       </c>
@@ -48183,14 +48183,14 @@
       <c r="AM34" s="259"/>
     </row>
     <row r="35" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A35" s="294" t="s">
+      <c r="A35" s="296" t="s">
         <v>371</v>
       </c>
-      <c r="B35" s="321">
+      <c r="B35" s="318">
         <f>40/150</f>
         <v>0.26666666666666666</v>
       </c>
-      <c r="C35" s="296">
+      <c r="C35" s="301">
         <v>20000</v>
       </c>
       <c r="D35" s="52" t="s">
@@ -48275,9 +48275,9 @@
       <c r="AM35" s="258"/>
     </row>
     <row r="36" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A36" s="294"/>
-      <c r="B36" s="321"/>
-      <c r="C36" s="296"/>
+      <c r="A36" s="296"/>
+      <c r="B36" s="318"/>
+      <c r="C36" s="301"/>
       <c r="D36" s="52" t="s">
         <v>117</v>
       </c>
@@ -48403,13 +48403,13 @@
       <c r="AM37" s="51"/>
     </row>
     <row r="38" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A38" s="295" t="s">
+      <c r="A38" s="298" t="s">
         <v>372</v>
       </c>
-      <c r="B38" s="295" t="s">
+      <c r="B38" s="298" t="s">
         <v>12</v>
       </c>
-      <c r="C38" s="300">
+      <c r="C38" s="299">
         <v>27800</v>
       </c>
       <c r="D38" s="52" t="s">
@@ -48482,9 +48482,9 @@
       <c r="AM38" s="258"/>
     </row>
     <row r="39" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A39" s="295"/>
-      <c r="B39" s="295"/>
-      <c r="C39" s="300"/>
+      <c r="A39" s="298"/>
+      <c r="B39" s="298"/>
+      <c r="C39" s="299"/>
       <c r="D39" s="52" t="s">
         <v>117</v>
       </c>
@@ -48555,13 +48555,13 @@
       <c r="AM39" s="264"/>
     </row>
     <row r="40" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A40" s="294" t="s">
+      <c r="A40" s="296" t="s">
         <v>373</v>
       </c>
-      <c r="B40" s="295" t="s">
+      <c r="B40" s="298" t="s">
         <v>12</v>
       </c>
-      <c r="C40" s="296">
+      <c r="C40" s="301">
         <v>14500</v>
       </c>
       <c r="D40" s="52" t="s">
@@ -48664,9 +48664,9 @@
       <c r="AM40" s="258"/>
     </row>
     <row r="41" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A41" s="294"/>
-      <c r="B41" s="295"/>
-      <c r="C41" s="296"/>
+      <c r="A41" s="296"/>
+      <c r="B41" s="298"/>
+      <c r="C41" s="301"/>
       <c r="D41" s="52" t="s">
         <v>117</v>
       </c>
@@ -48767,13 +48767,13 @@
       <c r="AM41" s="259"/>
     </row>
     <row r="42" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A42" s="294" t="s">
+      <c r="A42" s="296" t="s">
         <v>374</v>
       </c>
-      <c r="B42" s="295" t="s">
+      <c r="B42" s="298" t="s">
         <v>12</v>
       </c>
-      <c r="C42" s="296">
+      <c r="C42" s="301">
         <v>22500</v>
       </c>
       <c r="D42" s="52" t="s">
@@ -48848,9 +48848,9 @@
       <c r="AM42" s="258"/>
     </row>
     <row r="43" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A43" s="294"/>
-      <c r="B43" s="295"/>
-      <c r="C43" s="296"/>
+      <c r="A43" s="296"/>
+      <c r="B43" s="298"/>
+      <c r="C43" s="301"/>
       <c r="D43" s="52" t="s">
         <v>117</v>
       </c>
@@ -48923,13 +48923,13 @@
       <c r="AM43" s="259"/>
     </row>
     <row r="44" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A44" s="294" t="s">
+      <c r="A44" s="296" t="s">
         <v>375</v>
       </c>
-      <c r="B44" s="295" t="s">
+      <c r="B44" s="298" t="s">
         <v>12</v>
       </c>
-      <c r="C44" s="296">
+      <c r="C44" s="301">
         <v>31500</v>
       </c>
       <c r="D44" s="52" t="s">
@@ -49016,9 +49016,9 @@
       <c r="AM44" s="258"/>
     </row>
     <row r="45" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A45" s="294"/>
-      <c r="B45" s="295"/>
-      <c r="C45" s="296"/>
+      <c r="A45" s="296"/>
+      <c r="B45" s="298"/>
+      <c r="C45" s="301"/>
       <c r="D45" s="52" t="s">
         <v>117</v>
       </c>
@@ -49146,13 +49146,13 @@
       <c r="AM46" s="51"/>
     </row>
     <row r="47" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A47" s="294" t="s">
+      <c r="A47" s="296" t="s">
         <v>376</v>
       </c>
-      <c r="B47" s="294" t="s">
+      <c r="B47" s="296" t="s">
         <v>12</v>
       </c>
-      <c r="C47" s="296">
+      <c r="C47" s="301">
         <v>3700</v>
       </c>
       <c r="D47" s="52" t="s">
@@ -49223,9 +49223,9 @@
       <c r="AM47" s="258"/>
     </row>
     <row r="48" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A48" s="294"/>
-      <c r="B48" s="294"/>
-      <c r="C48" s="296"/>
+      <c r="A48" s="296"/>
+      <c r="B48" s="296"/>
+      <c r="C48" s="301"/>
       <c r="D48" s="52" t="s">
         <v>117</v>
       </c>
@@ -49294,13 +49294,13 @@
       <c r="AM48" s="259"/>
     </row>
     <row r="49" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A49" s="294" t="s">
+      <c r="A49" s="296" t="s">
         <v>377</v>
       </c>
-      <c r="B49" s="294" t="s">
+      <c r="B49" s="296" t="s">
         <v>12</v>
       </c>
-      <c r="C49" s="296">
+      <c r="C49" s="301">
         <v>4000</v>
       </c>
       <c r="D49" s="52" t="s">
@@ -49371,9 +49371,9 @@
       <c r="AM49" s="258"/>
     </row>
     <row r="50" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A50" s="294"/>
-      <c r="B50" s="294"/>
-      <c r="C50" s="296"/>
+      <c r="A50" s="296"/>
+      <c r="B50" s="296"/>
+      <c r="C50" s="301"/>
       <c r="D50" s="52" t="s">
         <v>117</v>
       </c>
@@ -49570,13 +49570,13 @@
       <c r="AC55" s="4"/>
     </row>
     <row r="56" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A56" s="317" t="s">
+      <c r="A56" s="319" t="s">
         <v>379</v>
       </c>
-      <c r="B56" s="294" t="s">
+      <c r="B56" s="296" t="s">
         <v>12</v>
       </c>
-      <c r="C56" s="296">
+      <c r="C56" s="301">
         <f>+E56</f>
         <v>299.97278596475797</v>
       </c>
@@ -49648,9 +49648,9 @@
       <c r="AM56" s="258"/>
     </row>
     <row r="57" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A57" s="317"/>
-      <c r="B57" s="294"/>
-      <c r="C57" s="296"/>
+      <c r="A57" s="319"/>
+      <c r="B57" s="296"/>
+      <c r="C57" s="301"/>
       <c r="D57" s="52" t="s">
         <v>117</v>
       </c>
@@ -49719,13 +49719,13 @@
       <c r="AM57" s="259"/>
     </row>
     <row r="58" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A58" s="317" t="s">
+      <c r="A58" s="319" t="s">
         <v>380</v>
       </c>
-      <c r="B58" s="294" t="s">
+      <c r="B58" s="296" t="s">
         <v>12</v>
       </c>
-      <c r="C58" s="296">
+      <c r="C58" s="301">
         <f>+I58</f>
         <v>304.471539948898</v>
       </c>
@@ -49788,9 +49788,9 @@
       </c>
     </row>
     <row r="59" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A59" s="317"/>
-      <c r="B59" s="294"/>
-      <c r="C59" s="296"/>
+      <c r="A59" s="319"/>
+      <c r="B59" s="296"/>
+      <c r="C59" s="301"/>
       <c r="D59" s="52" t="s">
         <v>117</v>
       </c>
@@ -49850,13 +49850,13 @@
       </c>
     </row>
     <row r="60" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A60" s="317" t="s">
+      <c r="A60" s="319" t="s">
         <v>381</v>
       </c>
-      <c r="B60" s="294" t="s">
+      <c r="B60" s="296" t="s">
         <v>12</v>
       </c>
-      <c r="C60" s="296">
+      <c r="C60" s="301">
         <f>+K60</f>
         <v>411.48014529125697</v>
       </c>
@@ -49919,9 +49919,9 @@
       </c>
     </row>
     <row r="61" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A61" s="317"/>
-      <c r="B61" s="294"/>
-      <c r="C61" s="296"/>
+      <c r="A61" s="319"/>
+      <c r="B61" s="296"/>
+      <c r="C61" s="301"/>
       <c r="D61" s="52" t="s">
         <v>117</v>
       </c>
@@ -49981,13 +49981,13 @@
       </c>
     </row>
     <row r="62" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A62" s="317" t="s">
+      <c r="A62" s="319" t="s">
         <v>382</v>
       </c>
-      <c r="B62" s="294" t="s">
+      <c r="B62" s="296" t="s">
         <v>12</v>
       </c>
-      <c r="C62" s="296">
+      <c r="C62" s="301">
         <f>+E62</f>
         <v>14.1809996187</v>
       </c>
@@ -50065,9 +50065,9 @@
       <c r="AM62" s="258"/>
     </row>
     <row r="63" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A63" s="317"/>
-      <c r="B63" s="294"/>
-      <c r="C63" s="296"/>
+      <c r="A63" s="319"/>
+      <c r="B63" s="296"/>
+      <c r="C63" s="301"/>
       <c r="D63" s="52" t="s">
         <v>117</v>
       </c>
@@ -50142,13 +50142,13 @@
       <c r="AM63" s="264"/>
     </row>
     <row r="64" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A64" s="317" t="s">
+      <c r="A64" s="319" t="s">
         <v>383</v>
       </c>
-      <c r="B64" s="294" t="s">
+      <c r="B64" s="296" t="s">
         <v>12</v>
       </c>
-      <c r="C64" s="296">
+      <c r="C64" s="301">
         <f>+E64</f>
         <v>77.5139928551</v>
       </c>
@@ -50205,9 +50205,9 @@
       </c>
     </row>
     <row r="65" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A65" s="317"/>
-      <c r="B65" s="294"/>
-      <c r="C65" s="296"/>
+      <c r="A65" s="319"/>
+      <c r="B65" s="296"/>
+      <c r="C65" s="301"/>
       <c r="D65" s="139" t="s">
         <v>117</v>
       </c>
@@ -50261,13 +50261,13 @@
       </c>
     </row>
     <row r="66" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A66" s="317" t="s">
+      <c r="A66" s="319" t="s">
         <v>384</v>
       </c>
-      <c r="B66" s="294" t="s">
+      <c r="B66" s="296" t="s">
         <v>12</v>
       </c>
-      <c r="C66" s="296">
+      <c r="C66" s="301">
         <f>+E66</f>
         <v>103.654610475</v>
       </c>
@@ -50341,9 +50341,9 @@
       <c r="AM66" s="261"/>
     </row>
     <row r="67" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A67" s="317"/>
-      <c r="B67" s="294"/>
-      <c r="C67" s="296"/>
+      <c r="A67" s="319"/>
+      <c r="B67" s="296"/>
+      <c r="C67" s="301"/>
       <c r="D67" s="52" t="s">
         <v>117</v>
       </c>
@@ -50414,14 +50414,14 @@
       <c r="AM67" s="264"/>
     </row>
     <row r="68" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A68" s="318" t="s">
+      <c r="A68" s="320" t="s">
         <v>12</v>
       </c>
-      <c r="B68" s="297">
+      <c r="B68" s="300">
         <f>+E68</f>
         <v>0</v>
       </c>
-      <c r="C68" s="296">
+      <c r="C68" s="301">
         <v>0</v>
       </c>
       <c r="D68" s="52" t="s">
@@ -50464,9 +50464,9 @@
       <c r="AM68" s="258"/>
     </row>
     <row r="69" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A69" s="318"/>
-      <c r="B69" s="297"/>
-      <c r="C69" s="296"/>
+      <c r="A69" s="320"/>
+      <c r="B69" s="300"/>
+      <c r="C69" s="301"/>
       <c r="D69" s="52" t="s">
         <v>117</v>
       </c>
@@ -50540,13 +50540,13 @@
       <c r="AC70" s="4"/>
     </row>
     <row r="71" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A71" s="317" t="s">
+      <c r="A71" s="319" t="s">
         <v>385</v>
       </c>
-      <c r="B71" s="294" t="s">
+      <c r="B71" s="296" t="s">
         <v>12</v>
       </c>
-      <c r="C71" s="296">
+      <c r="C71" s="301">
         <f>+E71</f>
         <v>542.01797255752001</v>
       </c>
@@ -50624,9 +50624,9 @@
       <c r="AM71" s="258"/>
     </row>
     <row r="72" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A72" s="317"/>
-      <c r="B72" s="294"/>
-      <c r="C72" s="296"/>
+      <c r="A72" s="319"/>
+      <c r="B72" s="296"/>
+      <c r="C72" s="301"/>
       <c r="D72" s="52" t="s">
         <v>117</v>
       </c>
@@ -50701,13 +50701,13 @@
       <c r="AM72" s="259"/>
     </row>
     <row r="73" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A73" s="317" t="s">
+      <c r="A73" s="319" t="s">
         <v>386</v>
       </c>
-      <c r="B73" s="294" t="s">
+      <c r="B73" s="296" t="s">
         <v>12</v>
       </c>
-      <c r="C73" s="296">
+      <c r="C73" s="301">
         <f>+G73</f>
         <v>538.005973433431</v>
       </c>
@@ -50773,9 +50773,9 @@
       </c>
     </row>
     <row r="74" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A74" s="317"/>
-      <c r="B74" s="294"/>
-      <c r="C74" s="296"/>
+      <c r="A74" s="319"/>
+      <c r="B74" s="296"/>
+      <c r="C74" s="301"/>
       <c r="D74" s="52" t="s">
         <v>117</v>
       </c>
@@ -50838,13 +50838,13 @@
       </c>
     </row>
     <row r="75" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A75" s="317" t="s">
+      <c r="A75" s="319" t="s">
         <v>387</v>
       </c>
-      <c r="B75" s="294" t="s">
+      <c r="B75" s="296" t="s">
         <v>12</v>
       </c>
-      <c r="C75" s="296">
+      <c r="C75" s="301">
         <f>+H75</f>
         <v>540.81199952922702</v>
       </c>
@@ -50910,9 +50910,9 @@
       </c>
     </row>
     <row r="76" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A76" s="317"/>
-      <c r="B76" s="294"/>
-      <c r="C76" s="296"/>
+      <c r="A76" s="319"/>
+      <c r="B76" s="296"/>
+      <c r="C76" s="301"/>
       <c r="D76" s="52" t="s">
         <v>117</v>
       </c>
@@ -50975,13 +50975,13 @@
       </c>
     </row>
     <row r="77" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A77" s="317" t="s">
+      <c r="A77" s="319" t="s">
         <v>388</v>
       </c>
-      <c r="B77" s="294" t="s">
+      <c r="B77" s="296" t="s">
         <v>12</v>
       </c>
-      <c r="C77" s="296">
+      <c r="C77" s="301">
         <f>+E77</f>
         <v>70.703999727247606</v>
       </c>
@@ -51063,9 +51063,9 @@
       <c r="AM77" s="258"/>
     </row>
     <row r="78" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A78" s="317"/>
-      <c r="B78" s="294"/>
-      <c r="C78" s="296"/>
+      <c r="A78" s="319"/>
+      <c r="B78" s="296"/>
+      <c r="C78" s="301"/>
       <c r="D78" s="52" t="s">
         <v>117</v>
       </c>
@@ -51144,13 +51144,13 @@
       <c r="AM78" s="259"/>
     </row>
     <row r="79" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A79" s="317" t="s">
+      <c r="A79" s="319" t="s">
         <v>389</v>
       </c>
-      <c r="B79" s="294" t="s">
+      <c r="B79" s="296" t="s">
         <v>12</v>
       </c>
-      <c r="C79" s="296">
+      <c r="C79" s="301">
         <f>+E79</f>
         <v>487.78598291406001</v>
       </c>
@@ -51234,9 +51234,9 @@
       <c r="AM79" s="258"/>
     </row>
     <row r="80" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A80" s="317"/>
-      <c r="B80" s="294"/>
-      <c r="C80" s="296"/>
+      <c r="A80" s="319"/>
+      <c r="B80" s="296"/>
+      <c r="C80" s="301"/>
       <c r="D80" s="52" t="s">
         <v>117</v>
       </c>
@@ -51317,13 +51317,13 @@
       <c r="AM80" s="259"/>
     </row>
     <row r="81" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A81" s="317" t="s">
+      <c r="A81" s="319" t="s">
         <v>390</v>
       </c>
-      <c r="B81" s="294" t="s">
+      <c r="B81" s="296" t="s">
         <v>12</v>
       </c>
-      <c r="C81" s="296">
+      <c r="C81" s="301">
         <f>+E81</f>
         <v>881.48595333719004</v>
       </c>
@@ -51401,9 +51401,9 @@
       <c r="AM81" s="258"/>
     </row>
     <row r="82" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A82" s="317"/>
-      <c r="B82" s="294"/>
-      <c r="C82" s="296"/>
+      <c r="A82" s="319"/>
+      <c r="B82" s="296"/>
+      <c r="C82" s="301"/>
       <c r="D82" s="52" t="s">
         <v>117</v>
       </c>
@@ -51478,14 +51478,14 @@
       <c r="AM82" s="259"/>
     </row>
     <row r="83" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A83" s="318" t="s">
+      <c r="A83" s="320" t="s">
         <v>12</v>
       </c>
-      <c r="B83" s="297">
+      <c r="B83" s="300">
         <f>+E83</f>
         <v>0</v>
       </c>
-      <c r="C83" s="296">
+      <c r="C83" s="301">
         <v>0</v>
       </c>
       <c r="D83" s="52" t="s">
@@ -51528,9 +51528,9 @@
       <c r="AM83" s="258"/>
     </row>
     <row r="84" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A84" s="318"/>
-      <c r="B84" s="297"/>
-      <c r="C84" s="297"/>
+      <c r="A84" s="320"/>
+      <c r="B84" s="300"/>
+      <c r="C84" s="300"/>
       <c r="D84" s="52" t="s">
         <v>117</v>
       </c>
@@ -51571,14 +51571,14 @@
       <c r="AM84" s="259"/>
     </row>
     <row r="85" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A85" s="318" t="s">
+      <c r="A85" s="320" t="s">
         <v>12</v>
       </c>
-      <c r="B85" s="321">
+      <c r="B85" s="318">
         <f>+E85</f>
         <v>0</v>
       </c>
-      <c r="C85" s="296">
+      <c r="C85" s="301">
         <v>0</v>
       </c>
       <c r="D85" s="52" t="s">
@@ -51621,9 +51621,9 @@
       <c r="AM85" s="258"/>
     </row>
     <row r="86" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A86" s="318"/>
-      <c r="B86" s="321"/>
-      <c r="C86" s="296"/>
+      <c r="A86" s="320"/>
+      <c r="B86" s="318"/>
+      <c r="C86" s="301"/>
       <c r="D86" s="52" t="s">
         <v>117</v>
       </c>
@@ -51697,13 +51697,13 @@
       <c r="AC87" s="4"/>
     </row>
     <row r="88" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A88" s="320" t="s">
+      <c r="A88" s="321" t="s">
         <v>12</v>
       </c>
-      <c r="B88" s="295" t="s">
+      <c r="B88" s="298" t="s">
         <v>12</v>
       </c>
-      <c r="C88" s="300">
+      <c r="C88" s="299">
         <v>0</v>
       </c>
       <c r="D88" s="52" t="s">
@@ -51746,9 +51746,9 @@
       <c r="AM88" s="258"/>
     </row>
     <row r="89" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A89" s="320"/>
-      <c r="B89" s="295"/>
-      <c r="C89" s="300"/>
+      <c r="A89" s="321"/>
+      <c r="B89" s="298"/>
+      <c r="C89" s="299"/>
       <c r="D89" s="52" t="s">
         <v>117</v>
       </c>
@@ -51789,13 +51789,13 @@
       <c r="AM89" s="264"/>
     </row>
     <row r="90" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A90" s="317" t="s">
+      <c r="A90" s="319" t="s">
         <v>391</v>
       </c>
-      <c r="B90" s="295" t="s">
+      <c r="B90" s="298" t="s">
         <v>12</v>
       </c>
-      <c r="C90" s="296">
+      <c r="C90" s="301">
         <f>+E90</f>
         <v>2314.1137144060499</v>
       </c>
@@ -51849,9 +51849,9 @@
       </c>
     </row>
     <row r="91" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A91" s="317"/>
-      <c r="B91" s="295"/>
-      <c r="C91" s="296"/>
+      <c r="A91" s="319"/>
+      <c r="B91" s="298"/>
+      <c r="C91" s="301"/>
       <c r="D91" s="52" t="s">
         <v>117</v>
       </c>
@@ -51902,13 +51902,13 @@
       </c>
     </row>
     <row r="92" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A92" s="317" t="s">
+      <c r="A92" s="319" t="s">
         <v>392</v>
       </c>
-      <c r="B92" s="295" t="s">
+      <c r="B92" s="298" t="s">
         <v>12</v>
       </c>
-      <c r="C92" s="296">
+      <c r="C92" s="301">
         <f>+E92</f>
         <v>2309.2137610162299</v>
       </c>
@@ -51984,9 +51984,9 @@
       <c r="AM92" s="258"/>
     </row>
     <row r="93" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A93" s="317"/>
-      <c r="B93" s="295"/>
-      <c r="C93" s="296"/>
+      <c r="A93" s="319"/>
+      <c r="B93" s="298"/>
+      <c r="C93" s="301"/>
       <c r="D93" s="52" t="s">
         <v>117</v>
       </c>
@@ -52059,13 +52059,13 @@
       <c r="AM93" s="259"/>
     </row>
     <row r="94" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A94" s="317" t="s">
+      <c r="A94" s="319" t="s">
         <v>393</v>
       </c>
-      <c r="B94" s="295" t="s">
+      <c r="B94" s="298" t="s">
         <v>12</v>
       </c>
-      <c r="C94" s="296">
+      <c r="C94" s="301">
         <f>+E94</f>
         <v>2588.6587743893901</v>
       </c>
@@ -52139,9 +52139,9 @@
       <c r="AM94" s="258"/>
     </row>
     <row r="95" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A95" s="317"/>
-      <c r="B95" s="295"/>
-      <c r="C95" s="296"/>
+      <c r="A95" s="319"/>
+      <c r="B95" s="298"/>
+      <c r="C95" s="301"/>
       <c r="D95" s="52" t="s">
         <v>117</v>
       </c>
@@ -52245,11 +52245,11 @@
       <c r="AC96" s="4"/>
     </row>
     <row r="97" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A97" s="318"/>
-      <c r="B97" s="294" t="s">
+      <c r="A97" s="320"/>
+      <c r="B97" s="296" t="s">
         <v>12</v>
       </c>
-      <c r="C97" s="296">
+      <c r="C97" s="301">
         <f>+E97</f>
         <v>0</v>
       </c>
@@ -52293,9 +52293,9 @@
       <c r="AM97" s="258"/>
     </row>
     <row r="98" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A98" s="318"/>
-      <c r="B98" s="294"/>
-      <c r="C98" s="296"/>
+      <c r="A98" s="320"/>
+      <c r="B98" s="296"/>
+      <c r="C98" s="301"/>
       <c r="D98" s="52" t="s">
         <v>117</v>
       </c>
@@ -52336,11 +52336,11 @@
       <c r="AM98" s="259"/>
     </row>
     <row r="99" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A99" s="318"/>
-      <c r="B99" s="294" t="s">
+      <c r="A99" s="320"/>
+      <c r="B99" s="296" t="s">
         <v>12</v>
       </c>
-      <c r="C99" s="319">
+      <c r="C99" s="322">
         <f>+E99</f>
         <v>0</v>
       </c>
@@ -52384,9 +52384,9 @@
       <c r="AM99" s="258"/>
     </row>
     <row r="100" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A100" s="318"/>
-      <c r="B100" s="294"/>
-      <c r="C100" s="319"/>
+      <c r="A100" s="320"/>
+      <c r="B100" s="296"/>
+      <c r="C100" s="322"/>
       <c r="D100" s="52" t="s">
         <v>117</v>
       </c>
@@ -52555,13 +52555,13 @@
       <c r="AC106" s="277"/>
     </row>
     <row r="107" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A107" s="317" t="s">
+      <c r="A107" s="319" t="s">
         <v>395</v>
       </c>
-      <c r="B107" s="294" t="s">
+      <c r="B107" s="296" t="s">
         <v>12</v>
       </c>
-      <c r="C107" s="296">
+      <c r="C107" s="301">
         <f>+E107</f>
         <v>5.8600034000000001</v>
       </c>
@@ -52609,9 +52609,9 @@
       <c r="S107" s="258"/>
     </row>
     <row r="108" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A108" s="317"/>
-      <c r="B108" s="294"/>
-      <c r="C108" s="296"/>
+      <c r="A108" s="319"/>
+      <c r="B108" s="296"/>
+      <c r="C108" s="301"/>
       <c r="D108" s="52" t="s">
         <v>117</v>
       </c>
@@ -52656,13 +52656,13 @@
       <c r="S108" s="259"/>
     </row>
     <row r="109" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A109" s="317" t="s">
+      <c r="A109" s="319" t="s">
         <v>396</v>
       </c>
-      <c r="B109" s="294" t="s">
+      <c r="B109" s="296" t="s">
         <v>12</v>
       </c>
-      <c r="C109" s="296">
+      <c r="C109" s="301">
         <f>+E109</f>
         <v>5.86</v>
       </c>
@@ -52712,9 +52712,9 @@
       <c r="S109" s="258"/>
     </row>
     <row r="110" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A110" s="317"/>
-      <c r="B110" s="294"/>
-      <c r="C110" s="296"/>
+      <c r="A110" s="319"/>
+      <c r="B110" s="296"/>
+      <c r="C110" s="301"/>
       <c r="D110" s="52" t="s">
         <v>117</v>
       </c>
@@ -52761,13 +52761,13 @@
       <c r="S110" s="264"/>
     </row>
     <row r="111" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A111" s="317" t="s">
+      <c r="A111" s="319" t="s">
         <v>397</v>
       </c>
-      <c r="B111" s="294" t="s">
+      <c r="B111" s="296" t="s">
         <v>12</v>
       </c>
-      <c r="C111" s="296">
+      <c r="C111" s="301">
         <f>+E111</f>
         <v>7.2400155000000002</v>
       </c>
@@ -52843,9 +52843,9 @@
       <c r="AM111" s="258"/>
     </row>
     <row r="112" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A112" s="317"/>
-      <c r="B112" s="294"/>
-      <c r="C112" s="296"/>
+      <c r="A112" s="319"/>
+      <c r="B112" s="296"/>
+      <c r="C112" s="301"/>
       <c r="D112" s="52" t="s">
         <v>117</v>
       </c>
@@ -52918,13 +52918,13 @@
       <c r="AM112" s="259"/>
     </row>
     <row r="113" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A113" s="317" t="s">
+      <c r="A113" s="319" t="s">
         <v>398</v>
       </c>
-      <c r="B113" s="294" t="s">
+      <c r="B113" s="296" t="s">
         <v>12</v>
       </c>
-      <c r="C113" s="296">
+      <c r="C113" s="301">
         <f>+E113</f>
         <v>0</v>
       </c>
@@ -52970,9 +52970,9 @@
       <c r="AM113" s="258"/>
     </row>
     <row r="114" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A114" s="317"/>
-      <c r="B114" s="294"/>
-      <c r="C114" s="296"/>
+      <c r="A114" s="319"/>
+      <c r="B114" s="296"/>
+      <c r="C114" s="301"/>
       <c r="D114" s="52" t="s">
         <v>117</v>
       </c>
@@ -53015,13 +53015,13 @@
       <c r="AM114" s="264"/>
     </row>
     <row r="115" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A115" s="317" t="s">
+      <c r="A115" s="319" t="s">
         <v>399</v>
       </c>
-      <c r="B115" s="294" t="s">
+      <c r="B115" s="296" t="s">
         <v>12</v>
       </c>
-      <c r="C115" s="296">
+      <c r="C115" s="301">
         <f>+E115</f>
         <v>0</v>
       </c>
@@ -53067,9 +53067,9 @@
       <c r="AM115" s="258"/>
     </row>
     <row r="116" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A116" s="317"/>
-      <c r="B116" s="294"/>
-      <c r="C116" s="296"/>
+      <c r="A116" s="319"/>
+      <c r="B116" s="296"/>
+      <c r="C116" s="301"/>
       <c r="D116" s="52" t="s">
         <v>117</v>
       </c>
@@ -53112,13 +53112,13 @@
       <c r="AM116" s="259"/>
     </row>
     <row r="117" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A117" s="317" t="s">
+      <c r="A117" s="319" t="s">
         <v>400</v>
       </c>
-      <c r="B117" s="294" t="s">
+      <c r="B117" s="296" t="s">
         <v>12</v>
       </c>
-      <c r="C117" s="296">
+      <c r="C117" s="301">
         <f>+E117</f>
         <v>0</v>
       </c>
@@ -53164,9 +53164,9 @@
       <c r="AM117" s="261"/>
     </row>
     <row r="118" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A118" s="317"/>
-      <c r="B118" s="294"/>
-      <c r="C118" s="296"/>
+      <c r="A118" s="319"/>
+      <c r="B118" s="296"/>
+      <c r="C118" s="301"/>
       <c r="D118" s="52" t="s">
         <v>117</v>
       </c>
@@ -53209,14 +53209,14 @@
       <c r="AM118" s="264"/>
     </row>
     <row r="119" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A119" s="318" t="s">
+      <c r="A119" s="320" t="s">
         <v>12</v>
       </c>
-      <c r="B119" s="297">
+      <c r="B119" s="300">
         <f>+E119</f>
         <v>0</v>
       </c>
-      <c r="C119" s="296">
+      <c r="C119" s="301">
         <v>0</v>
       </c>
       <c r="D119" s="52" t="s">
@@ -53259,9 +53259,9 @@
       <c r="AM119" s="258"/>
     </row>
     <row r="120" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A120" s="318"/>
-      <c r="B120" s="297"/>
-      <c r="C120" s="296"/>
+      <c r="A120" s="320"/>
+      <c r="B120" s="300"/>
+      <c r="C120" s="301"/>
       <c r="D120" s="52" t="s">
         <v>117</v>
       </c>
@@ -53335,13 +53335,13 @@
       <c r="AC121" s="277"/>
     </row>
     <row r="122" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A122" s="317" t="s">
+      <c r="A122" s="319" t="s">
         <v>401</v>
       </c>
-      <c r="B122" s="294" t="s">
+      <c r="B122" s="296" t="s">
         <v>12</v>
       </c>
-      <c r="C122" s="296">
+      <c r="C122" s="301">
         <f>+E122</f>
         <v>4.2299990999999997</v>
       </c>
@@ -53411,9 +53411,9 @@
       <c r="AM122" s="258"/>
     </row>
     <row r="123" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A123" s="317"/>
-      <c r="B123" s="294"/>
-      <c r="C123" s="296"/>
+      <c r="A123" s="319"/>
+      <c r="B123" s="296"/>
+      <c r="C123" s="301"/>
       <c r="D123" s="52" t="s">
         <v>117</v>
       </c>
@@ -53480,13 +53480,13 @@
       <c r="AM123" s="259"/>
     </row>
     <row r="124" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A124" s="317" t="s">
+      <c r="A124" s="319" t="s">
         <v>402</v>
       </c>
-      <c r="B124" s="294" t="s">
+      <c r="B124" s="296" t="s">
         <v>12</v>
       </c>
-      <c r="C124" s="296">
+      <c r="C124" s="301">
         <f>+E124</f>
         <v>5.3000118000000001</v>
       </c>
@@ -53558,9 +53558,9 @@
       <c r="AM124" s="258"/>
     </row>
     <row r="125" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A125" s="317"/>
-      <c r="B125" s="294"/>
-      <c r="C125" s="296"/>
+      <c r="A125" s="319"/>
+      <c r="B125" s="296"/>
+      <c r="C125" s="301"/>
       <c r="D125" s="52" t="s">
         <v>117</v>
       </c>
@@ -53629,13 +53629,13 @@
       <c r="AM125" s="259"/>
     </row>
     <row r="126" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A126" s="317" t="s">
+      <c r="A126" s="319" t="s">
         <v>403</v>
       </c>
-      <c r="B126" s="294" t="s">
+      <c r="B126" s="296" t="s">
         <v>12</v>
       </c>
-      <c r="C126" s="296">
+      <c r="C126" s="301">
         <f>+E126</f>
         <v>5.3000049000000002</v>
       </c>
@@ -53709,9 +53709,9 @@
       <c r="AM126" s="258"/>
     </row>
     <row r="127" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A127" s="317"/>
-      <c r="B127" s="294"/>
-      <c r="C127" s="296"/>
+      <c r="A127" s="319"/>
+      <c r="B127" s="296"/>
+      <c r="C127" s="301"/>
       <c r="D127" s="52" t="s">
         <v>117</v>
       </c>
@@ -53782,13 +53782,13 @@
       <c r="AM127" s="259"/>
     </row>
     <row r="128" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A128" s="317" t="s">
+      <c r="A128" s="319" t="s">
         <v>404</v>
       </c>
-      <c r="B128" s="294" t="s">
+      <c r="B128" s="296" t="s">
         <v>12</v>
       </c>
-      <c r="C128" s="296">
+      <c r="C128" s="301">
         <f>+E128</f>
         <v>0</v>
       </c>
@@ -53834,9 +53834,9 @@
       <c r="AM128" s="258"/>
     </row>
     <row r="129" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A129" s="317"/>
-      <c r="B129" s="294"/>
-      <c r="C129" s="296"/>
+      <c r="A129" s="319"/>
+      <c r="B129" s="296"/>
+      <c r="C129" s="301"/>
       <c r="D129" s="52" t="s">
         <v>117</v>
       </c>
@@ -53879,13 +53879,13 @@
       <c r="AM129" s="259"/>
     </row>
     <row r="130" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A130" s="317" t="s">
+      <c r="A130" s="319" t="s">
         <v>405</v>
       </c>
-      <c r="B130" s="294" t="s">
+      <c r="B130" s="296" t="s">
         <v>12</v>
       </c>
-      <c r="C130" s="296">
+      <c r="C130" s="301">
         <f>+E130</f>
         <v>0</v>
       </c>
@@ -53931,9 +53931,9 @@
       <c r="AM130" s="258"/>
     </row>
     <row r="131" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A131" s="317"/>
-      <c r="B131" s="294"/>
-      <c r="C131" s="296"/>
+      <c r="A131" s="319"/>
+      <c r="B131" s="296"/>
+      <c r="C131" s="301"/>
       <c r="D131" s="52" t="s">
         <v>117</v>
       </c>
@@ -53976,13 +53976,13 @@
       <c r="AM131" s="259"/>
     </row>
     <row r="132" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A132" s="317" t="s">
+      <c r="A132" s="319" t="s">
         <v>406</v>
       </c>
-      <c r="B132" s="294" t="s">
+      <c r="B132" s="296" t="s">
         <v>12</v>
       </c>
-      <c r="C132" s="296">
+      <c r="C132" s="301">
         <f>+E132</f>
         <v>0</v>
       </c>
@@ -54028,9 +54028,9 @@
       <c r="AM132" s="258"/>
     </row>
     <row r="133" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A133" s="317"/>
-      <c r="B133" s="294"/>
-      <c r="C133" s="296"/>
+      <c r="A133" s="319"/>
+      <c r="B133" s="296"/>
+      <c r="C133" s="301"/>
       <c r="D133" s="52" t="s">
         <v>117</v>
       </c>
@@ -54073,14 +54073,14 @@
       <c r="AM133" s="259"/>
     </row>
     <row r="134" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A134" s="318" t="s">
+      <c r="A134" s="320" t="s">
         <v>12</v>
       </c>
-      <c r="B134" s="297">
+      <c r="B134" s="300">
         <f>+E134</f>
         <v>0</v>
       </c>
-      <c r="C134" s="296">
+      <c r="C134" s="301">
         <v>0</v>
       </c>
       <c r="D134" s="278" t="s">
@@ -54123,9 +54123,9 @@
       <c r="AM134" s="258"/>
     </row>
     <row r="135" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A135" s="318"/>
-      <c r="B135" s="297"/>
-      <c r="C135" s="296"/>
+      <c r="A135" s="320"/>
+      <c r="B135" s="300"/>
+      <c r="C135" s="301"/>
       <c r="D135" s="52" t="s">
         <v>117</v>
       </c>
@@ -54166,14 +54166,14 @@
       <c r="AM135" s="259"/>
     </row>
     <row r="136" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A136" s="318" t="s">
+      <c r="A136" s="320" t="s">
         <v>12</v>
       </c>
-      <c r="B136" s="321">
+      <c r="B136" s="318">
         <f>+E136</f>
         <v>0</v>
       </c>
-      <c r="C136" s="296">
+      <c r="C136" s="301">
         <v>0</v>
       </c>
       <c r="D136" s="52" t="s">
@@ -54216,9 +54216,9 @@
       <c r="AM136" s="258"/>
     </row>
     <row r="137" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A137" s="318"/>
-      <c r="B137" s="321"/>
-      <c r="C137" s="296"/>
+      <c r="A137" s="320"/>
+      <c r="B137" s="318"/>
+      <c r="C137" s="301"/>
       <c r="D137" s="52" t="s">
         <v>117</v>
       </c>
@@ -54292,13 +54292,13 @@
       <c r="AC138" s="277"/>
     </row>
     <row r="139" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A139" s="320" t="s">
+      <c r="A139" s="321" t="s">
         <v>12</v>
       </c>
-      <c r="B139" s="295" t="s">
+      <c r="B139" s="298" t="s">
         <v>12</v>
       </c>
-      <c r="C139" s="296">
+      <c r="C139" s="301">
         <v>0</v>
       </c>
       <c r="D139" s="52" t="s">
@@ -54341,9 +54341,9 @@
       <c r="AM139" s="258"/>
     </row>
     <row r="140" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A140" s="320"/>
-      <c r="B140" s="295"/>
-      <c r="C140" s="296"/>
+      <c r="A140" s="321"/>
+      <c r="B140" s="298"/>
+      <c r="C140" s="301"/>
       <c r="D140" s="226" t="s">
         <v>117</v>
       </c>
@@ -54384,13 +54384,13 @@
       <c r="AM140" s="264"/>
     </row>
     <row r="141" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A141" s="317" t="s">
+      <c r="A141" s="319" t="s">
         <v>407</v>
       </c>
-      <c r="B141" s="295" t="s">
+      <c r="B141" s="298" t="s">
         <v>12</v>
       </c>
-      <c r="C141" s="296">
+      <c r="C141" s="301">
         <f>+E141</f>
         <v>3.8630089000000001</v>
       </c>
@@ -54416,9 +54416,9 @@
       <c r="S141" s="258"/>
     </row>
     <row r="142" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A142" s="317"/>
-      <c r="B142" s="295"/>
-      <c r="C142" s="296"/>
+      <c r="A142" s="319"/>
+      <c r="B142" s="298"/>
+      <c r="C142" s="301"/>
       <c r="D142" s="52" t="s">
         <v>117</v>
       </c>
@@ -54441,13 +54441,13 @@
       <c r="S142" s="259"/>
     </row>
     <row r="143" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A143" s="317" t="s">
+      <c r="A143" s="319" t="s">
         <v>408</v>
       </c>
-      <c r="B143" s="295" t="s">
+      <c r="B143" s="298" t="s">
         <v>12</v>
       </c>
-      <c r="C143" s="296">
+      <c r="C143" s="301">
         <f>+E143</f>
         <v>3.8630089600000002</v>
       </c>
@@ -54493,9 +54493,9 @@
       <c r="AM143" s="258"/>
     </row>
     <row r="144" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A144" s="317"/>
-      <c r="B144" s="295"/>
-      <c r="C144" s="296"/>
+      <c r="A144" s="319"/>
+      <c r="B144" s="298"/>
+      <c r="C144" s="301"/>
       <c r="D144" s="52" t="s">
         <v>117</v>
       </c>
@@ -54538,13 +54538,13 @@
       <c r="AM144" s="259"/>
     </row>
     <row r="145" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A145" s="317" t="s">
+      <c r="A145" s="319" t="s">
         <v>409</v>
       </c>
-      <c r="B145" s="295" t="s">
+      <c r="B145" s="298" t="s">
         <v>12</v>
       </c>
-      <c r="C145" s="296">
+      <c r="C145" s="301">
         <f>+E145</f>
         <v>7.0260103999999997</v>
       </c>
@@ -54614,9 +54614,9 @@
       <c r="AM145" s="258"/>
     </row>
     <row r="146" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A146" s="317"/>
-      <c r="B146" s="295"/>
-      <c r="C146" s="296"/>
+      <c r="A146" s="319"/>
+      <c r="B146" s="298"/>
+      <c r="C146" s="301"/>
       <c r="D146" s="52" t="s">
         <v>117</v>
       </c>
@@ -54716,11 +54716,11 @@
       <c r="AC147" s="277"/>
     </row>
     <row r="148" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A148" s="318"/>
-      <c r="B148" s="294" t="s">
+      <c r="A148" s="320"/>
+      <c r="B148" s="296" t="s">
         <v>12</v>
       </c>
-      <c r="C148" s="296">
+      <c r="C148" s="301">
         <f>+E148</f>
         <v>0</v>
       </c>
@@ -54764,9 +54764,9 @@
       <c r="AM148" s="258"/>
     </row>
     <row r="149" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A149" s="318"/>
-      <c r="B149" s="294"/>
-      <c r="C149" s="296"/>
+      <c r="A149" s="320"/>
+      <c r="B149" s="296"/>
+      <c r="C149" s="301"/>
       <c r="D149" s="52" t="s">
         <v>117</v>
       </c>
@@ -54807,11 +54807,11 @@
       <c r="AM149" s="259"/>
     </row>
     <row r="150" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A150" s="318"/>
-      <c r="B150" s="294" t="s">
+      <c r="A150" s="320"/>
+      <c r="B150" s="296" t="s">
         <v>12</v>
       </c>
-      <c r="C150" s="319">
+      <c r="C150" s="322">
         <f>+E150</f>
         <v>0</v>
       </c>
@@ -54855,9 +54855,9 @@
       <c r="AM150" s="258"/>
     </row>
     <row r="151" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A151" s="318"/>
-      <c r="B151" s="294"/>
-      <c r="C151" s="319"/>
+      <c r="A151" s="320"/>
+      <c r="B151" s="296"/>
+      <c r="C151" s="322"/>
       <c r="D151" s="52" t="s">
         <v>117</v>
       </c>
@@ -54899,6 +54899,186 @@
     </row>
   </sheetData>
   <mergeCells count="189">
+    <mergeCell ref="A145:A146"/>
+    <mergeCell ref="B145:B146"/>
+    <mergeCell ref="C145:C146"/>
+    <mergeCell ref="A148:A149"/>
+    <mergeCell ref="B148:B149"/>
+    <mergeCell ref="C148:C149"/>
+    <mergeCell ref="A150:A151"/>
+    <mergeCell ref="B150:B151"/>
+    <mergeCell ref="C150:C151"/>
+    <mergeCell ref="A139:A140"/>
+    <mergeCell ref="B139:B140"/>
+    <mergeCell ref="C139:C140"/>
+    <mergeCell ref="A141:A142"/>
+    <mergeCell ref="B141:B142"/>
+    <mergeCell ref="C141:C142"/>
+    <mergeCell ref="A143:A144"/>
+    <mergeCell ref="B143:B144"/>
+    <mergeCell ref="C143:C144"/>
+    <mergeCell ref="A132:A133"/>
+    <mergeCell ref="B132:B133"/>
+    <mergeCell ref="C132:C133"/>
+    <mergeCell ref="A134:A135"/>
+    <mergeCell ref="B134:B135"/>
+    <mergeCell ref="C134:C135"/>
+    <mergeCell ref="A136:A137"/>
+    <mergeCell ref="B136:B137"/>
+    <mergeCell ref="C136:C137"/>
+    <mergeCell ref="A126:A127"/>
+    <mergeCell ref="B126:B127"/>
+    <mergeCell ref="C126:C127"/>
+    <mergeCell ref="A128:A129"/>
+    <mergeCell ref="B128:B129"/>
+    <mergeCell ref="C128:C129"/>
+    <mergeCell ref="A130:A131"/>
+    <mergeCell ref="B130:B131"/>
+    <mergeCell ref="C130:C131"/>
+    <mergeCell ref="A119:A120"/>
+    <mergeCell ref="B119:B120"/>
+    <mergeCell ref="C119:C120"/>
+    <mergeCell ref="A122:A123"/>
+    <mergeCell ref="B122:B123"/>
+    <mergeCell ref="C122:C123"/>
+    <mergeCell ref="A124:A125"/>
+    <mergeCell ref="B124:B125"/>
+    <mergeCell ref="C124:C125"/>
+    <mergeCell ref="A113:A114"/>
+    <mergeCell ref="B113:B114"/>
+    <mergeCell ref="C113:C114"/>
+    <mergeCell ref="A115:A116"/>
+    <mergeCell ref="B115:B116"/>
+    <mergeCell ref="C115:C116"/>
+    <mergeCell ref="A117:A118"/>
+    <mergeCell ref="B117:B118"/>
+    <mergeCell ref="C117:C118"/>
+    <mergeCell ref="A107:A108"/>
+    <mergeCell ref="B107:B108"/>
+    <mergeCell ref="C107:C108"/>
+    <mergeCell ref="A109:A110"/>
+    <mergeCell ref="B109:B110"/>
+    <mergeCell ref="C109:C110"/>
+    <mergeCell ref="A111:A112"/>
+    <mergeCell ref="B111:B112"/>
+    <mergeCell ref="C111:C112"/>
+    <mergeCell ref="A94:A95"/>
+    <mergeCell ref="B94:B95"/>
+    <mergeCell ref="C94:C95"/>
+    <mergeCell ref="A97:A98"/>
+    <mergeCell ref="B97:B98"/>
+    <mergeCell ref="C97:C98"/>
+    <mergeCell ref="A99:A100"/>
+    <mergeCell ref="B99:B100"/>
+    <mergeCell ref="C99:C100"/>
+    <mergeCell ref="A88:A89"/>
+    <mergeCell ref="B88:B89"/>
+    <mergeCell ref="C88:C89"/>
+    <mergeCell ref="A90:A91"/>
+    <mergeCell ref="B90:B91"/>
+    <mergeCell ref="C90:C91"/>
+    <mergeCell ref="A92:A93"/>
+    <mergeCell ref="B92:B93"/>
+    <mergeCell ref="C92:C93"/>
+    <mergeCell ref="A81:A82"/>
+    <mergeCell ref="B81:B82"/>
+    <mergeCell ref="C81:C82"/>
+    <mergeCell ref="A83:A84"/>
+    <mergeCell ref="B83:B84"/>
+    <mergeCell ref="C83:C84"/>
+    <mergeCell ref="A85:A86"/>
+    <mergeCell ref="B85:B86"/>
+    <mergeCell ref="C85:C86"/>
+    <mergeCell ref="A75:A76"/>
+    <mergeCell ref="B75:B76"/>
+    <mergeCell ref="C75:C76"/>
+    <mergeCell ref="A77:A78"/>
+    <mergeCell ref="B77:B78"/>
+    <mergeCell ref="C77:C78"/>
+    <mergeCell ref="A79:A80"/>
+    <mergeCell ref="B79:B80"/>
+    <mergeCell ref="C79:C80"/>
+    <mergeCell ref="A68:A69"/>
+    <mergeCell ref="B68:B69"/>
+    <mergeCell ref="C68:C69"/>
+    <mergeCell ref="A71:A72"/>
+    <mergeCell ref="B71:B72"/>
+    <mergeCell ref="C71:C72"/>
+    <mergeCell ref="A73:A74"/>
+    <mergeCell ref="B73:B74"/>
+    <mergeCell ref="C73:C74"/>
+    <mergeCell ref="A62:A63"/>
+    <mergeCell ref="B62:B63"/>
+    <mergeCell ref="C62:C63"/>
+    <mergeCell ref="A64:A65"/>
+    <mergeCell ref="B64:B65"/>
+    <mergeCell ref="C64:C65"/>
+    <mergeCell ref="A66:A67"/>
+    <mergeCell ref="B66:B67"/>
+    <mergeCell ref="C66:C67"/>
+    <mergeCell ref="A56:A57"/>
+    <mergeCell ref="B56:B57"/>
+    <mergeCell ref="C56:C57"/>
+    <mergeCell ref="A58:A59"/>
+    <mergeCell ref="B58:B59"/>
+    <mergeCell ref="C58:C59"/>
+    <mergeCell ref="A60:A61"/>
+    <mergeCell ref="B60:B61"/>
+    <mergeCell ref="C60:C61"/>
+    <mergeCell ref="A44:A45"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="C47:C48"/>
+    <mergeCell ref="A49:A50"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="C49:C50"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="A40:A41"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="C40:C41"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C16:C17"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="C6:C7"/>
@@ -54908,186 +55088,6 @@
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="B10:B11"/>
     <mergeCell ref="C10:C11"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="A35:A36"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="C38:C39"/>
-    <mergeCell ref="A40:A41"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="C40:C41"/>
-    <mergeCell ref="A42:A43"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="C42:C43"/>
-    <mergeCell ref="A44:A45"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="A47:A48"/>
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="C47:C48"/>
-    <mergeCell ref="A49:A50"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="C49:C50"/>
-    <mergeCell ref="A56:A57"/>
-    <mergeCell ref="B56:B57"/>
-    <mergeCell ref="C56:C57"/>
-    <mergeCell ref="A58:A59"/>
-    <mergeCell ref="B58:B59"/>
-    <mergeCell ref="C58:C59"/>
-    <mergeCell ref="A60:A61"/>
-    <mergeCell ref="B60:B61"/>
-    <mergeCell ref="C60:C61"/>
-    <mergeCell ref="A62:A63"/>
-    <mergeCell ref="B62:B63"/>
-    <mergeCell ref="C62:C63"/>
-    <mergeCell ref="A64:A65"/>
-    <mergeCell ref="B64:B65"/>
-    <mergeCell ref="C64:C65"/>
-    <mergeCell ref="A66:A67"/>
-    <mergeCell ref="B66:B67"/>
-    <mergeCell ref="C66:C67"/>
-    <mergeCell ref="A68:A69"/>
-    <mergeCell ref="B68:B69"/>
-    <mergeCell ref="C68:C69"/>
-    <mergeCell ref="A71:A72"/>
-    <mergeCell ref="B71:B72"/>
-    <mergeCell ref="C71:C72"/>
-    <mergeCell ref="A73:A74"/>
-    <mergeCell ref="B73:B74"/>
-    <mergeCell ref="C73:C74"/>
-    <mergeCell ref="A75:A76"/>
-    <mergeCell ref="B75:B76"/>
-    <mergeCell ref="C75:C76"/>
-    <mergeCell ref="A77:A78"/>
-    <mergeCell ref="B77:B78"/>
-    <mergeCell ref="C77:C78"/>
-    <mergeCell ref="A79:A80"/>
-    <mergeCell ref="B79:B80"/>
-    <mergeCell ref="C79:C80"/>
-    <mergeCell ref="A81:A82"/>
-    <mergeCell ref="B81:B82"/>
-    <mergeCell ref="C81:C82"/>
-    <mergeCell ref="A83:A84"/>
-    <mergeCell ref="B83:B84"/>
-    <mergeCell ref="C83:C84"/>
-    <mergeCell ref="A85:A86"/>
-    <mergeCell ref="B85:B86"/>
-    <mergeCell ref="C85:C86"/>
-    <mergeCell ref="A88:A89"/>
-    <mergeCell ref="B88:B89"/>
-    <mergeCell ref="C88:C89"/>
-    <mergeCell ref="A90:A91"/>
-    <mergeCell ref="B90:B91"/>
-    <mergeCell ref="C90:C91"/>
-    <mergeCell ref="A92:A93"/>
-    <mergeCell ref="B92:B93"/>
-    <mergeCell ref="C92:C93"/>
-    <mergeCell ref="A94:A95"/>
-    <mergeCell ref="B94:B95"/>
-    <mergeCell ref="C94:C95"/>
-    <mergeCell ref="A97:A98"/>
-    <mergeCell ref="B97:B98"/>
-    <mergeCell ref="C97:C98"/>
-    <mergeCell ref="A99:A100"/>
-    <mergeCell ref="B99:B100"/>
-    <mergeCell ref="C99:C100"/>
-    <mergeCell ref="A107:A108"/>
-    <mergeCell ref="B107:B108"/>
-    <mergeCell ref="C107:C108"/>
-    <mergeCell ref="A109:A110"/>
-    <mergeCell ref="B109:B110"/>
-    <mergeCell ref="C109:C110"/>
-    <mergeCell ref="A111:A112"/>
-    <mergeCell ref="B111:B112"/>
-    <mergeCell ref="C111:C112"/>
-    <mergeCell ref="A113:A114"/>
-    <mergeCell ref="B113:B114"/>
-    <mergeCell ref="C113:C114"/>
-    <mergeCell ref="A115:A116"/>
-    <mergeCell ref="B115:B116"/>
-    <mergeCell ref="C115:C116"/>
-    <mergeCell ref="A117:A118"/>
-    <mergeCell ref="B117:B118"/>
-    <mergeCell ref="C117:C118"/>
-    <mergeCell ref="A119:A120"/>
-    <mergeCell ref="B119:B120"/>
-    <mergeCell ref="C119:C120"/>
-    <mergeCell ref="A122:A123"/>
-    <mergeCell ref="B122:B123"/>
-    <mergeCell ref="C122:C123"/>
-    <mergeCell ref="A124:A125"/>
-    <mergeCell ref="B124:B125"/>
-    <mergeCell ref="C124:C125"/>
-    <mergeCell ref="A126:A127"/>
-    <mergeCell ref="B126:B127"/>
-    <mergeCell ref="C126:C127"/>
-    <mergeCell ref="A128:A129"/>
-    <mergeCell ref="B128:B129"/>
-    <mergeCell ref="C128:C129"/>
-    <mergeCell ref="A130:A131"/>
-    <mergeCell ref="B130:B131"/>
-    <mergeCell ref="C130:C131"/>
-    <mergeCell ref="A132:A133"/>
-    <mergeCell ref="B132:B133"/>
-    <mergeCell ref="C132:C133"/>
-    <mergeCell ref="A134:A135"/>
-    <mergeCell ref="B134:B135"/>
-    <mergeCell ref="C134:C135"/>
-    <mergeCell ref="A136:A137"/>
-    <mergeCell ref="B136:B137"/>
-    <mergeCell ref="C136:C137"/>
-    <mergeCell ref="A139:A140"/>
-    <mergeCell ref="B139:B140"/>
-    <mergeCell ref="C139:C140"/>
-    <mergeCell ref="A141:A142"/>
-    <mergeCell ref="B141:B142"/>
-    <mergeCell ref="C141:C142"/>
-    <mergeCell ref="A143:A144"/>
-    <mergeCell ref="B143:B144"/>
-    <mergeCell ref="C143:C144"/>
-    <mergeCell ref="A145:A146"/>
-    <mergeCell ref="B145:B146"/>
-    <mergeCell ref="C145:C146"/>
-    <mergeCell ref="A148:A149"/>
-    <mergeCell ref="B148:B149"/>
-    <mergeCell ref="C148:C149"/>
-    <mergeCell ref="A150:A151"/>
-    <mergeCell ref="B150:B151"/>
-    <mergeCell ref="C150:C151"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>